<commit_message>
Se realizo la descomposicion LU de la diagonal
</commit_message>
<xml_diff>
--- a/Excel/Clase 24-abr-2021.xlsx
+++ b/Excel/Clase 24-abr-2021.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luis\Documents\GitProjects\Clases-octave\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clases-octave\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81431C37-5C57-4CDD-8558-E26AACD810C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943B8472-6C16-4E1A-91D3-AC8BD050916E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C23CBDC8-AF82-4E14-AFB7-38945A7880BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C23CBDC8-AF82-4E14-AFB7-38945A7880BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Newtom-Raphson" sheetId="3" r:id="rId3"/>
+    <sheet name="Descomposicion LU" sheetId="4" r:id="rId4"/>
+    <sheet name="Gauss-Seidel" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Xi</t>
   </si>
@@ -137,6 +138,30 @@
   <si>
     <t>L</t>
   </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>-0.19+0.19/7.00333*-0.19</t>
+  </si>
+  <si>
+    <t>F=-0.49/2.04</t>
+  </si>
+  <si>
+    <t>-0.49-(-0.49/2.04)*2.04</t>
+  </si>
+  <si>
+    <t>-0.645-(-0.645/1.55)*1.55</t>
+  </si>
+  <si>
+    <t>F-0.645/1.55</t>
+  </si>
+  <si>
+    <t>F=-0.717/1.395</t>
+  </si>
+  <si>
+    <t>-0.717-(-0.717/1.395)*1.395</t>
+  </si>
 </sst>
 </file>
 
@@ -151,15 +176,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,13 +198,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,8 +285,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>58560</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
@@ -226,7 +305,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Entrada de lápiz 1">
@@ -271,8 +350,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Entrada de lápiz 7">
@@ -291,7 +370,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Entrada de lápiz 7">
@@ -336,8 +415,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>15060</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Entrada de lápiz 8">
@@ -356,7 +435,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Entrada de lápiz 8">
@@ -401,8 +480,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Entrada de lápiz 9">
@@ -421,7 +500,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Entrada de lápiz 9">
@@ -466,8 +545,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>21540</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="13" name="Entrada de lápiz 12">
@@ -486,7 +565,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="13" name="Entrada de lápiz 12">
@@ -531,8 +610,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>41340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Entrada de lápiz 13">
@@ -551,7 +630,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Entrada de lápiz 13">
@@ -596,8 +675,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>120300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="31" name="Entrada de lápiz 30">
@@ -616,7 +695,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="31" name="Entrada de lápiz 30">
@@ -661,8 +740,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="50" name="Entrada de lápiz 49">
@@ -681,7 +760,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="50" name="Entrada de lápiz 49">
@@ -726,8 +805,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>95940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="51" name="Entrada de lápiz 50">
@@ -746,7 +825,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="51" name="Entrada de lápiz 50">
@@ -791,8 +870,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="59" name="Entrada de lápiz 58">
@@ -811,7 +890,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="59" name="Entrada de lápiz 58">
@@ -856,8 +935,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="66" name="Entrada de lápiz 65">
@@ -876,7 +955,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="66" name="Entrada de lápiz 65">
@@ -921,8 +1000,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>26460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="70" name="Entrada de lápiz 69">
@@ -941,7 +1020,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="70" name="Entrada de lápiz 69">
@@ -986,8 +1065,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="71" name="Entrada de lápiz 70">
@@ -1006,7 +1085,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="71" name="Entrada de lápiz 70">
@@ -1051,8 +1130,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Entrada de lápiz 77">
@@ -1071,7 +1150,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Entrada de lápiz 77">
@@ -1116,8 +1195,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="79" name="Entrada de lápiz 78">
@@ -1136,7 +1215,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="79" name="Entrada de lápiz 78">
@@ -1181,8 +1260,8 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>176400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="84" name="Entrada de lápiz 83">
@@ -1201,7 +1280,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="84" name="Entrada de lápiz 83">
@@ -1246,8 +1325,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Entrada de lápiz 87">
@@ -1266,7 +1345,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Entrada de lápiz 87">
@@ -1311,8 +1390,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>96780</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="95" name="Entrada de lápiz 94">
@@ -1331,7 +1410,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="95" name="Entrada de lápiz 94">
@@ -1376,8 +1455,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>16020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Entrada de lápiz 96">
@@ -1396,7 +1475,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Entrada de lápiz 96">
@@ -1441,8 +1520,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="100" name="Entrada de lápiz 99">
@@ -1461,7 +1540,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="100" name="Entrada de lápiz 99">
@@ -1506,8 +1585,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>85620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="101" name="Entrada de lápiz 100">
@@ -1526,7 +1605,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="101" name="Entrada de lápiz 100">
@@ -1571,8 +1650,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>106260</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="102" name="Entrada de lápiz 101">
@@ -1591,7 +1670,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="102" name="Entrada de lápiz 101">
@@ -1636,8 +1715,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>89160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="120" name="Entrada de lápiz 119">
@@ -1656,7 +1735,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="120" name="Entrada de lápiz 119">
@@ -1701,8 +1780,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>12480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="121" name="Entrada de lápiz 120">
@@ -1721,7 +1800,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="121" name="Entrada de lápiz 120">
@@ -1766,8 +1845,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>55920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="176" name="Entrada de lápiz 175">
@@ -1786,7 +1865,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="176" name="Entrada de lápiz 175">
@@ -1831,8 +1910,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>101220</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="177" name="Entrada de lápiz 176">
@@ -1851,7 +1930,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="177" name="Entrada de lápiz 176">
@@ -1896,8 +1975,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>164400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="182" name="Entrada de lápiz 181">
@@ -1916,7 +1995,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="182" name="Entrada de lápiz 181">
@@ -1961,8 +2040,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>134820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="190" name="Entrada de lápiz 189">
@@ -1981,7 +2060,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="190" name="Entrada de lápiz 189">
@@ -2026,8 +2105,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>77640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId57">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="191" name="Entrada de lápiz 190">
@@ -2046,7 +2125,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="191" name="Entrada de lápiz 190">
@@ -2091,8 +2170,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>186060</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="194" name="Entrada de lápiz 193">
@@ -2111,7 +2190,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="194" name="Entrada de lápiz 193">
@@ -2156,8 +2235,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>101040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="199" name="Entrada de lápiz 198">
@@ -2176,7 +2255,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="199" name="Entrada de lápiz 198">
@@ -2221,8 +2300,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>141660</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="208" name="Entrada de lápiz 207">
@@ -2241,7 +2320,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="208" name="Entrada de lápiz 207">
@@ -2286,8 +2365,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>37380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId65">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="212" name="Entrada de lápiz 211">
@@ -2306,7 +2385,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="212" name="Entrada de lápiz 211">
@@ -2351,8 +2430,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId67">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="217" name="Entrada de lápiz 216">
@@ -2371,7 +2450,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="217" name="Entrada de lápiz 216">
@@ -2416,8 +2495,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>141645</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId69">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="225" name="Entrada de lápiz 224">
@@ -2436,7 +2515,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="225" name="Entrada de lápiz 224">
@@ -2481,8 +2560,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>186945</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId71">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="226" name="Entrada de lápiz 225">
@@ -2501,7 +2580,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="226" name="Entrada de lápiz 225">
@@ -2546,8 +2625,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>59625</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId72">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="227" name="Entrada de lápiz 226">
@@ -2566,7 +2645,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="227" name="Entrada de lápiz 226">
@@ -2611,8 +2690,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>61785</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId74">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="228" name="Entrada de lápiz 227">
@@ -2631,7 +2710,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="228" name="Entrada de lápiz 227">
@@ -2676,8 +2755,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>47805</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId76">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="231" name="Entrada de lápiz 230">
@@ -2696,7 +2775,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="231" name="Entrada de lápiz 230">
@@ -2741,8 +2820,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>134865</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId78">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="232" name="Entrada de lápiz 231">
@@ -2761,7 +2840,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="232" name="Entrada de lápiz 231">
@@ -2806,8 +2885,8 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>20700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId80">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="233" name="Entrada de lápiz 232">
@@ -2826,7 +2905,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="233" name="Entrada de lápiz 232">
@@ -2871,8 +2950,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>48720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId82">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="262" name="Entrada de lápiz 261">
@@ -2891,7 +2970,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="262" name="Entrada de lápiz 261">
@@ -2936,8 +3015,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>20100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId84">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="268" name="Entrada de lápiz 267">
@@ -2956,7 +3035,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="268" name="Entrada de lápiz 267">
@@ -3001,8 +3080,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>155940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId86">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="269" name="Entrada de lápiz 268">
@@ -3021,7 +3100,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="269" name="Entrada de lápiz 268">
@@ -3066,8 +3145,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId88">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="271" name="Entrada de lápiz 270">
@@ -3086,7 +3165,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="271" name="Entrada de lápiz 270">
@@ -3131,8 +3210,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId90">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="272" name="Entrada de lápiz 271">
@@ -3151,7 +3230,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="272" name="Entrada de lápiz 271">
@@ -3196,8 +3275,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId92">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="273" name="Entrada de lápiz 272">
@@ -3216,7 +3295,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="273" name="Entrada de lápiz 272">
@@ -3310,8 +3389,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>164700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="55" name="Entrada de lápiz 54">
@@ -3330,7 +3409,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="55" name="Entrada de lápiz 54">
@@ -3375,8 +3454,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="56" name="Entrada de lápiz 55">
@@ -3395,7 +3474,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="56" name="Entrada de lápiz 55">
@@ -3440,8 +3519,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>120960</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="59" name="Entrada de lápiz 58">
@@ -3460,7 +3539,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="59" name="Entrada de lápiz 58">
@@ -3505,8 +3584,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>29100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="71" name="Entrada de lápiz 70">
@@ -3525,7 +3604,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="71" name="Entrada de lápiz 70">
@@ -3570,8 +3649,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="72" name="Entrada de lápiz 71">
@@ -3590,7 +3669,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="72" name="Entrada de lápiz 71">
@@ -3635,8 +3714,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>6600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Entrada de lápiz 77">
@@ -3655,7 +3734,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Entrada de lápiz 77">
@@ -3700,8 +3779,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>6420</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="93" name="Entrada de lápiz 92">
@@ -3720,7 +3799,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="93" name="Entrada de lápiz 92">
@@ -3814,8 +3893,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>39840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="7" name="Entrada de lápiz 6">
@@ -3834,7 +3913,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="7" name="Entrada de lápiz 6">
@@ -3879,8 +3958,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>161880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Entrada de lápiz 7">
@@ -3899,7 +3978,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Entrada de lápiz 7">
@@ -3944,8 +4023,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>166140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Entrada de lápiz 8">
@@ -3964,7 +4043,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Entrada de lápiz 8">
@@ -4009,8 +4088,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>60300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Entrada de lápiz 13">
@@ -4029,7 +4108,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Entrada de lápiz 13">
@@ -4074,8 +4153,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>50520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="22" name="Entrada de lápiz 21">
@@ -4094,7 +4173,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="22" name="Entrada de lápiz 21">
@@ -4139,8 +4218,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>152580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="28" name="Entrada de lápiz 27">
@@ -4159,7 +4238,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="28" name="Entrada de lápiz 27">
@@ -4204,8 +4283,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>181680</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="29" name="Entrada de lápiz 28">
@@ -4224,7 +4303,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="29" name="Entrada de lápiz 28">
@@ -4269,8 +4348,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>174840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Entrada de lápiz 42">
@@ -4289,7 +4368,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Entrada de lápiz 42">
@@ -4334,8 +4413,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>149940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="55" name="Entrada de lápiz 54">
@@ -4354,7 +4433,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="55" name="Entrada de lápiz 54">
@@ -4399,8 +4478,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Entrada de lápiz 60">
@@ -4419,7 +4498,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Entrada de lápiz 60">
@@ -4464,8 +4543,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>3840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Entrada de lápiz 61">
@@ -4484,7 +4563,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Entrada de lápiz 61">
@@ -4529,8 +4608,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>59700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="65" name="Entrada de lápiz 64">
@@ -4549,7 +4628,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="65" name="Entrada de lápiz 64">
@@ -4594,8 +4673,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>85620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="66" name="Entrada de lápiz 65">
@@ -4614,7 +4693,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="66" name="Entrada de lápiz 65">
@@ -4659,8 +4738,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>108300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="69" name="Entrada de lápiz 68">
@@ -4679,7 +4758,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="69" name="Entrada de lápiz 68">
@@ -4724,8 +4803,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>164820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="70" name="Entrada de lápiz 69">
@@ -4744,7 +4823,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="70" name="Entrada de lápiz 69">
@@ -4789,8 +4868,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>30840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="77" name="Entrada de lápiz 76">
@@ -4809,7 +4888,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="77" name="Entrada de lápiz 76">
@@ -4854,8 +4933,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>181020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="89" name="Entrada de lápiz 88">
@@ -4874,7 +4953,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="89" name="Entrada de lápiz 88">
@@ -4919,8 +4998,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>138480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="90" name="Entrada de lápiz 89">
@@ -4939,7 +5018,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="90" name="Entrada de lápiz 89">
@@ -4984,8 +5063,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>104700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="91" name="Entrada de lápiz 90">
@@ -5004,7 +5083,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="91" name="Entrada de lápiz 90">
@@ -5049,8 +5128,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>70440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="92" name="Entrada de lápiz 91">
@@ -5069,7 +5148,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="92" name="Entrada de lápiz 91">
@@ -5114,8 +5193,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>37380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="95" name="Entrada de lápiz 94">
@@ -5134,7 +5213,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="95" name="Entrada de lápiz 94">
@@ -5179,8 +5258,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>49140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="99" name="Entrada de lápiz 98">
@@ -5199,7 +5278,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="99" name="Entrada de lápiz 98">
@@ -5244,8 +5323,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>180</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="100" name="Entrada de lápiz 99">
@@ -5264,7 +5343,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="100" name="Entrada de lápiz 99">
@@ -5309,8 +5388,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>27240</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="107" name="Entrada de lápiz 106">
@@ -5329,7 +5408,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="107" name="Entrada de lápiz 106">
@@ -5374,8 +5453,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="118" name="Entrada de lápiz 117">
@@ -5394,7 +5473,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="118" name="Entrada de lápiz 117">
@@ -5439,8 +5518,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="121" name="Entrada de lápiz 120">
@@ -5459,7 +5538,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="121" name="Entrada de lápiz 120">
@@ -5504,8 +5583,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>144300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Entrada de lápiz 121">
@@ -5524,7 +5603,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Entrada de lápiz 121">
@@ -5569,8 +5648,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>46380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="128" name="Entrada de lápiz 127">
@@ -5589,7 +5668,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="128" name="Entrada de lápiz 127">
@@ -5634,8 +5713,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>87420</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId58">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="132" name="Entrada de lápiz 131">
@@ -5654,7 +5733,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="132" name="Entrada de lápiz 131">
@@ -5699,8 +5778,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId60">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="133" name="Entrada de lápiz 132">
@@ -5719,7 +5798,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="133" name="Entrada de lápiz 132">
@@ -5764,8 +5843,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId62">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="134" name="Entrada de lápiz 133">
@@ -5784,7 +5863,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="134" name="Entrada de lápiz 133">
@@ -5829,8 +5908,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>59820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId64">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="136" name="Entrada de lápiz 135">
@@ -5849,7 +5928,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="136" name="Entrada de lápiz 135">
@@ -5894,8 +5973,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>31860</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId66">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="137" name="Entrada de lápiz 136">
@@ -5914,7 +5993,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="137" name="Entrada de lápiz 136">
@@ -5959,8 +6038,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>169380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="138" name="Entrada de lápiz 137">
@@ -5979,7 +6058,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="138" name="Entrada de lápiz 137">
@@ -6024,8 +6103,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>80040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId70">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="141" name="Entrada de lápiz 140">
@@ -6044,7 +6123,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="141" name="Entrada de lápiz 140">
@@ -6089,8 +6168,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>94740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId72">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="144" name="Entrada de lápiz 143">
@@ -6109,7 +6188,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="144" name="Entrada de lápiz 143">
@@ -6154,8 +6233,8 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>112200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId74">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="145" name="Entrada de lápiz 144">
@@ -6174,7 +6253,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="145" name="Entrada de lápiz 144">
@@ -6219,8 +6298,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>78300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId76">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="146" name="Entrada de lápiz 145">
@@ -6239,7 +6318,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="146" name="Entrada de lápiz 145">
@@ -6284,8 +6363,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>168660</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId78">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="147" name="Entrada de lápiz 146">
@@ -6304,7 +6383,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="147" name="Entrada de lápiz 146">
@@ -6349,8 +6428,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>146340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId80">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="150" name="Entrada de lápiz 149">
@@ -6369,7 +6448,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="150" name="Entrada de lápiz 149">
@@ -6414,8 +6493,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>23100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId82">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="157" name="Entrada de lápiz 156">
@@ -6434,7 +6513,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="157" name="Entrada de lápiz 156">
@@ -6518,6 +6597,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>478685</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>42136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3EB7A67-E711-49B1-B74F-5A95E6F6D460}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="68580"/>
+          <a:ext cx="3801005" cy="1619476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -6541,7 +6669,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">613 0,'-40'250,"-78"263,34-164,-101 530,120-431,32-170,-2-88,15-100,-12 170,31-232</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">612 0,'-40'240,"-78"254,34-159,-100 510,119-414,32-164,-2-84,15-97,-12 164,31-223</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6595,17 +6723,17 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">6774 0,'0'2550,"-41"-1656,1-69,37 160,-8 461,-2 1170,16-1599,-2-751,-19 625,13-829</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1171.37">1 5742,'68'3,"75"12,-67-6,317 38,771 70,455-63,18-53,-1099-3,4755-4,1154 6,-6389 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4000.47">2382 10319,'0'0,"1"0,0-1,0 0,0 1,0-1,0 1,-1-1,1 0,0 0,0 1,-1-1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,0-2,8-12,96-176,-8-6,-8-3,78-268,-30-106,-44-9,-35 262,130-418,-109 496,10 4,11 3,172-298,-119 283,204-256,227-192,-430 532,215-182,-255 256,5 4,256-143,-201 146,3 7,3 9,4 7,1 8,3 8,2 9,228-17,-264 46,257 19,-372-5,-1 1,0 2,0 2,-1 1,46 21,166 92,-216-107,83 47,212 157,-264-169,-1 2,-4 3,-1 3,67 94,-24-7,-8 5,87 193,113 342,-104-229,43 112,38 87,-209-526,141 229,-160-301,2-1,2-2,3-2,2-2,101 80,-68-71,2-4,2-4,3-3,170 66,-228-106,0-1,1-1,0-2,63 3,134-13,-166 1,3-2,1-4,-1-2,-1-4,0-2,98-40,303-162,-396 182,311-166,-9-16,465-361,-78-59,-594 479,-6-7,178-243,-190 201,-9-6,-9-6,181-426,-293 601,277-753,-170 381,47-149,-113 410,-33 93,-2-1,27-124,-27 76,51-140,-41 146,-14 52,-12 36</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="67069.59">9552 13892,'0'0,"0"0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,-12 7,-8 20,2 6,0 1,2 1,2 1,-13 48,-26 156,43-188,-115 741,33 14,60-506,-108 1619,110 18,30-1875,-3 730,-53-7,35-624,-31 268,4-88,-7 91,53-384</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="68312.59">239 18125,'1166'-44,"-748"-4,90-12,198-18,4255-182,-4303 258,-71 4,-77 2,1198-12,-432-1,-821 11,442-4,-716-12,16 1,-76 16,177 26,-238-19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70644.24">3176 21141,'-3'-3,"0"-1,1 0,-1 0,1-1,1 1,-1 0,0-1,1 1,0-1,0 0,0 1,0-8,-1-6,-32-201,-3-230,24-221,13 567,-1 52,9-495,1 407,51-259,-2 170,150-379,157-188,-289 651,143-200,125-105,-153 221,412-382,-451 481,5 6,5 7,313-168,-342 221,3 6,2 5,2 7,1 5,3 7,1 7,0 5,183-2,-258 22,249-2,-249 6,1 3,101 22,-137-18,-1 1,0 1,-1 2,-1 2,0 1,0 1,-2 1,44 39,11 17,102 121,-178-186,208 247,286 445,-456-629,-2 3,-4 1,-3 2,-4 1,45 161,60 268,7 30,-34-9,-24 5,35 990,-62-704,58-7,-89-643,104 333,-102-401,-24-83</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73089.34">5187 20956,'22'1,"1"1,-1 1,0 1,36 11,85 38,-116-43,37 15,1-3,1-3,1-3,0-3,71 5,662-3,-565-17,-10 3,440-14,-577 4,-1-5,0-3,163-56,236-128,-316 126,138-56,395-179,-497 208,250-165,-284 147,-5-7,253-251,-309 260,-4-5,-6-4,-5-5,82-152,58-202,-37-13,-29 70,-83 236,140-229,148-153,105-160,-77-42,-337 626,-7-4,51-210,-78 196,14-200,-45 345</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="104768.33">15188 13627,'2'-8,"0"1,0-1,1 0,1 1,-1-1,1 1,1 0,-1 0,1 0,0 1,0 0,9-7,-9 6,7-7,0 0,1 1,1 0,0 1,1 0,0 1,0 1,1 1,0 0,1 1,0 0,1 2,-1 0,1 1,0 1,0 0,1 1,26 0,-23 3,1 2,-1 0,1 1,-1 1,43 14,-29-4,-1 1,55 34,-45-21,-18-11,1 0,1-2,47 18,-67-30,0 0,0-1,0 0,0-1,0 0,0 0,0-1,1 0,-1-1,0 0,0 0,0-1,0 0,0-1,-1 0,1 0,10-6,42-30,-2-2,-1-3,56-56,-85 74</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="106054.34">15929 13521,'-1'3,"1"-1,0 1,-1-1,1 0,-1 1,0-1,0 0,1 0,-2 0,1 1,-2 2,-5 10,-52 114,8-20,-39 123,79-196,2 1,2-1,1 1,2 0,2 1,1 0,6 66,-1-78,2 1,1-2,15 41,-16-52,1 0,1 0,0 0,1-1,1 0,0-1,15 18,-3-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="108211.34">3837 13680,'-1'0,"-1"0,1-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,1-2,-1-39,0 38,3-20,1 0,1 0,1 1,1-1,1 2,1-1,1 1,1 0,1 1,1 0,1 1,0 1,2 0,0 1,1 1,1 0,0 1,1 1,1 1,38-21,2 6,0 2,76-23,-98 39,0 1,1 3,0 0,1 3,41 0,-47 6,0 1,0 2,0 1,-1 2,1 1,61 26,176 109,-171-86,-65-41,1 0,0-3,1 0,1-3,0-1,0-2,1-2,0-1,1-2,59-3,-3 0,124-5,-204 3,-2-1,1 0,0-1,-1-1,0-1,0 0,0 0,-1-2,0 1,21-17,-4 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="109041.36">5504 13071,'0'21,"-1"-1,0 0,-2 0,0 0,-1-1,-1 1,-1-1,0 0,-2 0,0-1,-16 27,-155 232,48-76,127-196,1 1,-1 0,2 0,-1 0,1 0,0 0,0 1,0-1,0 11,1 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">7053 0,'0'2448,"-43"-1590,2-66,38 153,-9 443,-1 1124,16-1536,-2-721,-20 600,14-795</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1171.36">1 5512,'71'3,"78"11,-70-5,330 36,803 67,474-60,18-51,-1144-3,4952-4,1200 6,-6651 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4000.47">2480 9905,'0'0,"1"0,0-1,0 0,0 1,0-1,0 1,-1 0,1-1,0 0,1 1,-2-1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,0-2,8-11,100-170,-8-5,-8-3,81-257,-32-102,-45-9,-37 252,136-401,-114 476,11 3,11 4,179-287,-123 272,211-246,237-184,-447 511,223-175,-266 246,6 3,267-136,-210 139,3 7,3 9,5 7,1 7,2 8,3 8,237-16,-275 45,268 17,-387-4,-2 1,1 2,0 1,-2 2,48 20,174 88,-226-103,87 45,220 151,-274-162,-2 2,-3 3,-2 3,70 89,-25-6,-8 5,90 186,118 327,-108-219,45 107,39 83,-218-504,148 220,-168-290,3 0,2-2,3-2,2-2,105 76,-70-67,1-4,3-5,2-2,178 64,-238-103,1 0,0-1,0-3,66 4,140-13,-173 1,2-1,2-5,-1-2,-1-3,-1-2,103-39,315-155,-412 174,324-159,-10-15,485-347,-82-56,-618 459,-6-6,185-233,-198 192,-10-5,-8-7,188-408,-306 577,289-723,-176 366,48-143,-118 393,-34 90,-2-2,28-118,-28 72,53-134,-42 141,-15 49,-13 35</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="67069.59">9946 13335,'0'0,"0"0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,-2 0,2 0,0 0,0 0,-1 0,1 0,-12 7,-9 19,2 6,1 0,1 2,2 1,-13 45,-27 151,45-182,-120 713,34 12,62-485,-111 1554,113 18,32-1801,-3 701,-55-6,36-600,-32 258,4-85,-7 88,55-369</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="68312.59">249 17398,'1214'-42,"-779"-4,94-11,206-18,4431-175,-4481 248,-74 4,-80 2,1247-12,-449 0,-855 10,460-4,-746-12,17 2,-79 15,184 24,-247-17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70644.23">3307 20294,'-3'-3,"0"-1,1 0,-2 0,2-1,1 2,-1-1,0-1,1 1,0-1,0 0,0 2,0-9,-1-5,-34-193,-2-221,24-213,14 546,-1 49,10-476,0 392,53-249,-1 163,155-364,165-180,-302 625,149-192,130-101,-159 212,429-366,-470 461,5 6,6 6,326-160,-357 211,4 6,1 6,3 5,1 6,3 6,1 7,0 5,190-2,-268 21,259-2,-259 6,1 3,105 21,-142-18,-2 2,0 0,0 3,-2 1,0 2,1 0,-3 1,46 38,12 16,105 116,-184-179,216 238,297 427,-474-604,-2 3,-4 1,-4 2,-3 1,46 154,63 258,7 28,-36-8,-24 4,36 951,-64-676,60-6,-93-618,108 320,-105-386,-26-78</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73089.34">5401 20116,'23'1,"1"1,-2 1,1 1,38 10,88 37,-121-42,38 15,2-2,1-4,1-3,-1-2,75 4,689-3,-588-16,-11 3,458-13,-600 3,-1-4,-1-4,170-53,247-123,-330 121,143-53,412-173,-517 200,259-158,-294 141,-7-7,265-241,-323 250,-3-5,-7-4,-5-5,85-146,61-193,-39-13,-30 67,-86 227,145-220,155-147,108-154,-79-40,-351 601,-8-3,54-203,-82 189,15-192,-47 331</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="104768.33">15814 13081,'2'-8,"0"1,0 0,1-1,1 1,0 0,0 0,1 0,-1 0,1 1,1 0,-1 0,9-6,-8 5,6-6,1-1,0 2,2-1,-1 2,2-1,-1 2,1 0,1 1,-1 1,2 0,0 0,1 3,-2-1,2 1,0 1,-1 0,2 1,27 1,-24 2,1 1,-1 1,1 1,-1 1,44 13,-29-3,-2 0,58 33,-47-20,-19-11,1 1,1-3,49 18,-69-29,-1 0,1-1,-1-1,0 0,1 0,-1 0,0-1,2 0,-2-1,1 0,-1 0,0 0,1-1,-1-1,-1 0,2 0,10-6,43-28,-2-2,0-4,58-53,-89 71</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="106054.34">16585 12979,'-1'3,"1"-1,0 1,-1-1,1 0,-1 0,0 0,0 0,1 0,-2 0,1 1,-2 2,-5 9,-55 110,9-19,-41 117,83-187,1 0,3 0,1 0,2 1,1 0,2 1,7 63,-2-75,2 1,1-2,16 39,-17-50,1 1,2-1,-1 1,1-2,2 1,-1-2,16 18,-3-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="108211.34">3995 13132,'-1'0,"-1"0,1-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,-1 0,2 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,-1 1,1-1,0 0,1-2,-1-38,0 38,3-20,2-1,0 1,1 1,1-1,2 2,0-1,1 1,2 0,0 1,2 0,1 0,-1 2,3 0,-1 1,2 0,1 1,0 1,0 0,2 2,40-21,1 6,1 2,78-22,-101 38,-1 0,2 4,-1-1,2 3,42 0,-48 6,-1 1,1 2,-1 1,-1 1,2 2,63 24,183 106,-178-84,-68-38,2-1,-1-3,2 1,1-4,-1 0,1-2,0-3,1 0,1-2,61-3,-3 0,129-5,-213 3,-1 0,1-1,-1-1,0-1,-1-1,1 0,-1 1,0-3,0 1,21-16,-4 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="109041.36">5731 12547,'0'20,"-1"-1,0 1,-2-1,-1 0,0-1,-1 1,-1 0,0-1,-3 0,1-1,-17 27,-161 222,49-74,133-187,1 1,-1 0,2 0,-1-1,0 1,1 0,0 1,0-2,0 12,1 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6632,9 +6760,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'59'3,"-1"1,1 4,-1 1,0 4,71 24,-33-2,-2 4,107 61,-189-93,2 0,1 1,-2 0,1 1,-1 1,21 20,-32-28,0 0,-1 0,1 0,-1 0,1 1,-1-1,0 1,0-1,0 1,0 0,-1-1,1 1,0 0,-1-1,0 1,0 4,-1-3,0-1,0 1,0 0,0-1,-1 0,1 1,-1-1,0 0,0 0,-1 0,1 0,0 0,-1 0,0-1,-4 4,-11 7,0 0,0-1,-1-1,-1-1,0-1,-21 8,-131 33,161-47,-40 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1264">1615 80,'-3'36,"-1"0,-2 0,-1-1,-18 52,-6 31,15-48,3-13,2 0,-7 111,17-110,4 140,-3-196,0-1,1 1,-1 0,0 0,1 0,-1 0,1-1,0 1,-1 0,1 0,0-1,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,1-1,-1 0,1 0,-1 0,1 0,1 1,1-1,0 0,-1 0,1 0,0-1,0 1,0-1,0 0,-1 0,1-1,0 1,5-2,8-2,0-2,0 0,-1 0,16-10,30-22,-37 19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2352">1324 582,'9'0,"7"0,11 0,4 0,6 0,2 0,-2 0,-2 0,-3 0,-7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'62'3,"-1"1,1 3,-1 2,-1 4,76 22,-36-1,-1 3,112 59,-198-89,1 0,2 0,-2 1,0 1,0 0,22 20,-34-27,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 1,0-1,0 1,0 0,-1-1,1 1,1 0,-2-1,0 0,0 5,-2-3,1-1,0 1,0 0,0-2,-1 1,1 1,-1-1,0 0,0 0,-1 0,1 0,-1-1,0 1,0-1,-4 4,-12 6,0 1,0-1,-1-2,-1 0,0-2,-22 9,-137 31,168-45,-41 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1264">1695 77,'-4'34,"0"1,-2 0,-1-2,-20 51,-5 29,15-46,3-12,3 0,-8 106,18-105,4 134,-3-188,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0-1,0 1,0-1,0 1,1-1,0 1,-1-1,0 1,1-2,-1 1,1 0,-1 0,1 0,1 1,1-1,1 0,-2 0,1 0,0-1,0 1,1-1,-1 0,-1 0,1-1,0 1,6-2,8-2,-1-1,1-1,-1 0,17-9,31-22,-39 19</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2352">1389 559,'10'0,"6"0,13 0,3 0,7 0,2 0,-2 0,-2 0,-4 0,-7 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6688,12 +6816,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2144 0,'1'223,"-3"247,-8-359,5-66</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="507.99">1933 1587,'0'5,"0"6,0 5,0 5,0 3,0 2,0 1,0 1,0-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="858">1880 2249,'0'9,"0"8,0 9,0 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1559.99">1 2831,'4'0,"11"5,8 1,8-1,8 0,6-2,5-1,-6-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1907">927 2805,'4'0,"2"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2301">1298 2725,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2229 0,'1'215,"-3"238,-9-347,6-62</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="507.98">2010 1529,'0'5,"0"5,0 6,0 4,0 3,0 2,0 1,0 1,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="858">1954 2166,'0'9,"0"7,0 9,0 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1559.99">1 2727,'4'0,"12"5,8 1,8-2,8 1,7-2,5-1,-6-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1907">964 2702,'4'0,"2"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2301">1349 2625,'0'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6720,7 +6848,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 9125,'251'2,"270"-4,265-87,-506 47,322-64,-362 60,-37 2,330-116,-177 2,-141 56,24-15,400-173,-576 260,-2-2,-2-3,-1-2,-2-3,-2-2,-1-2,63-71,1-38,-8 8,45-48,-93 112,4 3,90-87,-90 107,-2-2,76-97,-80 77,84-150,-22 34,1-4,350-658,-460 836,251-518,-80 152,-65 159,136-278,-43-18,-205 506,145-472,-113 344,26-203,11-62,-67 372,-1-4,3-84,2-17,12-7,29-167,-47 280,-2 0,-3-79,0-16,1 123,1-1,-1 1,2 0,0 0,6-14,9-25,-13 27</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 8765,'261'2,"280"-4,275-83,-525 44,334-61,-376 58,-38 2,343-112,-184 3,-147 53,25-15,416-165,-599 249,-1-2,-3-3,-1-1,-2-4,-2-1,-1-2,66-69,0-36,-7 8,46-46,-97 107,4 3,94-83,-93 102,-3-2,80-93,-84 75,87-145,-22 32,1-3,363-632,-477 803,260-498,-83 147,-68 152,142-267,-45-18,-212 487,149-454,-116 331,26-195,12-60,-70 358,0-4,2-81,3-17,12-6,30-160,-49 268,-2 1,-3-76,0-16,1 118,1 0,-1 0,2 1,1-1,5-13,10-24,-14 26</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6777,9 +6905,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">460 158,'-2'36,"-9"53,2-28,-29 172,-2 11,35-195,2 1,6 94,-2-133,1 1,0-1,0 0,1 0,1 0,0 0,0-1,1 0,1 0,-1 0,1 0,9 9,-10-13,1-1,-1 1,2-1,-1 0,0-1,1 0,0 0,0 0,0-1,0 0,1 0,-1 0,1-1,0-1,-1 1,1-1,0-1,9 1,-4-1,0-1,0 0,-1-1,1 0,-1-1,1 0,-1-1,0-1,0 0,0 0,-1-1,0 0,11-9,-8 3,-1 0,0 0,-1-2,0 1,-1-2,0 1,-2-1,12-23,2-16,-2-2,-2 0,-3-2,14-91,-1-145,-2 12,-5 161,-17 195,-51 997,27-884,-6 56,-70 306,86-520,0 1,-2-1,-1-1,-2 0,-1-1,0-1,-2 0,-1-1,-2-1,0 0,-1-2,-1 0,-1-2,-1 0,-1-2,0 0,-50 24,57-33,-1-1,1-1,-1-1,-1 0,1-1,-1-1,-30 2,41-5,1-1,-1 0,0 0,1-1,-1 0,1 0,-1-1,1 0,0-1,0 0,0 0,0-1,0 0,0 0,1-1,0 0,0 0,0 0,-11-13,4-3,0-1,1 0,1-1,1 0,1-1,1 0,1-1,-7-39,6 11,2 0,2 0,3-65,1 110,2 0,-1 0,1 0,1 0,-1 0,1 0,5-11,-6 16,1 0,0 1,0-1,0 0,0 1,0-1,0 1,1 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0 0,0-1,0 1,0 0,1 0,3 0,20-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1023.02">1228 2142,'2'0,"0"0,1-1,-1 0,0 0,0 1,0-1,1-1,-1 1,0 0,0 0,-1-1,1 1,0-1,0 0,-1 1,1-1,2-3,25-41,-19 30,25-39,-4 4,76-91,-105 139,0 1,-1 0,1 0,0 0,1 0,-1 1,0-1,1 1,-1-1,0 1,1 0,0 0,-1 0,1 0,0 0,-1 0,4 0,-5 2,0-1,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 2,2 28,-9 7,-2 1,-23 61,10-33,-43 123,27-85,-44 196,80-285,0 0,0 0,1 0,1 1,1-1,3 23,-3-35,-1 0,1 0,0-1,0 1,0 0,0 0,1-1,-1 1,1-1,0 1,0-1,-1 0,1 1,1-1,-1 0,3 2,-2-3,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0-1,0 0,1-1,-1 1,0 0,0-1,0 0,0 0,0 0,0 0,3-1,6-4,0 0,0 0,0-1,-1-1,0 0,0 0,-1-1,0-1,-1 1,0-2,0 1,-1-1,10-18,-1-3,-1-2,-1 0,16-58,-4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1367">1730 1136,'-5'0,"-1"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">482 152,'-2'35,"-9"50,1-26,-30 165,-2 11,37-188,2 2,6 89,-2-127,1 0,0 0,1 0,0-1,1 1,0-1,0 0,2 0,0-1,-1 1,1-1,10 10,-11-13,2-2,-2 2,2-1,-1 0,1-1,0-1,0 1,1 0,-1-1,0 0,2 0,-2 0,2-1,-1-1,-1 1,2-2,-1 0,10 1,-4-1,-1-1,1 1,-2-2,2 0,-1-1,0 0,0-1,-1-1,1 0,0 1,-2-2,1 0,11-8,-9 2,0 1,0-1,-2-2,1 2,-2-2,1 0,-3 0,13-23,2-15,-2-2,-2 0,-3-2,15-87,-2-140,-2 11,-5 156,-17 187,-55 960,30-851,-8 54,-72 295,89-501,1 0,-3 0,0-1,-3 0,-1-1,1-1,-3 0,-1-1,-2-1,0 1,-1-3,-1 0,-1-2,-1 0,-2-1,1-1,-53 24,61-33,-2 0,1-1,-1-2,-1 1,1-1,-1-1,-31 2,42-5,2-1,-2 0,1 0,1-1,-2 0,2 0,-2-1,2 0,-1-1,1 0,0 0,-1-1,1 0,0 1,0-2,1 0,0 0,-1 0,-11-12,5-3,-1-1,1-1,2 0,0 0,2-1,0 0,2-1,-8-38,7 11,1 0,3 0,3-62,1 105,2 0,-1 1,1-1,1 0,-1 0,1 1,6-12,-7 17,1-1,0 1,0-1,0 0,0 1,0-1,0 1,2 0,-2 0,1 0,0 1,-1-1,1 0,0 1,0 0,1-1,-1 1,0 0,1 0,3 0,22-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1023.02">1288 2062,'2'0,"0"0,1-1,-1 0,0 0,0 1,0-1,1-1,0 1,-1 0,0 0,-1-1,1 1,0-1,0 1,-1 0,1-1,2-3,27-39,-21 28,27-37,-4 4,79-88,-110 135,0 0,-1 0,1 0,0 0,1 0,-1 1,0-1,2 1,-2-1,0 1,1 0,0 0,-1 0,1 0,1 0,-2 0,4 0,-5 2,0-1,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,2 1,-2 0,1-1,-1 2,2 27,-10 7,-1 0,-25 59,11-31,-45 118,28-82,-46 189,84-275,0 1,0-1,1 1,1 0,1-1,3 23,-3-34,-1 0,1 0,0-1,0 0,0 1,1 0,0-1,-1 1,1-1,0 1,0-1,-1 0,1 1,1-1,-1-1,4 3,-3-3,0 0,0 0,0 0,0 0,0-1,1 1,-1-1,0 1,0-1,0 0,1-1,0 1,-1 0,0-1,0 0,0 0,0 0,0 0,4-1,5-3,1-1,-1 0,1-1,-1 0,-1-1,1 0,-2 0,1-2,-2 1,0-1,1 0,-2-1,11-17,-1-2,-1-3,-2 0,18-55,-5-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1367">1814 1094,'-5'0,"-2"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6836,7 +6964,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">292 222,'0'5,"0"32,0 24,0 11,0-3,0-9,0-5,0-8,-5-16,-6-13,0-15,-4-7,1-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="453.99">1 433,'0'-4,"8"-2,9 1,14 0,6 2,6 1,14 1,1 0,1 1,-7 0,-2 1,-5-1,-1 0,-9 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="453.98">1 433,'0'-4,"8"-2,9 1,14 0,6 2,6 1,14 1,1 0,1 1,-7 0,-2 1,-5-1,-1 0,-9 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1183.99">662 301,'11'-20,"2"0,22-28,4-6,-14 15,-12 17,2 0,0 0,26-26,-40 47,-1 1,0-1,0 1,1 0,-1-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,0 0,2 1,7 19,-2 35,-7-52,2 51,-3 0,-3-1,-2 1,-23 97,-85 200,94-300</inkml:trace>
 </inkml:ink>
 </file>
@@ -6864,7 +6992,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 55,'326'-15,"-117"3,12 2,238-6,2751 15,-1528 2,2605-1,-4247 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 56,'339'-15,"-121"2,12 3,247-6,2864 15,-1590 2,2710-1,-4419 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6891,7 +7019,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 28,'0'-1,"0"0,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,-1-1,1 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,1 0,35-5,-32 4,127-5,248 19,-82 2,-129-15,-132 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 29,'0'-1,"0"0,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,-1 1,1-1,1 0,-1 1,0-1,0 0,0 1,-1-2,1 2,0 0,0-1,0 1,0 0,0-1,1 1,0 0,0 0,38-5,-35 4,137-5,268 19,-88 3,-140-16,-142 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6946,7 +7074,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">54 0,'9'0,"12"0,16 0,10 0,12 0,26 0,8 0,2 0,-2 0,-8 0,-9 0,-13 0,-13 0,-15 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="502.99">1 212,'0'5,"4"6,11 0,12 0,15-4,13-1,2-3,5-2,10 0,11 3,9 2,16 4,-6 0,-16 3,-22-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="502.98">1 212,'0'5,"4"6,11 0,12 0,15-4,13-1,2-3,5-2,10 0,11 3,9 2,16 4,-6 0,-16 3,-22-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6973,18 +7101,18 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">4047 493,'-1'-4,"1"0,0 0,1 0,-1 0,1 0,-1 0,1 0,1 0,-1 0,0 0,1 0,0 0,0 1,0-1,0 1,1-1,-1 1,1 0,0 0,0 0,0 1,0-1,1 0,-1 1,1 0,-1 0,1 0,0 1,0-1,-1 1,1 0,0 0,0 0,8-1,0 2,0-1,0 1,0 1,0 0,0 1,0 0,-1 1,1 0,-1 1,0 1,11 5,25 16,-2 3,46 38,-11-7,-78-58,0-1,0 1,0-1,0 0,1 1,-1-1,0 0,1 0,-1-1,0 1,1 0,-1-1,1 1,-1-1,1 0,-1 0,3 0,12-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="509.52">4550 175,'-5'0,"-5"5,-6 10,-5 12,-3 14,-2 5,3 4,6-2,1-5,-1-5,2-5,3-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1899.21">4524 572,'15'-1,"0"-2,1 0,-1-1,0 0,0-2,-1 1,0-2,0 0,0 0,23-18,-12 9,46-21,-63 33,1 1,-1 0,1 1,-1 0,1 0,0 1,0 0,0 1,-1 0,11 1,-17-1,1 1,0-1,-1 1,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,0 1,1 0,-1 0,0-1,-1 1,1 1,0-1,0 0,-1 0,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,-1 0,1-1,-1 1,1 4,-1 9,1 1,-2-1,0 0,-5 22,1-6,-3 119,8-116</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2408.22">4973 16,'4'-4,"7"-2,5 1,14 9,15 5,0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4599.77">5212 493,'0'5,"0"14,0 14,0 9,0 12,0 1,0 0,0 4,0-3,0-7,-5-12,-15-11,-21-25,-5-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4957.37">4868 810,'4'0,"15"0,27 0,19 5,4 6,-3 0,-2 0,-8-4,-8-1,-9-3,-6-2,-4 0,-3-1,-5-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5616.42">5450 625,'4'-9,"11"-7,2-6,4 1,-3 0,5-6,4-3,-4 31,-5 24,-6 22,-5 16,-3 1,-3 0,-2-7,0-14</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7746.51">502 3509,'-2'1,"1"-1,0 1,0-1,0 1,0-1,0 1,0 0,-1 0,2-1,-1 1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 1,0-1,-1 2,-4 41,5-39,-1 7,1 0,0 1,0-1,2 0,-1 0,1 0,1 0,0 0,9 19,-10-26,1 0,0 0,0 0,1 0,0-1,-1 0,1 1,1-1,-1-1,1 1,-1-1,1 1,0-1,0-1,1 1,-1-1,1 0,-1 0,1 0,-1-1,1 0,7 1,-9-2,-1 0,1 1,-1-1,1-1,-1 1,1 0,-1-1,1 0,-1 0,1 0,-1 0,0 0,0-1,0 0,0 1,0-1,0 0,3-3,-2 0,1 0,-1 0,0 0,0 0,0-1,-1 0,0 0,0 0,2-6,2-12,-1 0,-1 0,4-50,-7-102,-4 93,4 519,-15 212,11-633,1-1,-2 0,0 0,-1 0,0 0,-1 0,0-1,-1 0,-11 17,12-23,-1 0,0 0,0-1,0 0,-1 0,0 0,0-1,0 0,-1-1,0 1,0-2,0 1,0-1,0 0,-1-1,-13 3,-45 4,0-4,0-2,-89-8,146 5,0-1,0 0,1 0,-1-1,1-1,-1 0,-12-5,19 6,-1 0,0-1,1 1,0-1,-1 1,1-1,0 0,0-1,1 1,-1 0,1-1,-1 0,1 1,0-1,0 0,1 0,-1 0,-1-8,-2-18,1-1,1-53,-4-28,-13-19,16 101</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8451.03">925 4064,'4'0,"2"14,0 18,-1 12,-2 3,-1 3,-1-2,0-6,3-5,2-17,-1-22,-1-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8843.03">1058 3747,'4'5,"2"5,-1 33,4 23,0 9,-1 0,-2 2,-3-8,-1-12,-1-5,-1-27,0-16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9278.03">1031 4091,'4'0,"7"0,5 0,5 0,3 0,2 0,1 0,-4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9858.03">1243 3959,'1'-1,"1"0,0-1,-1 1,1-1,-1 1,0-1,1 0,-1 1,0-1,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1-2,5-11,17-23,2 2,53-61,-7 10,29-59,-99 144,1 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 1,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,3 0,-3 1,0 1,-1-1,1 1,-1-1,1 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,0-1,-1 1,1-1,0 1,-1-1,1 4,6 12,-1 0,-1 1,-1 0,-1 0,1 20,2 98,-6-94,-1 420,0-405</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4229 473,'-1'-4,"1"0,0 1,1-1,-1 0,1 0,-1 0,1 0,1 0,-1 1,0-1,2 0,-1 0,0 1,0-1,0 2,1-2,-1 1,1 0,0 0,1 0,-1 1,0-1,1 1,-1 0,1 0,-1 0,2 0,-1 1,0-1,-1 1,1 0,1 0,-1 0,8-1,1 2,-1-1,1 1,-1 1,1 0,-1 1,1 0,-1 1,0 0,0 1,-1 0,12 6,26 15,-2 3,48 36,-11-6,-82-56,0-2,0 2,0-1,0 0,1 1,0-1,-1 0,1 0,-1-1,0 1,1 0,-1-1,1 1,-1-1,2 0,-2 0,3 0,13-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="509.52">4755 168,'-5'0,"-6"5,-6 9,-4 12,-5 13,-1 5,3 4,6-1,2-6,-2-5,2-4,4-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1899.21">4728 549,'15'-1,"1"-2,1 0,-2-1,1 0,0-1,-2 0,1-2,0 0,-1 1,25-18,-13 8,48-19,-65 31,0 1,-1 0,2 1,-2 0,2 1,-1 0,0 0,1 1,-2 0,12 1,-18-1,1 1,0-1,-1 1,2-1,-1 1,-1 0,1 0,-1 0,1 0,-1 1,0-1,0 1,2 0,-2 0,0-1,-1 1,1 1,0-1,0-1,-1 1,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-2 0,1-2,-1 2,1 4,-1 8,1 2,-2-2,0 0,-6 22,2-6,-3 113,8-110</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2408.21">5197 15,'4'-3,"8"-3,4 1,16 9,15 4,0 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4599.76">5447 473,'0'5,"0"13,0 14,0 8,0 12,0 1,0-1,0 5,0-3,0-7,-6-12,-14-10,-23-24,-5-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4957.37">5087 777,'4'0,"16"0,28 0,20 5,4 6,-3-1,-2 1,-8-5,-9 0,-9-3,-7-2,-4 0,-2-1,-6-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5616.42">5695 600,'5'-9,"10"-6,3-6,4 0,-3 1,5-6,4-2,-4 29,-5 23,-7 21,-4 15,-4 1,-3 1,-2-7,0-14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7746.51">525 3367,'-3'1,"2"-1,0 1,0-1,0 0,0 0,0 1,0 0,-1 0,2-1,-1 1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 1,0-1,-1 1,-5 41,6-39,-1 8,1 0,0 0,0-1,2 1,-1 0,2-1,0 1,0-1,9 19,-10-25,2-1,-1 1,0 0,1 0,0-1,-1-1,2 2,0-1,-1-1,1 1,-1-1,2 1,-1-2,0 0,1 1,-1-1,2 0,-2 0,1 0,-1-1,2 0,6 1,-8-2,-2 0,1 1,-1-1,1-1,-1 1,1 0,0-1,0 0,-1 0,1 0,-1 0,0 0,0-1,1 0,-1 1,0-1,0 0,3-2,-2-1,2 0,-2 0,0 0,0 1,0-2,0 0,-1 0,0 1,2-7,2-11,0 0,-2 0,4-48,-7-98,-4 89,4 499,-15 202,11-606,1-2,-2 1,-1-1,0 1,0-1,-1 0,0 0,-2-1,-10 17,11-22,0 0,0-1,-1 0,1 0,-1 0,0-1,-1 0,1 0,-1-1,-1 1,1-3,0 2,-1-1,1 0,-2-1,-13 3,-47 3,0-3,0-2,-93-8,153 5,-1-1,1 0,1 0,-2-1,2 0,-2-1,-12-5,20 6,-1 0,0-1,1 1,0 0,-2 0,2-1,0 0,0-1,1 1,-1 0,1-1,-2 1,2 0,0-1,0 0,1 0,-1 0,-1-7,-2-18,1-1,0-50,-3-28,-14-17,17 96</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8451.03">967 3899,'4'0,"2"14,0 16,0 12,-3 4,-1 1,-1 0,0-7,3-5,2-15,0-22,-2-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8843.03">1106 3595,'4'5,"2"4,-1 33,5 21,-1 9,-1 0,-1 2,-4-8,-1-11,-1-6,-1-25,0-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9278.03">1077 3925,'5'0,"6"0,6 0,5 0,3 0,2 0,1 0,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9858.03">1299 3798,'1'-1,"1"0,0-1,-1 2,1-2,-1 1,0-1,1 0,0 1,-1-1,0 0,0 0,0 0,0 0,-1 0,1 0,-1 1,1-3,5-11,18-21,2 1,56-58,-8 10,30-57,-102 138,0 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 1,0 0,0-1,0 1,0 1,2-1,-2 0,0 0,0 0,3 0,-3 1,0 1,-1-1,1 1,-1-1,2 1,-2 0,1-1,-1 1,0-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,0-1,-1 1,1-1,0 1,-1-1,1 4,7 11,-2 0,-1 1,-1 1,0-1,0 19,2 95,-6-91,-1 403,0-388</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7038,45 +7166,45 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 450,'1'-11,"0"-1,1 1,1-1,0 1,1 0,0 0,0 0,1 1,1-1,0 1,0 0,1 1,0 0,12-12,7-6,2 0,1 2,33-23,-52 42,0-1,0 1,0 1,0 0,1 0,0 1,0 0,0 1,23-3,-27 5,0 1,0 0,-1 0,1 1,0 0,0 0,0 0,-1 1,1 0,-1 0,1 1,-1 0,0 0,0 1,0-1,-1 1,10 9,0 1,-1 2,0-1,-2 2,0 0,18 33,36 100,-25-51,-17-44,28 62,116 194,-158-298,0 1,1-2,0 1,1-1,0-1,1 0,0-1,1-1,0 0,0 0,1-1,28 10,-15-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="552.99">1218 0,'0'9,"-9"17,-26 30,-11 20,-11 19,-14 16,-13 3,-24 22,-2-3,13-15,18-27,18-25,15-20,16-12,12-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2080">1588 1297,'1'-9,"0"-1,1 1,1-1,0 1,0 0,1 0,4-9,9-21,-11 19,1 1,1 0,1 0,0 1,2 0,0 1,1 0,0 1,2 1,0 0,0 0,2 1,19-13,-33 25,-1 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 1,1-1,0 1,0 0,0-1,0 1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0 2,4 8,-1 0,0 0,-1 0,0 0,1 19,5 102,-11 167,-1-96,1-91,4 117,-1-218,0 0,1 0,0 0,0 0,1 0,1 0,0-1,6 12,-8-20,0 0,1 1,-1-1,1 0,0 0,0-1,0 1,0-1,0 1,0-1,1 0,-1 0,1 0,0-1,-1 1,1-1,0 0,0 0,0 0,0 0,0-1,0 0,0 0,0 0,0 0,0 0,0-1,4-1,-5 1,0 1,0-1,0 0,-1 0,1-1,0 1,-1-1,1 1,-1-1,1 0,-1 0,0 0,1 0,-1 0,0-1,-1 1,1-1,0 1,-1-1,2-2,14-31</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2695.99">1985 397,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4019.99">2858 741,'14'0,"-1"-2,1 0,0 0,17-6,20-4,247-16,-581 61,166-18,92-10,42-2,47-2,-60-1,165-2,-120 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5546.99">4049 741,'7014'0,"-6982"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15260.58">4393 1482,'5'0,"0"-1,0 0,0 0,0 0,0-1,0 0,0 0,0 0,0-1,-1 0,1 1,-1-2,0 1,0 0,0-1,0 0,-1 0,4-4,31-27,-33 31,4-3,0 0,0 1,0 0,1 1,13-5,-21 9,-1 1,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,2 2,-1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 1,-1-1,0 0,0 0,0 1,-1 1,-1 23,-10 46,0 7,6-41,-1-1,-1 0,-28 71,31-94,-1 2,1 0,1 0,0 1,1 0,1 0,1-1,0 1,2 0,0 0,5 29,-5-43,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 0,0 0,0 0,4 2,1-1,-1-1,1 1,-1-1,1 0,0-1,0 0,12 0,-3-1,1-1,-1-1,1 0,-1-1,0-1,23-9,-31 11,-1-1,1 0,-1-1,0 0,0 0,0-1,-1 0,0 0,0-1,0 0,-1 0,1 0,-1-1,-1 0,1 0,-2-1,1 1,6-14,9-31,23-99,-28 92,29-74,-36 109,0 0,-1-1,5-44,-29 237,6-85,6-45,-17 52,14-61,1 1,1 0,-2 44,8-67,-1 2,1 1,0-1,0 1,1 0,1-1,2 11,-3-17,0-1,1 1,-1-1,0 1,1-1,0 1,0-1,-1 0,1 0,1 0,-1 0,0 0,0 0,1-1,-1 1,1-1,-1 0,1 0,0 0,-1 0,1 0,0 0,0-1,4 1,53 3,-33-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16598.58">5292 2091,'-1'-9,"1"0,1-1,0 1,0-1,1 1,0 0,3-10,-3 16,-1 0,1 0,0 0,0 0,0 0,1 0,-1 0,1 1,-1-1,1 1,0 0,0 0,0 0,0 0,0 1,0-1,1 1,-1-1,1 1,-1 0,6 0,1-1,-1 0,0 1,1 0,-1 1,18 1,-23-1,-1 1,0 0,0-1,0 1,0 1,0-1,0 0,0 1,0-1,0 1,0 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,-1 1,3 4,8 18,-2 1,0 1,-2 0,-2 0,5 31,8 34,-17-87,-1 0,2 0,-1 1,0-1,1-1,0 1,0 0,1-1,7 9,0-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17424.59">5663 1985,'-5'9,"-6"3,0 4,-4 8,-3 0,-13 6,-5 1,-1 0,6-1,3-5,7-2,7-1,1-4,3 3,4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19072.58">6033 1217,'-2'63,"-1"0,-4-1,-18 75,15-66,2-1,3 1,8 124,1-49,-5-136,1 0,1 0,-1 0,2 0,-1-1,2 1,-1 0,1-1,0 0,1 1,0-1,1-1,0 1,0-1,1 0,13 15,-3-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26106.44">6298 1561,'0'-4,"0"0,1 0,0 0,0 0,0 1,0-1,1 0,0 0,-1 1,1-1,0 1,1-1,-1 1,1 0,-1 0,1 0,0 0,0 1,0-1,1 1,-1-1,1 1,5-2,1-1,0 1,1 0,-1 0,1 1,-1 1,1 0,17-1,-19 3,-1 1,1 0,-1 0,1 1,-1 0,0 1,1 0,-1 0,-1 1,1 0,0 0,-1 0,0 1,0 1,0-1,-1 1,0 0,0 0,0 1,6 10,12 17,-3 0,-1 2,17 39,-24-47,26 47,60 87,-85-140</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26972.44">6959 1614,'-9'0,"1"1,-1-1,1 1,-1 1,1-1,-1 2,1-1,0 1,0 0,1 1,-1-1,-13 10,5 1,0 0,1 1,-26 33,15-18,2 2,1 0,-21 43,0-4,31-48</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27637.44">7118 1985,'0'5,"0"5,0 6,0 5,0 3,0 2,0 2,0-1,0 1,0-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28744.47">7330 1270,'0'12,"2"-1,0 0,0 0,1-1,6 19,4 10,11 62,-5 2,-4 0,-5 0,-3 121,-7-146,1-28,-2 0,-8 55,7-92,0 1,-2-1,1 0,-2 0,0 0,0 0,-1-1,-1 0,0 0,0 0,-1-1,-13 14,4-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36182.71">7753 1403,'14'170,"-7"-113,0 62,-7-49,14 111,-9-151,-3-2,2 0,2 0,0-1,1 0,2 0,17 35,-25-60,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,0-1,0 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,-1 0,1 1,-1-1,0 0,1-1,-1 1,3-2,4-2,1-1,-1 0,-1 0,1-1,-1 0,0-1,9-11,-8 4,-1 0,0-1,-1 0,-1 0,-1 0,0 0,-1-1,-1 0,3-30,8-37,55-270,-60 311,-5 18,1-1,2 1,0 1,2 0,0 0,19-32,-14 35</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55731.54">8256 2276,'-4'1,"1"0,-1-1,1 1,-1 0,1 1,0-1,0 0,-1 1,1 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 1,1 0,0 0,0-1,0 1,0 1,1-1,-1 0,1 0,0 1,0-1,-1 4,1-4,0 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0-1,0 1,0 0,0-1,1 1,0-1,-1 1,1-1,0 0,0 1,0-1,0 0,0-1,1 1,-1 0,1 0,-1-1,4 2,-2-1,-1-1,1 1,0-1,0 0,-1 0,1-1,0 1,0-1,0 0,-1 0,1 0,0 0,0-1,0 1,0-1,-1 0,1 0,0 0,4-3,-4 1,0-1,-1 1,1 0,-1-1,0 0,0 0,0 0,-1 0,1-1,-1 1,0 0,0-1,-1 0,3-8,-3 9,11-32,-12 36,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,2 29,-1 67,-4 178,3-266,-1-1,1 1,-1-1,-1 1,1-1,-1 1,0-1,0 0,-1 0,0 0,-4 6,4-8,0-1,0 0,0 0,0-1,-1 1,1-1,-1 0,0 0,0 0,0 0,0 0,0-1,0 0,0 0,0 0,-1 0,1-1,-5 1,-71 2,-84-6,48-1,115 4,-8 0,0 0,1-1,-1 0,1 0,-13-4,19 5,1-1,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0-1,-1 1,1-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1 0,0 0,-1 0,2-2,2-3,0-1,1 0,0 1,0 0,0 0,0 1,1 0,0 0,12-8,-2 3,1 0,30-12,-13 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56751.54">8732 1429,'0'56,"-2"-1,-2 0,-21 100,5-78,-39 171,49-192,3-1,-1 88,8-103,0-11,0 0,6 33,-4-53,0 1,1-1,-1 1,2-1,0 0,0 0,0-1,1 1,0-1,9 11,35 32,-26-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57751.54">8812 2144,'1'-4,"1"1,-1-1,1 0,0 1,0-1,1 1,-1-1,1 1,0 0,-1 0,1 0,1 0,4-3,6-6,40-44,2 3,111-81,-165 133,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,0 1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,2 0,-1 1,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0-1,0 1,0 0,0 0,0-1,0 5,7 29,-3 0,-1 1,-1 0,-2 0,-4 37,3 79,3-133,1-1,1 1,1-1,1 0,16 34,-21-50,8 19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58785.54">9552 1879,'-31'18,"2"0,-45 37,45-32,-9 8,1 1,2 2,2 2,1 1,-42 64,-7 21,68-102</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59902.54">9499 2435,'4'-4,"7"-7,0 4,0 7,-3 13,-3 8,-2 6,-2 2,0 1,-1 0,-1-1,1-1,-1 0,1-1,0 0,4-5,2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60338.57">9711 2196,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61708.63">9870 1323,'14'18,"0"0,-1 0,12 22,7 11,15 18,49 93,-83-135,0 2,-2 0,-1 0,-2 0,0 1,5 56,-8 5,-4 0,-4 0,-16 94,14-152,-1 0,-2-1,-2 0,0-1,-2 0,-2 0,0-2,-2 0,-1 0,-2-2,0 0,-30 31,29-42,5-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="62329.06">10478 2117,'4'0,"7"0,5 0,14 0,15 0,14 0,5 0,6 0,17 9,4 3,-10 0,-14-3,-14-2,-11 1,-13 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63736.06">10743 794,'286'-2,"306"5,-267 22,28 0,633-20,-528-8,1698 3,-2110 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73095.44">12119 1482,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1-1,-1 1,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 0,2 0,1 1,-1 0,0 0,1 0,-1 1,1-1,-1 1,0 0,0 0,1 0,-1 1,0-1,0 1,0-1,-1 1,1 0,0 0,-1 1,1-1,-1 0,4 5,45 57,-42-50,-1 1,0 0,-1 0,-1 0,0 1,-1 0,-1 0,-1 0,3 22,-3 15,-4 85,-1-50,-12 57,1 1,13-141,-1 5,1 0,0 1,1-1,0 0,1 0,4 14,-5-21,0 0,1-1,-1 1,1 0,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,0 1,-1-1,1-1,0 1,0 0,0-1,1 1,5-1,15 2,1-1,-1-1,1-1,0-1,40-9,-59 9,0-1,0 0,-1 0,1 0,-1-1,0 0,0 0,0 0,0-1,-1 1,0-1,0 0,0-1,-1 1,1 0,-1-1,-1 0,3-7,3-9,-1-1,-1 0,5-35,42-173,-3 18,5-60,-69 475,10-174,-1-1,-1 1,-19 52,16-56,1 0,1 0,1 1,2 0,-3 33,10 337,-4-387,2 0,-1 0,1 0,0-1,1 1,0 0,0-1,5 11,-5-14,0-1,0 1,0-1,1 0,0 1,-1-1,1-1,0 1,0 0,0-1,1 1,-1-1,1 0,-1 0,1 0,0-1,7 3,11 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74868.96">13045 2355,'-2'50,"0"-20,3 47,-1-71,1 0,0 0,0 0,0 0,1 0,0-1,0 1,0 0,1-1,-1 0,1 0,1 0,6 9,-7-11,-1-1,0 0,1 1,0-1,-1 0,1 0,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0-1,0 1,1-1,-1 0,1 0,-1 0,5-1,-3 0,-1-1,1 0,-1 0,1 0,-1-1,0 1,0-1,0 0,0 0,-1-1,1 1,-1-1,3-3,5-9,0 0,-1 0,-1-1,-1 0,-1-1,7-21,-14 39,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,2 19,-4 33,-7 29,-4 1,-4-2,-39 119,51-186,-1 1,0-1,-1-1,0 1,-1-1,0 0,-1 0,0-1,-1 0,-1-1,-16 15,18-19,0 0,-1 0,0-1,0 0,0-1,-1 0,1-1,-1 0,0 0,0-1,0 0,0-1,0 0,0 0,-1-1,-12-2,18 1,1 0,0 0,-1 0,1-1,0 0,0 0,0 0,0 0,0 0,1-1,-1 0,1 0,-1 0,1 0,0 0,0-1,1 1,-1-1,1 0,0 0,0 0,0 0,0 0,1 0,-1-1,0-7,-1 2,1-1,1 1,0-1,0 0,1 1,0-1,1 0,0 1,1-1,4-14,-4 20,1-1,0 1,0 0,0 0,1 0,0 0,0 1,0-1,1 1,6-5,-3 1,13-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="76160">13733 1561,'0'76,"2"14,-4-1,-25 160,14-172,3 0,4 0,3 1,9 96,-6-167,1-1,0 0,0 1,1-1,-1 0,1 0,1 0,-1 0,1 0,7 10,-9-14,1 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,-1-1,1 1,0-1,0 1,-1-1,1 0,0 0,0 0,0-1,-1 1,1-1,4-1,10-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="77063.01">14077 2196,'-1'-20,"2"0,0 0,1 1,1-1,1 0,12-36,-13 50,-1 1,1-1,0 0,1 1,-1 0,1 0,0 0,0 0,1 1,-1-1,1 1,0 0,0 1,0-1,1 1,0 0,-1 0,1 1,0 0,0 0,0 0,0 1,0-1,1 2,11-1,-11 1,0 0,0 1,0 0,0 1,0 0,0 0,0 0,-1 1,1 0,-1 0,1 0,-1 1,0 0,-1 1,1-1,-1 1,0 0,9 11,6 10,-1 0,30 57,-29-48,13 25,-2 1,30 89,-57-138,1 0,0 1,0-1,1-1,12 18,-17-28,0 0,0 1,-1-1,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,0 0,2-2,23-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="77611.96">14818 1932,'0'-4,"-9"-2,-8 4,-10 13,-13 12,-32 26,-21 17,-5 2,2 4,8-7,14-5,15-13,18-14</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78508.64">14976 2567,'0'5,"0"5,0 6,0 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79572.64">15241 1561,'4'1,"0"0,1 0,-1 0,0 0,1 1,-1 0,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0 0,1 0,-1 0,3 5,9 12,24 40,-28-42,15 26,-3 2,-2 0,-2 2,-1 0,-3 1,-2 1,10 84,-9 12,-5 205,-9-335,-1 1,-1 0,0 0,-1-1,-1 1,0-1,-1 0,-1 0,0-1,-1 0,-1 0,-1 0,0-1,0 0,-2-1,1 0,-2-1,0 0,-14 11,2-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="81189.64">15876 1667,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 2,2 3,85 316,72 310,-152-595,-4-18,0 0,1 0,2 0,-1-1,17 34,-21-51,0 0,-1 0,1 1,0-1,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,0-1,0 1,1-1,0 1,-1-1,0 0,0 0,0 0,0 0,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0-1,-1 0,1 1,-1-1,1 0,-1 0,1 0,4-8,-1 0,0-1,-1 1,3-12,-3 10,22-74,106-331,-88 299,87-168,-103 231,-6 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="82096.77">16564 2858,'-1'-21,"2"0,1 0,0 1,10-39,-10 54,-1 0,1 0,0 0,0 0,0 1,1-1,-1 0,1 1,0 0,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,1 0,-1 1,1 0,0-1,0 2,0-1,10-2,-10 4,0 0,1 0,-1 1,0 0,0 0,0 0,0 1,0-1,0 1,0 0,0 1,-1-1,1 1,-1 0,0 0,0 0,0 1,0-1,0 1,-1 0,0 0,5 7,8 12,0 1,21 46,-32-59,9 16,-2 1,0 0,-2 0,-1 1,-1 1,-2 0,3 38,-9-64,1-1,-1 1,0 0,1 0,0 0,0-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1-1,1 1,0-1,1 0,-1 1,0-1,1-1,-1 1,1-1,-1 1,1-1,0 0,-1 0,1 0,7 0,22-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="82597.3">17146 2620,'-5'0,"-5"5,-7 1,-8 8,-9 7,-13 9,-12 8,-8 7,-12 8,3-3,1 2,9-7,11-7,6-6,12 1,7 0,4-2,7-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83822.3">17596 1747,'-2'1,"1"-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 2,-14 36,10-26,-107 305,93-263,1 2,4 0,2 0,2 2,3-1,1 74,5-58,5 308,-4-378,0-1,0 1,1-1,-1 0,1 1,-1-1,1 1,0-1,0 0,1 0,-1 1,1-1,0 0,-1 0,6 5,10 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="84676.3">18072 2408,'-2'0,"1"-1,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,-1 1,1 0,0-3,-3-41,3 39,1-1,0 0,0 1,1-1,-1 1,1-1,1 1,-1 0,1 0,1 0,-1 0,1 0,0 1,7-9,-9 12,0 0,0 0,0 1,1-1,-1 1,0 0,0-1,1 1,-1 0,1 0,-1 1,1-1,-1 0,1 1,0 0,3-1,-2 2,-1-1,1 1,-1 0,0 0,0 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,0 1,-1-1,5 5,5 7,-2-1,1 2,-2-1,0 1,-1 1,0 0,7 22,30 125,-3-7,-39-148,3 9,0 0,2-1,16 30,-22-43,1 0,-1 1,1-1,-1 0,1 0,0 0,0-1,1 1,-1-1,0 1,1-1,-1 0,1-1,0 1,0-1,-1 1,1-1,0 0,0 0,0-1,0 1,9-1,1-3,0 0,0-1,0 0,0-2,-1 1,0-2,0 1,0-2,21-16,15-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85121.3">18575 2064,'-9'0,"-26"0,-20 9,-10 12,-2 12,-13 22,-7 20,4 6,-8 12,4-1,6-2,14-8,17-9,18-17</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="86062.3">18575 2779,'9'0,"1"-1,-1-1,1 0,-1 0,0-1,0 0,0-1,0 0,0 0,15-11,7-7,41-37,-24 19,-11 17,-36 22,0 1,0 0,0-1,0 1,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 1,0-1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,-1-1,1 1,0-1,-1 1,1 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,1 14,0 1,-1-1,-1 1,0-1,-1 1,-7 30,-32 106,30-120,0-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="86994.3">18998 1905,'5'1,"0"0,1 0,-1 0,0 1,0 0,0 0,0 0,0 0,0 1,0 0,-1 0,0 0,1 1,-1-1,4 6,4 3,0 2,-1-1,11 20,-9-8,-2 0,-1 1,-1 0,-1 1,-2 0,7 52,-4-27,10 45,-5 1,-3 0,-6 193,-8-271,0 0,-2 0,0-1,-1 1,-1-1,-1 0,-1-1,-14 24,1-8,-1-1,-2-1,-35 36,40-49,-1-1,0-1,-1 0,-1-2,0-1,-1 0,-43 16,31-18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 430,'1'-10,"0"-2,1 2,1-2,0 2,2-1,-1 1,0-1,1 2,1-2,1 2,-1-1,1 2,0-1,13-11,7-6,2 0,1 2,35-22,-55 41,1-2,-1 1,0 1,1 1,0-1,1 1,-1 0,1 1,23-2,-28 4,0 1,1 0,-2 0,1 1,1 0,-1-1,0 1,-1 1,2 0,-2 0,1 1,-1 0,1 0,-1 1,0-2,-1 2,11 9,-1 0,0 2,0 0,-3 1,0 0,20 32,36 96,-25-50,-18-41,29 59,121 185,-165-284,0 0,2-1,-1 0,2 0,-1-2,2 1,-1-2,2 0,-1-1,1 1,0-1,30 9,-16-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="552.99">1266 0,'0'9,"-9"15,-28 30,-10 19,-13 18,-13 15,-15 3,-24 21,-2-3,13-14,19-26,18-24,16-19,17-11,12-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2080">1651 1241,'1'-9,"0"0,1 0,1-1,0 2,0-1,1 1,5-10,8-19,-10 18,0 1,1 0,2-1,-1 2,2 0,1 1,0-1,1 2,1 1,1-1,-1 1,3 1,19-13,-33 24,-2 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 1,1-1,0 1,0 0,1-1,-1 1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0 0,-1-1,1 1,1 0,-2 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,0 2,4 8,0-1,-1 0,-1 1,0-1,1 19,6 97,-13 160,0-92,1-86,4 111,-1-209,0 1,2-1,-1 0,0 1,1-1,1 1,0-2,7 12,-9-19,0 0,1 1,-1-1,1 0,0 0,0-1,0 0,0 0,1 1,-1-1,1 0,-1 0,1 0,0-1,-1 1,2-1,-1 0,0 0,0 0,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,5-2,-6 1,0 1,0-1,0 0,-1 0,1-1,0 1,-1-1,2 1,-2-1,1 0,-1 0,0 0,1 0,-1 1,0-2,-1 1,1-1,0 1,-1-1,3-2,13-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2695.99">2063 380,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4019.99">2971 709,'15'0,"-2"-2,2 0,-1 0,18-6,21-3,257-16,-604 59,172-18,96-9,44-2,49-2,-63-1,171-2,-124 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5546.99">4209 709,'7292'0,"-7259"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15260.58">4567 1418,'5'0,"0"-1,0 0,1 0,-1 0,0-1,0 0,0 0,1 0,-1-1,-1 0,1 2,-1-3,0 1,1 0,-1-1,0 0,-1 1,4-5,33-26,-35 31,4-4,1 0,-1 1,0 1,2 0,13-5,-22 9,-1 1,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,2-1,-2 1,0-1,0 1,0-1,2 2,-1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1 1,-1-1,0 0,0 0,0 1,-1 0,-1 23,-10 44,-1 7,7-40,-1-1,-2 1,-28 67,32-90,-1 3,0-1,2 0,0 1,1 0,1 1,1-2,0 1,2 0,0 1,5 27,-5-42,1 0,-1 0,1 0,-1 0,1 0,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 1,1-1,0 0,0 0,1 0,3 1,1 0,-1-1,2 1,-2-1,1 0,1-1,-1 0,13 0,-4-1,2-1,-1-1,1 0,-2-1,1-1,23-8,-31 10,-2-1,1 0,0-1,-1 1,0-1,1-1,-2 0,0 0,1 0,-1-1,-1 0,1 0,0 0,-2-1,1 0,-2 0,1 0,7-13,9-30,23-94,-28 87,30-70,-38 104,0 0,0-1,4-42,-30 227,7-82,6-42,-18 49,15-59,0 2,2 0,-2 42,8-65,-1 3,1 1,0-2,0 2,1-1,1 0,2 10,-3-16,0-1,1 1,-1-1,0 0,1 0,0 1,0-1,-1 0,2 0,0 0,-1 0,0 0,0 0,1-1,-1 0,1 0,-1 0,1 0,1 0,-2 0,1 0,0 0,0-1,4 1,56 3,-35-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16598.58">5501 2000,'-1'-8,"1"-1,1-1,0 2,0-2,1 2,1-1,2-9,-3 15,-1 0,1 0,0 0,0 1,0-1,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,0 1,0-1,0 1,0-1,2 1,-2-1,1 1,-1 0,6 0,2-1,-2 0,0 1,2 0,-2 1,19 1,-24-1,-1 1,1 0,-1-1,0 1,0 1,0-1,0 0,0 1,0-1,1 1,-1 0,-1 0,1-1,-1 1,0 1,0-1,1 1,-1-1,-1 1,4 3,7 18,-2 1,1 1,-3 0,-2 0,6 29,8 33,-18-83,-1 0,2 0,-1 0,0 0,1-1,0 1,0 0,1-2,8 10,-1-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17424.59">5887 1899,'-5'8,"-7"4,1 3,-5 8,-2 0,-15 6,-4 1,-2-1,7 0,3-5,7-2,8-1,0-4,4 3,4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19072.58">6272 1164,'-2'60,"-2"1,-3-2,-19 72,16-63,1-1,4 1,8 118,2-46,-7-130,2-1,2 1,-2-1,2 1,-1-1,2 0,-1 1,1-2,0 1,1 0,0 0,2-1,-1 0,0 0,1 0,14 14,-3-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26106.44">6547 1493,'0'-4,"0"1,1-1,0 0,0 0,0 1,0-1,1 1,0-1,-1 1,2-1,-1 1,1-1,-1 2,1-1,-1 0,1 0,0 0,0 1,1-1,0 1,-1-1,1 2,5-3,2-1,-1 1,2 0,-2 0,1 2,0 0,0 0,18-1,-19 3,-2 1,1 0,0 0,0 1,-1 0,1 0,0 1,-1 0,0 1,0 0,0 0,-1 0,1 0,-1 2,0-1,0 1,-1-1,0 1,0 1,7 9,12 17,-3-1,-2 2,19 38,-26-45,28 45,62 83,-89-134</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26972.44">7234 1544,'-9'0,"1"1,-2-1,2 1,-1 1,0-1,0 2,1-1,-1 0,1 1,1 1,-2-1,-13 9,6 2,-1-1,2 2,-28 30,16-16,2 2,1-1,-22 42,1-4,31-46</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27637.44">7400 1899,'0'5,"0"4,0 7,0 4,0 3,0 1,0 3,0-1,0 1,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28744.47">7620 1215,'0'11,"2"0,0-1,0 1,1-1,7 17,3 11,12 58,-5 3,-5-1,-4 1,-4 115,-7-139,1-28,-2 1,-8 53,7-89,0 2,-3-2,2 0,-2 1,0-1,0 1,-2-2,0 1,0-1,0 1,-2-2,-13 14,5-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36182.71">8060 1342,'14'163,"-7"-109,1 60,-8-47,14 106,-9-144,-2-2,1-1,2 1,0-1,1 0,3 0,17 33,-26-57,1 0,-1 0,1 0,-1 0,1 0,0-1,0 0,0 1,1-1,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,0 0,0 1,-1-1,0 0,1-1,-1 1,3-2,5-1,0-2,-1 0,0 0,0 0,-1-1,1-1,8-10,-7 4,-2-1,0 0,0 0,-2-1,-1 1,0 0,-1-1,-1-1,4-28,7-35,58-259,-63 298,-4 17,0-1,2 2,0 0,3 0,-1 0,20-31,-14 34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55731.54">8583 2177,'-5'1,"2"0,-1-1,1 1,-1 0,1 1,0-1,-1 0,0 1,1 0,0 0,0 0,1-1,-1 1,0 1,1-1,-2 1,2 0,0 0,0-1,0 1,0 0,1 0,-1 0,1 0,0 1,0-1,-1 3,1-3,0 0,0 0,1 0,-1 0,1 0,-1-1,1 0,0 1,0 0,1 0,-1 0,1 0,-1 0,1-1,0 1,0-1,0 1,0 0,0-1,1 1,0-1,-1 1,1-2,0 1,0 1,0-1,0 0,1-1,0 1,-1 0,1 0,-1-1,4 2,-2-1,-1-2,2 2,-1-1,0 0,-1 0,1-1,0 1,0-1,1 0,-2 0,1 0,0 0,0-1,0 1,1-1,-2 0,1 0,0 0,4-2,-4 0,1-1,-2 1,1 0,-1-1,0 1,0-1,0 0,-1 0,2-1,-2 1,0 1,0-2,-1 0,3-7,-3 8,12-31,-13 35,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,2 28,-1 64,-4 170,3-254,-1-1,1 0,-1 0,-1 1,0-2,0 2,0-1,0 0,-1-1,0 1,-4 6,4-9,-1 0,1 0,0 0,0-1,-1 1,1-1,-1 0,0-1,-1 1,1 0,0 0,0-1,0 0,0 0,-1 0,0 0,1-1,-5 1,-74 2,-88-6,50-1,120 4,-8 0,0 0,0-1,0 0,1 0,-14-4,20 5,1 0,0 0,0-1,-1 0,1 1,0-1,0 0,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1 0,0 0,-1 1,2-3,2-3,1-1,0 1,0 0,0 0,0 0,1 2,0-1,0 0,13-7,-3 2,2 0,31-11,-14 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56751.54">9077 1367,'0'54,"-2"-2,-2 1,-22 95,5-74,-40 163,51-183,2-2,0 85,8-99,0-10,0 0,6 31,-4-50,0 0,2 0,-2 0,2 0,0 0,0-1,0 0,1 0,1 0,8 10,37 31,-27-28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57751.54">9161 2051,'1'-4,"1"1,-1-1,1 1,0 0,0-1,1 1,-1-1,1 1,0 0,-1 1,2-1,0 0,4-3,7-5,41-43,2 3,116-77,-172 127,0 0,-1-1,1 1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,1 1,0-1,-1 1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,3 0,-2 1,-1 0,0-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0-1,0 0,0 1,1 0,-1-1,0 5,7 27,-3 1,-1 0,-1 0,-2 1,-4 35,3 75,3-127,2-1,0 1,1 0,1-1,17 32,-22-47,9 18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58785.54">9930 1797,'-32'18,"1"-1,-46 36,47-31,-9 7,0 2,3 1,2 3,0 0,-43 62,-7 19,71-96</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59902.54">9875 2329,'4'-3,"7"-8,1 4,-1 7,-3 13,-2 7,-3 6,-2 1,0 2,-1 0,-1-1,1-2,-1 1,1-1,0 0,4-5,2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60338.57">10095 2101,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61708.63">10260 1266,'15'17,"-1"0,0 0,12 22,7 9,16 18,51 89,-87-129,1 2,-3 0,0-1,-3 1,0 1,6 53,-9 5,-4 0,-4 0,-17 90,15-145,-1-1,-2 0,-3 0,1-2,-3 1,-1-1,-1-1,-1 0,-2 0,-2-2,0-1,-31 31,31-41,4-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="62329.06">10892 2025,'5'0,"6"0,6 0,14 0,16 0,14 0,5 0,7 0,18 9,3 2,-10 1,-14-4,-15-1,-11 1,-14-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63736.06">11168 760,'297'-2,"319"5,-279 20,30 1,658-19,-548-8,1764 3,-2193 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73095.43">12598 1418,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 0,-1 0,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,3-1,0 1,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1 1,0-1,0 1,0-1,-1 1,2 0,-1 0,-1 1,1-1,-1 0,4 4,47 55,-43-47,-2 0,0 1,-1-1,0 0,-1 2,-1-1,-1 0,-1 0,4 22,-4 14,-4 81,-1-48,-13 54,2 2,13-135,-1 4,1 1,0 1,1-2,0 1,1-1,4 14,-5-20,0 0,1-1,-1 1,1 0,0-2,0 1,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,1 0,-2 0,1-1,0 1,0 0,0-1,1 1,6-1,15 2,1-1,-1-1,1-1,-1-1,43-8,-62 8,1-1,-1 0,-1 0,1 0,-1 0,1-1,-1 0,0 0,0-1,-1 1,1 0,-1-1,0-1,-1 1,1 1,-1-2,-1 0,4-6,2-9,-1-1,-1 0,6-34,43-165,-3 17,5-57,-72 454,11-166,-1-1,-1 1,-20 49,17-53,0 0,2 0,1 1,2 0,-4 32,11 321,-4-369,2 0,-1-1,1 1,0-1,2 0,-1 1,0-1,5 10,-5-13,0-1,0 0,0 0,1 0,1 1,-2-1,1-1,0 1,0 0,0-2,1 2,-1-1,2 0,-2 0,1 0,0-1,7 3,12 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74868.95">13561 2253,'-2'48,"0"-20,3 46,-1-68,1-1,0 1,0 0,0 0,1-1,0 0,0 1,0 0,1-2,0 1,0 0,1 0,6 8,-7-10,-1-1,0 0,2 1,-1-1,-1 0,1 0,0-2,0 2,0-1,0 1,0-1,1 0,0 0,-1 0,0-1,0 1,1-1,-1 0,2 0,-2 0,5-1,-3 0,-1-1,2 0,-2 0,1 0,-1 0,0 0,0-1,1 0,-1 0,-1-1,1 1,-1 0,3-4,6-8,-1-1,0 1,-2-1,-1-1,0 0,6-20,-14 37,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,2 19,-4 30,-7 29,-4 0,-5-1,-40 113,53-177,-1 0,-1-1,0 0,0 0,-1 0,-1-1,0 1,0-2,-2 1,0-2,-17 15,19-18,-1 0,0-1,0 0,-1 0,1-1,-2 0,2-1,-1-1,-1 1,1-1,-1 0,1-1,0 0,-1 0,0-1,-13-2,19 1,1 0,-1 0,0 0,1-1,0 0,0 1,0-1,-1 0,1 0,1-1,-1 0,1 0,-1 0,1 0,-1 1,1-2,1 1,-1-1,1 0,0 0,0 1,0-1,0 0,1 0,-1-1,0-6,-2 1,2 0,1 0,0 0,0-1,1 2,0-2,1 1,0 0,1-1,5-12,-5 18,1-1,0 1,0 0,0 1,1-1,1 0,-1 1,0-1,1 2,6-6,-2 1,13-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="76160">14276 1493,'0'73,"2"13,-4-1,-26 153,15-164,2 0,5-1,3 2,9 91,-6-159,1-1,0 0,0 0,1 0,-1 0,1 0,2-1,-2 1,1 0,7 9,-9-13,1 0,0 0,0 0,0 0,1-1,0 0,-1 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,0-1,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,0-1,0 1,0-1,4-1,11-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="77063">14634 2101,'-1'-19,"2"-1,0 1,1 1,1-1,1 0,13-35,-14 49,-1 0,1-1,0 0,1 2,0-1,0 0,0 0,0 0,1 2,-1-2,2 1,-1 0,0 1,0-1,1 2,1-1,-2 0,1 1,0 0,1 0,-1 0,0 1,0-1,2 2,10-1,-10 1,-1 0,0 1,0 0,1 1,-1 0,0 0,0 0,0 1,0 0,-1 0,1-1,0 2,-1 0,-1 1,1-1,0 0,-1 1,9 11,7 8,-1 1,31 55,-30-47,13 25,-2 0,32 85,-60-131,1-1,0 2,0-2,2 0,11 17,-17-28,0 1,0 1,-1-1,1 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,2 0,-2 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,0 0,2-2,24-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="77611.95">15404 1848,'0'-4,"-9"-1,-9 3,-10 12,-14 12,-32 25,-23 16,-5 2,2 4,9-7,14-4,15-13,20-14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78508.64">15568 2456,'0'4,"0"6,0 5,0 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79572.64">15844 1493,'4'1,"0"0,1 0,0 0,-1 0,1 1,-1 0,0 0,0 0,0 0,1 0,-2 0,1 1,-1 0,0 0,1 0,-1 0,4 4,8 13,26 37,-30-40,16 25,-3 2,-2 0,-2 2,-2 0,-2 1,-2 1,9 80,-8 12,-6 195,-9-319,-1 0,-1 0,0 1,-1-2,-1 1,0-1,-1 1,-2-1,1-1,-1 1,-1-1,-2 0,1 0,-1-1,-1 0,1-1,-3 0,1-1,-15 11,2-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="81189.64">16504 1595,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 0,1 0,0 1,0 0,-1-1,1 1,0 0,-1 0,1-1,-1 1,1 0,-1 0,0 0,2 0,-2-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 2,2 2,88 303,75 297,-157-570,-5-16,0-1,1 0,2 0,-1-1,18 33,-22-49,0 0,-1 0,1 1,0-1,1 0,-2 0,1 0,0 0,0 0,0 0,0-1,0 1,1-1,-1 1,0 0,0-1,0 1,1-1,0 1,-1-1,0 0,0 0,0 0,0 0,0-1,-1 1,1 0,0-1,1 1,-2-1,1 1,0-1,0 1,-1-1,1 1,0 0,-1-1,1 1,-1-1,1 0,-1 0,1 0,4-8,-1 1,0-2,-1 1,4-11,-4 10,23-72,110-316,-91 287,90-162,-107 221,-6 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="82096.77">17219 2734,'-1'-20,"2"0,1 0,0 1,11-38,-11 52,-1 1,1-1,0 0,0 0,0 1,1 0,-1-1,2 1,-1 0,1 0,-1 1,1-1,0 0,0 1,1-1,-1 1,0 0,1 1,-1 0,1 0,1-1,-1 2,0-1,11-2,-11 4,0 0,1 0,-1 1,1 0,-1 0,0 0,0 1,0-1,1 1,-1 0,0 1,-1-2,1 2,0 0,-1 0,0 0,0 1,0-1,0 0,-1 1,1 0,4 7,9 11,-1 1,23 44,-34-57,9 16,-1 1,-1 0,-1-1,-2 2,-1 1,-1-1,2 37,-9-61,1-1,-1 1,0 0,1 0,0-1,0 0,0 1,0 0,1-1,-1 1,1-1,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1-1,1 0,0 0,2 0,-2 1,0-1,1-1,-1 1,1-1,-1 1,2-1,-1 0,-1 0,1 0,7 0,24-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="82597.3">17824 2506,'-5'0,"-5"5,-8 1,-8 7,-9 7,-14 9,-13 7,-7 7,-13 8,3-3,1 2,9-7,12-7,6-5,12 0,8 1,4-3,7-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83822.3">18292 1671,'-2'1,"1"-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 2,-15 35,11-26,-111 292,96-251,1 1,5 1,1-1,3 3,3-2,0 72,6-57,6 296,-5-362,0-2,0 2,1-1,-1 0,1 1,-1-1,1 1,0-2,0 1,1 0,-1 1,1-1,0 0,-1 0,6 4,11 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="84676.3">18787 2304,'-2'0,"1"-1,0 1,0-1,-1 0,0 1,1-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,0-1,-1 1,1 0,0-3,-3-39,3 37,1-1,0 1,0 0,1-1,-1 2,1-2,1 1,-1 0,1 1,2-1,-2 0,1 0,0 2,7-10,-8 12,-1 0,0 1,0 0,1-1,-1 1,0 0,0-1,1 1,-1 0,1 0,0 1,0-1,-1 0,1 1,0 0,3-1,-2 2,0-1,0 1,-1 0,0 0,0 0,1 1,-1-1,0 1,1-1,-1 1,-1-1,1 1,0 1,-1-1,5 5,6 6,-3 0,2 1,-3-1,0 2,0 0,-1 0,8 22,30 119,-2-7,-41-141,3 8,1 0,1-1,17 29,-23-41,1 0,-1 1,1-1,-1 0,1 0,1-1,-1 0,1 1,-1-1,0 1,1-1,-1 0,2-1,-1 1,0-1,-1 1,1-2,0 1,0 0,1-1,-1 1,9-1,2-3,-1 1,1-2,-1 0,1-2,-1 1,-1-1,1 0,-1-2,22-15,16-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85121.3">19310 1974,'-10'0,"-26"0,-21 9,-11 11,-1 12,-15 20,-6 20,4 6,-9 11,5-1,5-2,16-8,17-8,19-17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="86062.3">19310 2658,'9'0,"1"-1,0 0,0-1,0 0,-1-1,0 0,1-1,-1 0,0 1,16-12,8-6,41-35,-24 17,-11 17,-38 21,0 1,0 0,0-1,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,2-1,-1 1,0-1,0 1,-1-1,1 1,0-1,-1 1,1 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,1 13,0 1,-1-1,-1 2,0-2,-1 1,-7 29,-34 101,32-114,-1-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="86994.3">19749 1822,'6'1,"-1"0,1 0,-1 0,0 1,1 0,-1 0,0 0,0 0,0 1,1-1,-2 1,0 0,1 1,-1-1,5 6,3 2,1 2,-2 0,12 18,-10-7,-1 0,-2 1,0 0,-2 1,-2 0,8 49,-5-25,11 43,-6 0,-2 1,-7 185,-8-260,0 0,-2 0,-1-1,0 1,-1-1,-2 1,0-2,-15 23,1-7,-1-2,-2 0,-36 34,41-47,-1-1,1-1,-2 1,-1-3,0-1,-1 1,-45 15,33-18</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7103,7 +7231,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'2805'0,"-2677"10,-118-9,39 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'2964'0,"-2828"10,-126-9,42 4</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7159,12 +7287,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">822 1085,'-2'101,"4"110,-1-206,0 1,0-1,0 0,1 1,0-1,0 0,0 0,0 0,1 0,0 0,4 5,-6-9,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0-1,1 1,-1 0,0-1,1 1,-1-1,0 0,1 1,-1-1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,0-1,2-2,0-1,0 1,-1-1,0 1,0-1,0 0,-1 0,0 0,1-7,-2 7,1 0,0 0,1 0,-1 0,1 1,0-1,1 0,3-7,-5 12,-1 0,0 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,-1-1,1 1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,2 6,0-1,0 0,-1 1,0 0,2 8,4 43,-3-1,-3 1,-5 62,0-28,3-76,0-1,-1 1,-1-1,-4 16,5-27,0 1,-1-1,1 0,-1 0,0 0,0-1,-1 1,1 0,-1-1,1 0,-1 1,0-1,0 0,-1 0,1-1,0 1,-1-1,0 1,-5 1,-8 3,0-1,-1-1,0 0,0-2,0 0,-23 1,33-4,0 1,1-1,-1-1,1 0,-1 0,1 0,-1-1,1 0,0 0,0-1,0 0,0 0,0 0,1-1,0 0,-1-1,-10-9,14 8,-1 1,1-1,0 0,0 0,1 0,0 0,0 0,0-1,1 1,0-1,0 1,1-1,-1 1,2-1,0-7,-1 4,1 1,1-1,0 0,0 0,1 1,0-1,1 1,0 0,6-11,-4 12,1 0,0 0,0 0,13-10,4-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="906.97">1536 0,'-21'24,"2"1,0 0,2 2,1 0,1 0,-12 34,-1 21,3 0,-14 91,34-150,-9 55,-7 151,20 81,2-281,0-19,0-1,0 0,1 0,1-1,-1 1,2 0,-1-1,1 0,0 0,1 0,0 0,10 12,-4-6,1-1,1-1,0 0,0-1,24 16,-9-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2049.97">1695 556,'0'0,"0"-1,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,2 0,37 11,-37-12,14 8,0 0,0 1,-1 1,-1 0,1 1,-2 0,0 1,21 24,1 7,44 70,-71-101,9 13,-1 0,-1 1,-1 0,-1 1,-2 0,9 31,-19-50,1-1,1 1,-1-1,1 0,1 0,-1 0,7 9,-9-14,1 0,-1-1,1 1,-1 0,1 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,1 0,-1-1,0 0,1 1,-1-1,1 0,-1 0,0 0,1-1,4 0,20-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2660.97">2356 423,'-18'5,"-15"15,-11 12,-11 11,-6 6,-5 5,3-3,4 3,7-7,9-7,6-2,10 2,9-1,8 1,1-5,3-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4229.65">2647 979,'-5'0,"4"0,6 0,2 9,9 8,2 5,-2 3,-5 2,-3 2,-3-1,-3 0,-1 0,-1-1,-1 0,0 4,1 1,-1 5,1-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5463.65">2938 106,'10'1,"0"-1,0 1,0 1,0-1,0 2,-1-1,1 2,-1-1,1 1,-1 0,0 1,-1 0,1 1,-1 0,0 0,0 1,-1 0,0 0,0 0,-1 1,0 0,0 1,-1-1,6 12,7 19,-2 1,-2 1,-1 0,10 60,-8-33,-2-7,-2 0,-3 1,-3 0,-3 0,-8 96,3-141,0-1,-1 0,-1-1,0 1,-1-1,-1 0,-13 22,-67 92,71-108,-1 4,-1 0,-1-2,-1 0,-1-2,-41 34,37-39</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">828 1050,'-2'97,"4"107,-1-199,0 1,0-1,0 0,1 1,0-2,1 1,-1 0,0 0,1 0,0 0,4 4,-6-8,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0-1,2 1,-2 0,0-1,1 1,-1-1,0 0,1 1,-1-1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,0 0,1-1,-1 1,0-1,1 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,0 0,2-3,0-1,0 1,-1-1,0 1,0 0,0-1,0 0,-1 0,1-6,-2 6,1 0,0 0,1 0,-1 1,1 0,0-1,1 0,3-6,-5 11,-1 0,0 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,1 0,-2-1,1 1,0 0,0 0,-1-1,1 1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,2 5,0 0,1 0,-2 1,0-1,2 9,4 41,-3-1,-3 1,-5 60,0-27,3-73,0-2,-1 2,-1-2,-4 16,5-26,0 1,-1-1,1 0,-1 0,0 0,-1-2,0 2,1 0,-1-1,1 0,-1 1,0-1,0 0,-1 0,1-1,0 0,-2 0,1 1,-5 1,-9 3,1-1,-2-1,1-1,-1-1,1 0,-25 1,35-4,0 1,1-1,-2-1,2 0,-1 0,1 0,-2-1,2 0,0 0,0-1,-1 1,1-1,0 0,1-1,0 0,-2-1,-9-8,14 7,-1 1,1-1,-1 0,1 1,1-1,0 0,0 0,0-1,1 2,0-2,0 1,1-1,-1 1,2 0,0-8,-1 4,1 2,1-2,0 0,0 1,1 0,0-1,2 2,-1-1,6-10,-4 11,1 0,1 0,-1 1,14-11,3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="906.97">1565 0,'-22'23,"3"1,-1 1,3 1,0 0,2 0,-13 33,-1 20,3 1,-14 87,35-145,-10 54,-6 145,19 79,4-272,-1-18,0-1,0-1,1 1,1-1,-1 0,2 1,-1-1,1 0,0-1,1 1,1 0,9 11,-4-5,2-2,0 0,1 0,-1-2,25 16,-9-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2049.97">1729 538,'0'0,"0"-1,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1-1,1 1,1 0,-1 0,0 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,2 0,38 11,-38-12,15 8,-1-1,1 2,-2 1,0-1,0 2,-1 0,-1 0,22 24,1 7,46 67,-74-97,10 12,-2 0,0 1,-2 0,-1 1,-1 0,8 31,-19-50,2 0,0 1,-1-1,1-1,1 1,-1 0,7 8,-9-13,1 0,-1-1,1 1,0 0,0 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,1 0,-1-1,1 0,0 1,-1-1,1 0,-1 0,0 0,1-1,4 0,21-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2660.97">2411 409,'-18'5,"-16"14,-12 12,-11 11,-6 5,-5 6,3-4,4 3,8-6,8-8,7-1,10 2,10-1,7 0,2-4,3-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4229.65">2712 947,'-6'0,"5"0,6 0,3 9,8 7,3 6,-3 2,-4 2,-4 2,-3-1,-3 0,-1 0,-1-1,-1 0,0 4,1 1,-1 5,1-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5463.65">3012 103,'10'1,"0"-1,1 0,-1 2,0-1,1 2,-2-1,1 2,0-1,0 1,-1 0,0 1,0-1,0 2,-1 0,1 0,-1 1,-1-1,0 1,0 0,0 1,-1-1,0 2,-1-1,7 11,6 19,-1 1,-3 0,0 1,9 58,-7-33,-3-6,-2 0,-2 1,-4 0,-3 0,-8 93,3-136,0-2,-2 1,0-2,0 2,-1-2,-1 1,-14 20,-69 90,74-104,-2 3,0 0,-2-2,-1 0,0-1,-43 32,38-38</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7272,9 +7400,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 212,'2'21,"1"0,1-1,1 0,1 0,0 0,15 29,3 11,12 77,-28-97,27 76,5-27,61 96,-85-157,-14-24,0-1,0 1,0 0,1-1,0 0,-1 0,6 5,-8-8,1 0,-1 1,1-1,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1-1,2 1,12-19,43-125,4-9,-45 121,2 0,0 2,2 0,2 2,0 0,30-27,-27 30,-2 0,0-2,-2 0,-1-2,18-33,-24 35</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1861.99">4525 900,'4'0,"7"-4,5-2,5 0,3 1,2 2,1 1,5 1,2 0,3 1,1 0,3 1,-2-1,2 0,-2 0,2 0,-1 0,-9 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14623">7912 185,'15'-12,"2"1,-1 0,2 1,-1 0,1 2,20-7,-22 9,-7 1,0 2,0 0,1 0,0 0,0 1,-1 1,1 0,0 0,13 1,-18 1,0 0,1 0,-1 0,0 1,1 0,-1 0,0 0,-1 0,1 1,0 0,-1 0,1 0,-1 1,0-1,0 1,0 0,-1 0,4 5,6 10,-1 1,-1 1,-1-1,0 2,-2-1,0 1,-2 0,-1 1,4 29,-3-1,-3 1,-3-1,-5 58,0-82,-1 0,0-1,-2 0,-2 0,0-1,-1 0,-28 44,24-44,1 0,1 1,2 1,0 0,2 1,-9 42,17-66,0 0,1 0,0-1,0 1,0 0,0 0,0 0,1 0,0 0,0-1,0 1,0 0,0-1,1 1,0-1,-1 1,1-1,1 0,-1 1,0-1,5 4,-3-4,0-1,0 0,0 1,0-2,0 1,0 0,0-1,1 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,-1-1,1 1,-1 0,8-3,-6 2,0-1,1-1,-1 1,0-1,0 0,0 0,-1-1,1 1,-1-1,0-1,0 1,0-1,0 0,-1 0,5-7,7-12,-2-1,17-36,5-8,-24 48,172-308,-162 274,-3-1,21-108,-11 43,-21 93,1 0,1 0,2 1,1 1,1-1,17-24,-15 36,-14 29,-15 32,-109 269,98-245,2 1,4 1,-18 146,17-111,12-75,1 0,1 1,2-1,2 66,2-92,-1 0,1-1,1 1,-1-1,1 0,0 1,0-1,0 0,1 0,0 0,0 0,0-1,0 1,1-1,0 0,0 0,0 0,5 4,3-1,-1-1,1 0,0 0,0-2,0 1,21 4,-9-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 205,'2'20,"1"1,1-2,2 0,0 1,0-1,16 29,3 10,12 74,-29-93,29 73,4-26,64 93,-88-152,-15-23,0-1,0 1,0 0,1-1,0-1,-1 1,7 5,-9-8,1 0,-1 1,1-1,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1-1,2 1,13-18,44-122,4-8,-46 117,1 0,1 2,2 0,2 2,0 0,31-26,-28 29,-3 0,1-2,-2-1,-1-1,18-32,-24 34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1861.99">4697 871,'4'0,"8"-4,4-2,6 0,3 1,2 2,1 1,5 2,3-1,2 1,2 0,2 1,-1-1,1 0,-1 0,1 0,0 0,-10 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14623">8213 179,'16'-12,"2"2,-2-1,3 1,-2 1,2 1,21-7,-24 10,-6 0,-1 2,0 0,2 0,-1 0,0 1,0 1,0 0,0 0,14 1,-18 1,-1 0,1 0,-1 0,0 1,2 0,-2 0,0 0,-1 0,1 1,0 0,0 0,0 0,-1 0,0 0,0 1,0 0,0 0,3 5,6 9,0 1,-2 2,0-2,-1 2,-2 0,1 0,-3 0,-1 1,4 29,-2-2,-4 1,-3 0,-6 55,1-79,-1 0,0 0,-2-1,-3 0,1-1,-2 0,-28 43,24-43,2 0,0 1,3 2,-1-1,3 1,-10 41,18-65,0 1,1 0,0-1,0 1,0 0,0 0,0 0,1-1,0 1,0-1,0 1,1 0,-1-1,1 1,0-1,-1 0,1 0,1 0,-1 1,0-1,5 4,-3-4,1-1,-1 0,0 0,0-1,0 1,0 0,1-1,0 0,-1 0,1 0,-1 0,1-1,0 1,0-1,-1-1,1 1,-1 0,9-3,-7 2,0-1,1-1,0 1,-1 0,0-1,0 0,0-1,0 1,-1-1,0-1,0 1,1 0,-1-1,-1 0,5-7,8-11,-3-1,19-35,4-8,-25 47,179-298,-168 264,-3 0,21-104,-10 40,-23 91,1 0,2 0,1 1,2 1,0-1,18-23,-15 34,-15 29,-16 30,-112 261,101-238,2 2,4 1,-18 141,17-108,13-72,1 0,1 1,1-1,3 64,2-89,-1-1,2 0,0 1,-1-1,1 0,0 1,0-2,0 1,1 0,0 0,0 0,0-1,1 0,0 0,0 0,0 0,0 0,5 4,4-2,-2 0,2 0,-1 0,1-2,-1 1,22 3,-9-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7301,15 +7429,15 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">79 1005,'0'2,"0"-1,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,0 1,1-1,1 0,40 5,-38-5,3 0,0 0,0 1,0-1,0 1,0 1,0 0,-1 0,11 3,-16-3,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,-1 0,0 6,1 1,-1-1,1 0,-2 0,1 0,-2 0,1 0,-1 0,0 0,-1 0,0 0,0-1,-1 1,0-1,-1 0,1 0,-2-1,1 1,-1-1,0-1,-1 1,1-1,-1 0,0 0,-1-1,-8 6,-24 11,-30 19,65-38,1 0,-1 1,1 0,-1 0,1 0,1 1,-1-1,0 1,1 0,-4 8,6-11,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,-1 0,4 1,7 3,0-1,0 0,0 0,19 2,-14-3,8 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="513">397 793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9586">1932 1217,'-2'41,"1"-28,0 0,1 0,0 0,1 0,1 0,4 19,-5-30,-1-1,1 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0-1,1 1,-1 0,1 0,-1-1,1 1,-1-1,1 1,1-1,1 1,0-1,0 0,0-1,0 1,0-1,0 1,-1-1,1 0,6-3,5-3,-1 0,0 0,22-18,-7 1,-2 0,-1-2,-1 0,40-57,-65 83,0-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0-1,1 1,-1 0,0 0,0 0,1 0,-1 0,0-1,1 1,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,1 0,-1 0,0 0,1 1,4 18,-6 40,0-51,0 171,-2 35,1-204,1 1,-2-1,1 0,-2 0,1 0,-1 0,-1-1,1 1,-2-1,1-1,-1 1,-1-1,1 1,-1-2,-1 1,-10 7,-14 11,-1-2,-64 35,83-51,2-1,-1-1,1 1,-2-2,1 0,-18 4,29-8,0-1,0 1,0-1,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,0-1,0 1,0-1,0 0,0 1,0-1,0 0,1 0,-1 0,1 1,-1-1,1 0,0 0,0 0,-1 0,1 0,1 0,-1 0,0 0,1-2,-1-1,0 0,1 0,-1 1,1-1,0 0,0 1,1-1,0 1,0-1,0 1,0 0,0 0,1 0,0 0,0 0,0 0,0 1,0 0,1-1,0 1,-1 0,1 1,6-4,5 0,0 0,1 1,-1 0,1 1,23-2,-16 2,6-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10609">2963 0,'-13'32,"2"1,1-1,1 2,3-1,0 1,-1 50,-3 7,-16 68,-7 70,29-187,2-1,2 1,8 61,-6-89,2 0,-1 0,2-1,-1 1,2-1,0 0,1-1,13 20,2-2,2-1,27 25,-28-30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11527">3254 820,'0'-18,"-1"-10,7-50,-5 71,0 0,1 0,0-1,0 1,0 0,1 0,0 1,1-1,0 1,0 0,8-11,-9 14,0 0,1 1,-1-1,0 1,1 0,0 0,-1 0,1 0,0 1,0-1,0 1,0 0,0 0,0 1,0-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 1,0 0,0 0,0 1,0-1,0 1,4 2,7 4,0 1,0 0,-1 1,-1 0,18 18,1 4,-2 2,-1 0,31 51,57 120,-44-39,-51-113,-11-33,-1-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12402">3837 476,'-5'14,"-5"13,-11 11,-6 12,-12 12,-4 9,-12 5,3 4,5-8,7-16,10-12,11-11,7-5,7-3,3-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13547.99">4207 1111,'4'0,"2"5,0 5,-2 11,-1 6,-1 3,-1 0,0 1,-1-2,0 0,-1-1,1-1,0-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13941">4154 846,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15049">4419 211,'10'1,"0"-1,0 1,0 1,0 0,0 0,0 1,0 0,-1 1,1 0,-1 1,16 10,-12-6,-1 1,1 1,-2 0,0 1,0 0,16 26,-7-5,-1 2,-2 0,-2 1,-1 1,13 52,-4-3,-3 1,-4 1,8 166,-23-208,-8 54,4-83,0 0,-2 0,1 0,-2-1,0 1,-12 20,2-12,0-2,-2 0,-1-1,0 0,-26 21,-33 36,59-58,2-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">82 973,'0'2,"0"-1,1-1,0 1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,1 0,-1 1,1-1,1 0,41 5,-39-5,4 0,-1 0,0 1,1-1,-1 1,0 1,0 0,0 0,10 2,-16-2,1 0,-1 0,1 0,0 0,-1 0,0 0,0 0,0 1,-1-1,1 1,-1-1,1 0,-1 1,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,-1 0,0 5,1 2,-1-1,1-1,-2 1,1 0,-2 0,1-1,-1 1,0 0,-1-1,0 1,0-1,-1 1,0-2,-2 1,2 0,-2-1,1 0,-1 0,-1-1,0 1,1-2,-1 1,0 0,-2-1,-7 6,-26 10,-30 18,67-36,1 0,-2 1,2 0,-1 0,1 0,1 1,-1-2,0 2,0 0,-3 8,6-11,0 0,1 0,-1-1,1 0,-1 1,1 0,0 0,-1 0,1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0-1,0 0,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,2 0,-2 1,1-1,-1 0,1 0,0 0,-1 0,4 1,7 3,1-2,-1 1,1 0,19 2,-15-3,9 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="513">411 767</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9586">1999 1178,'-2'39,"1"-26,0 0,1-1,0 1,1-1,1 1,5 18,-6-29,-1-1,1 1,-1-1,1 1,0-1,0 0,0 1,0-2,0 1,0 0,0 1,0-1,0 0,1 0,-1 0,0-1,1 1,-1 0,1 0,-1-1,1 1,-1-1,1 1,2-1,0 1,0-1,0 0,0-1,0 1,0-1,1 1,-2-1,1 0,6-3,6-2,-2-1,1 0,22-17,-7 1,-2-1,-1-1,-1 0,41-55,-67 80,0-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0-1,1 1,-1 0,0 0,0 0,1 0,-1 0,0-1,1 1,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,1 0,-1 0,0 0,1 1,4 17,-6 39,0-49,0 165,-2 34,1-197,1 1,-2-2,1 1,-2 0,1-1,-1 1,-2-1,2 1,-2-2,1 0,-1 1,-2-2,2 2,-1-2,-1 1,-11 6,-14 11,-1-1,-67 33,87-50,2 0,-2-1,2 1,-3-2,2-1,-19 5,30-8,0-1,-1 1,1-1,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,1-1,-2 0,1 1,0-1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,1 0,-1 0,1 1,-1-1,1 0,0 0,0 0,-1 0,1 0,1 1,-1-1,0 0,1-2,-1-1,0 0,1 0,-1 1,1 0,0-1,0 1,1-1,0 1,0-1,0 1,0 1,0-1,1 0,0 0,0 0,1 0,-1 1,0 0,1 0,0 0,-1 0,1 1,7-4,4 0,1 0,0 2,0-1,0 1,25-2,-17 2,6-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10609">3066 0,'-13'31,"1"1,2-1,1 2,3-1,-1 1,0 48,-3 7,-17 66,-7 67,30-180,2-1,2 0,8 60,-6-86,2-1,-1 1,2-2,-1 2,3-2,-1 1,1-1,14 19,2-2,1-1,29 24,-29-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11527">3367 794,'0'-18,"-1"-9,8-48,-6 68,0 0,1 0,0 0,0 0,0 0,1 0,0 1,1 0,0 0,1 0,7-10,-9 13,0 0,1 1,-1-1,1 1,0 0,0 0,-1 0,1 0,0 1,0-1,1 1,-1 0,0 0,0 1,0-1,0 1,1 0,0 0,-1 0,0 1,0-1,0 1,0 0,0 0,1 1,-1-1,0 1,4 2,8 4,-1 0,1 1,-2 1,0 0,18 17,1 4,-2 2,-1-1,32 51,59 115,-45-37,-54-110,-10-32,-2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12402">3971 461,'-5'13,"-6"13,-10 11,-7 12,-13 11,-3 8,-13 6,3 3,5-7,8-16,10-11,11-11,8-5,7-3,3-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13547.99">4354 1075,'4'0,"2"5,0 5,-2 10,-1 6,0 3,-2 0,0 1,-1-2,0 0,-1-1,1 0,0-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13941">4299 819,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15049">4573 204,'10'1,"1"-1,-1 1,0 1,1 0,-1 0,1 1,-1 0,-1 1,2-1,-2 2,17 10,-13-6,0 0,0 2,-2 0,1 0,-1 1,17 25,-7-6,-2 3,-1 0,-2 1,-2 1,14 50,-4-3,-3 1,-5 2,9 159,-24-200,-8 52,4-81,0 1,-3-1,2 0,-2 0,0 0,-13 20,3-12,-1-1,-2-1,0-1,-1 1,-26 19,-35 36,61-57,3-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7336,9 +7464,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 76,'-1'0,"1"-1,0 0,-1 1,1-1,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,0 1,1-1,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,38-19,-34 17,8-3,1-1,1 2,-1 0,1 0,0 2,0 0,29-1,-37 4,-1-1,1 1,0 0,-1 1,1-1,-1 1,0 1,1-1,-1 1,0 0,-1 0,1 1,0 0,-1 0,0 0,0 1,0-1,-1 1,1 0,5 9,3 8,-1 1,-2 0,0 0,-1 1,-1 1,-1 0,6 41,6 187,-14-154,13 496,-19-583,1 3,0 0,1 1,0-1,1 0,5 18,-6-29,0-1,0 1,1-1,0 0,-1 1,1-1,0 0,1 0,-1 0,0-1,1 1,0 0,-1-1,1 0,0 0,0 1,1-2,-1 1,0 0,1-1,-1 1,0-1,1 0,0 0,-1-1,1 1,3-1,0 1,-1-1,0 0,0-1,1 1,-1-1,0-1,0 1,0-1,0 0,0 0,-1-1,1 0,5-3,-1-1,0-1,0 1,-1-2,0 1,-1-1,10-13,0-5,0 0,-2-2,-1 0,14-38,-11 11,-2 0,11-71,-21 84,3 1,1 0,2 1,2 1,1 0,22-40,69-78,-64 99,61-113,-68 110,-25 47,0-1,-2 0,0-1,9-25,-17 41,0 1,0 0,1-1,-1 1,0-1,0 1,0 0,0-1,0 1,0-1,1 1,-1 0,0-1,0 1,0-1,0 1,0 0,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1 0,1-1,0 1,0 0,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,0 0,-19 7,-18 23,20-8,2 2,0 0,-22 47,-28 87,39-89,-26 52,-43 119,86-208,1 0,1 1,2 0,2 1,-1 52,6-59,2-1,1 0,1 0,2-1,0 0,2 0,17 36,-9-26,2-2,1 1,2-2,35 40,-50-63,0-1,1 0,0-1,0 0,1 0,0 0,0-1,0-1,1 0,0 0,0 0,13 3,1-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1096.99">1326 1373,'2'1,"0"-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,1 1,-1-1,1 1,-1 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 5,10 60,-11-66,-1 187,-1-120,5 68,4-113,-6-23,-1 0,1-1,-1 1,1 0,0 0,-1 0,1-1,-1 1,1 0,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1-1,0 1,1-1,-1 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 0,11-27</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1522">1511 1003,'-5'0,"-1"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 73,'-1'0,"1"-1,0 0,-1 1,1-1,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,0 1,1-1,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1-1,1 1,-1-1,1 1,1 0,-2-1,1 1,0 0,-1-1,1 1,0 0,0 0,40-18,-36 16,9-3,1-1,1 2,-2 1,2-1,0 2,0 0,30-1,-38 4,-2-1,1 1,1 0,-2 1,2-1,-2 1,0 1,2-2,-2 2,0 0,0 0,0 1,0 0,-1-1,1 1,-1 1,0-1,0 1,0-1,5 10,4 7,-1 1,-3 0,1 0,-2 1,0 1,-2-1,7 41,6 177,-15-146,14 473,-20-556,1 2,0 0,1 2,0-2,1 0,6 18,-7-28,0-2,0 2,1-1,0 0,-1 1,1-1,0 0,2-1,-2 1,0-1,1 1,0 0,-1-1,1 0,1 0,-1 1,1-3,-1 2,0 0,2-1,-2 1,0-1,1 0,0 0,0-1,0 1,3-1,1 1,-2-1,0 0,1-1,0 1,-1-1,1-1,-1 1,0-1,1 0,-1 0,-1 0,2-1,4-3,0-1,-1 0,1 0,-2-2,1 2,-2-2,11-12,0-5,0 1,-2-3,-1 0,15-36,-12 11,-3-1,13-67,-23 80,4 1,0-1,3 2,2 1,1 0,23-39,73-73,-68 93,65-107,-72 105,-27 44,1 0,-3 0,1-2,9-23,-18 39,0 1,0 0,1-1,-1 1,0-1,0 1,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,0 1,0-1,0 1,0 0,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,-2 0,2-1,0 1,0 0,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,0 0,-20 7,-19 21,21-7,2 2,0 0,-23 45,-30 83,42-85,-28 50,-45 113,90-199,2 1,0 0,3 1,2 0,-2 51,7-58,3 0,0 0,1 0,2-1,1 0,1 0,19 34,-10-25,2-1,1 0,2-1,37 38,-52-61,-1 0,2 0,-1-2,0 1,2 0,-1-1,1 0,-1-1,2 0,0-1,-1 1,14 3,2-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1096.99">1400 1312,'2'1,"0"-1,0 1,0 0,0-1,0 0,0 1,1 0,-1 0,0 0,0 1,0-1,-1 0,1 1,-1-1,1 1,-1 0,2-1,-2 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 5,11 57,-12-63,-1 178,-2-114,7 65,3-108,-6-22,-1 0,1-1,-1 1,1 0,0 0,-1 0,1-1,-1 1,1 0,-1 0,1-1,-1 1,1-1,-1 1,2 0,-2-1,1 1,-1-1,0 1,1-1,-1 1,0-1,1 1,-1-1,0 0,0 1,1 0,-1 0,0-1,0 0,0 1,0-1,0 0,11-26</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1522">1595 958,'-5'0,"-2"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7365,9 +7493,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 504,'4'-4,"7"-2,14 1,30 0,38-3,20 0,14 1,-2 2,-7 2,-21 1,-26 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="886.99">81 848,'4'0,"11"5,7 1,4 0,3-1,0-2,0-1,5-1,0 0,-1-1,-1-1,-3 1,18 0,9 0,-1 0,-4-1,-12 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3204.99">1377 2,'26'0,"-13"-1,-1 0,0 1,23 4,-32-3,0-1,-1 1,1 0,0 0,-1 0,1 0,-1 0,1 1,-1-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,-1 1,1-1,-1 0,1 1,-1-1,2 3,2 12,-1 0,-1 0,0 0,-1 1,0-1,-2 0,0 1,-3 20,-28 139,31-176,-49 162,35-127,2 1,1 1,2-1,-7 72,16-101,-1 6,0 1,1-1,1 0,0 0,5 19,-5-30,0 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1-1,1 1,1-1,-1 1,0-1,1 1,-1-1,1 0,0 0,-1-1,1 1,0 0,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1-1,4 1,-1-1,0 0,0 0,-1-1,1 0,0 0,-1 0,1-1,0 1,-1-1,0-1,1 1,-1-1,0 0,0 0,0 0,-1-1,1 1,-1-1,0 0,0-1,0 1,-1-1,4-5,7-13,-1-1,-1 0,16-46,-17 39,17-40,1-8,4 3,67-119,-71 145,22-56,8-16,-47 106,-12 26,-14 36,-66 131,-16 40,88-192,0 0,2 1,1 0,-3 47,7 105,4-119,-11 115,4-149,1-14,1 0,1 0,0 0,1 0,0 0,2 12,-2-20,1 0,0 0,0 0,0 0,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,0 1,1-1,-1 0,0 0,1 0,-1 0,1-1,0 1,0-1,-1 1,1-1,0 0,0 0,0 0,4 0,0 1,0-1,0 0,0 0,0-1,0 0,0 0,0 0,0-1,0 0,0-1,0 0,0 0,0 0,-1 0,1-1,-1 0,0-1,0 0,0 0,0 0,-1 0,1-1,-1 0,8-10,2-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 487,'4'-4,"8"-2,14 2,31-1,40-3,21 0,14 2,-2 1,-7 2,-22 1,-27 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="886.99">84 820,'5'0,"10"4,8 2,4 0,3-1,1-2,-1-1,5-1,1 0,-2-1,-1-1,-2 1,18 0,9 0,-1 0,-4-1,-12 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3204.99">1435 2,'27'0,"-14"-1,0 0,-1 1,25 4,-34-3,0-1,-1 1,1 0,0 0,0 0,0 0,-1 0,1 1,-1-1,0 0,1 0,-1 1,0 0,0 0,0 0,1 0,-2 1,1-1,-1 0,1 1,-1-1,2 3,2 11,-1 0,-1 1,1-1,-2 2,0-2,-2 0,0 2,-3 19,-30 134,33-170,-51 156,37-122,1 1,2 0,1 0,-6 70,16-99,-1 7,0 0,1 0,1-1,0 1,5 18,-5-29,0 1,0-2,0 1,1 0,-1 0,1 0,0 0,-1-1,2 1,0-1,-1 1,0-1,1 0,-1 0,1 0,0 0,-1-1,1 1,1 0,-1-1,0 0,1 0,-1 0,0 0,0 0,2 0,-2-1,4 1,-1-1,1 0,-1 0,-1-1,1 0,0 0,0 0,0-1,0 1,-1-1,1-1,0 1,-1-1,0 0,0 1,1-1,-2-1,1 1,-1-1,0 0,1-1,-1 1,-1 0,4-6,8-12,-2-1,0-1,16-43,-18 37,19-39,0-7,4 2,70-114,-73 140,22-55,8-15,-48 103,-13 24,-15 36,-68 126,-17 39,91-186,1 0,2 1,1 0,-4 46,8 101,4-115,-11 111,4-144,1-13,1-1,1 1,0 0,1-1,0 1,2 11,-2-19,1 0,0 0,0 0,0 0,1 0,-1-2,1 2,0 0,-1-1,1 1,0-1,0 1,2-1,-2 0,0 0,1 0,-1 0,1-1,0 0,0 0,-1 1,2-1,-1 0,0 0,0 0,4 0,0 1,1-1,-1 0,0 0,1-1,-1 0,0 0,1 0,-1-1,0 0,0-1,1 0,-1 0,0 0,0 0,0 0,-1-1,0-1,1 0,-1 0,0 0,-1 0,2-1,-2 1,8-11,3-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7394,43 +7522,43 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1588 1297,'1'-9,"0"-1,1 1,1-1,0 1,0 0,1 0,4-9,9-21,-11 19,1 1,1 0,1 0,0 1,2 0,0 1,1 0,0 1,2 1,0 0,0 0,2 1,19-13,-33 25,-1 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 1,1-1,0 1,0 0,0-1,0 1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0 2,4 8,-1 0,0 0,-1 0,0 0,1 19,5 102,-11 167,-1-96,1-91,4 117,-1-218,0 0,1 0,0 0,0 0,1 0,1 0,0-1,6 12,-8-20,0 0,1 1,-1-1,1 0,0 0,0-1,0 1,0-1,0 1,0-1,1 0,-1 0,1 0,0-1,-1 1,1-1,0 0,0 0,0 0,0 0,0-1,0 0,0 0,0 0,0 0,0 0,0-1,4-1,-5 1,0 1,0-1,0 0,-1 0,1-1,0 1,-1-1,1 1,-1-1,1 0,-1 0,0 0,1 0,-1 0,0-1,-1 1,1-1,0 1,-1-1,2-2,14-31</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">1985 397,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">2858 741,'14'0,"-1"-2,1 0,0 0,17-6,20-4,247-16,-581 61,166-18,92-10,42-2,47-2,-60-1,165-2,-120 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">4049 741,'7014'0,"-6982"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">4393 1482,'5'0,"0"-1,0 0,0 0,0 0,0-1,0 0,0 0,0 0,0-1,-1 0,1 1,-1-2,0 1,0 0,0-1,0 0,-1 0,4-4,31-27,-33 31,4-3,0 0,0 1,0 0,1 1,13-5,-21 9,-1 1,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,2 2,-1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 1,-1-1,0 0,0 0,0 1,-1 1,-1 23,-10 46,0 7,6-41,-1-1,-1 0,-28 71,31-94,-1 2,1 0,1 0,0 1,1 0,1 0,1-1,0 1,2 0,0 0,5 29,-5-43,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 0,0 0,0 0,4 2,1-1,-1-1,1 1,-1-1,1 0,0-1,0 0,12 0,-3-1,1-1,-1-1,1 0,-1-1,0-1,23-9,-31 11,-1-1,1 0,-1-1,0 0,0 0,0-1,-1 0,0 0,0-1,0 0,-1 0,1 0,-1-1,-1 0,1 0,-2-1,1 1,6-14,9-31,23-99,-28 92,29-74,-36 109,0 0,-1-1,5-44,-29 237,6-85,6-45,-17 52,14-61,1 1,1 0,-2 44,8-67,-1 2,1 1,0-1,0 1,1 0,1-1,2 11,-3-17,0-1,1 1,-1-1,0 1,1-1,0 1,0-1,-1 0,1 0,1 0,-1 0,0 0,0 0,1-1,-1 1,1-1,-1 0,1 0,0 0,-1 0,1 0,0 0,0-1,4 1,53 3,-33-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">5292 2091,'-1'-9,"1"0,1-1,0 1,0-1,1 1,0 0,3-10,-3 16,-1 0,1 0,0 0,0 0,0 0,1 0,-1 0,1 1,-1-1,1 1,0 0,0 0,0 0,0 0,0 1,0-1,1 1,-1-1,1 1,-1 0,6 0,1-1,-1 0,0 1,1 0,-1 1,18 1,-23-1,-1 1,0 0,0-1,0 1,0 1,0-1,0 0,0 1,0-1,0 1,0 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,-1 1,3 4,8 18,-2 1,0 1,-2 0,-2 0,5 31,8 34,-17-87,-1 0,2 0,-1 1,0-1,1-1,0 1,0 0,1-1,7 9,0-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">5663 1985,'-5'9,"-6"3,0 4,-4 8,-3 0,-13 6,-5 1,-1 0,6-1,3-5,7-2,7-1,1-4,3 3,4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">6033 1217,'-2'63,"-1"0,-4-1,-18 75,15-66,2-1,3 1,8 124,1-49,-5-136,1 0,1 0,-1 0,2 0,-1-1,2 1,-1 0,1-1,0 0,1 1,0-1,1-1,0 1,0-1,1 0,13 15,-3-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">6298 1561,'0'-4,"0"0,1 0,0 0,0 0,0 1,0-1,1 0,0 0,-1 1,1-1,0 1,1-1,-1 1,1 0,-1 0,1 0,0 0,0 1,0-1,1 1,-1-1,1 1,5-2,1-1,0 1,1 0,-1 0,1 1,-1 1,1 0,17-1,-19 3,-1 1,1 0,-1 0,1 1,-1 0,0 1,1 0,-1 0,-1 1,1 0,0 0,-1 0,0 1,0 1,0-1,-1 1,0 0,0 0,0 1,6 10,12 17,-3 0,-1 2,17 39,-24-47,26 47,60 87,-85-140</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">6959 1614,'-9'0,"1"1,-1-1,1 1,-1 1,1-1,-1 2,1-1,0 1,0 0,1 1,-1-1,-13 10,5 1,0 0,1 1,-26 33,15-18,2 2,1 0,-21 43,0-4,31-48</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">7118 1985,'0'5,"0"5,0 6,0 5,0 3,0 2,0 2,0-1,0 1,0-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">7330 1270,'0'12,"2"-1,0 0,0 0,1-1,6 19,4 10,11 62,-5 2,-4 0,-5 0,-3 121,-7-146,1-28,-2 0,-8 55,7-92,0 1,-2-1,1 0,-2 0,0 0,0 0,-1-1,-1 0,0 0,0 0,-1-1,-13 14,4-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12">7753 1403,'14'170,"-7"-113,0 62,-7-49,14 111,-9-151,-3-2,2 0,2 0,0-1,1 0,2 0,17 35,-25-60,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,0-1,0 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,-1 0,1 1,-1-1,0 0,1-1,-1 1,3-2,4-2,1-1,-1 0,-1 0,1-1,-1 0,0-1,9-11,-8 4,-1 0,0-1,-1 0,-1 0,-1 0,0 0,-1-1,-1 0,3-30,8-37,55-270,-60 311,-5 18,1-1,2 1,0 1,2 0,0 0,19-32,-14 35</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13">8256 2276,'-4'1,"1"0,-1-1,1 1,-1 0,1 1,0-1,0 0,-1 1,1 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 1,1 0,0 0,0-1,0 1,0 1,1-1,-1 0,1 0,0 1,0-1,-1 4,1-4,0 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0-1,0 1,0 0,0-1,1 1,0-1,-1 1,1-1,0 0,0 1,0-1,0 0,0-1,1 1,-1 0,1 0,-1-1,4 2,-2-1,-1-1,1 1,0-1,0 0,-1 0,1-1,0 1,0-1,0 0,-1 0,1 0,0 0,0-1,0 1,0-1,-1 0,1 0,0 0,4-3,-4 1,0-1,-1 1,1 0,-1-1,0 0,0 0,0 0,-1 0,1-1,-1 1,0 0,0-1,-1 0,3-8,-3 9,11-32,-12 36,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,2 29,-1 67,-4 178,3-266,-1-1,1 1,-1-1,-1 1,1-1,-1 1,0-1,0 0,-1 0,0 0,-4 6,4-8,0-1,0 0,0 0,0-1,-1 1,1-1,-1 0,0 0,0 0,0 0,0 0,0-1,0 0,0 0,0 0,-1 0,1-1,-5 1,-71 2,-84-6,48-1,115 4,-8 0,0 0,1-1,-1 0,1 0,-13-4,19 5,1-1,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0-1,-1 1,1-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1 0,0 0,-1 0,2-2,2-3,0-1,1 0,0 1,0 0,0 0,0 1,1 0,0 0,12-8,-2 3,1 0,30-12,-13 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">8732 1429,'0'56,"-2"-1,-2 0,-21 100,5-78,-39 171,49-192,3-1,-1 88,8-103,0-11,0 0,6 33,-4-53,0 1,1-1,-1 1,2-1,0 0,0 0,0-1,1 1,0-1,9 11,35 32,-26-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">8812 2144,'1'-4,"1"1,-1-1,1 0,0 1,0-1,1 1,-1-1,1 1,0 0,-1 0,1 0,1 0,4-3,6-6,40-44,2 3,111-81,-165 133,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,0 1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,2 0,-1 1,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0-1,0 1,0 0,0 0,0-1,0 5,7 29,-3 0,-1 1,-1 0,-2 0,-4 37,3 79,3-133,1-1,1 1,1-1,1 0,16 34,-21-50,8 19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">9552 1879,'-31'18,"2"0,-45 37,45-32,-9 8,1 1,2 2,2 2,1 1,-42 64,-7 21,68-102</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">9499 2435,'4'-4,"7"-7,0 4,0 7,-3 13,-3 8,-2 6,-2 2,0 1,-1 0,-1-1,1-1,-1 0,1-1,0 0,4-5,2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">9711 2196,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">9870 1323,'14'18,"0"0,-1 0,12 22,7 11,15 18,49 93,-83-135,0 2,-2 0,-1 0,-2 0,0 1,5 56,-8 5,-4 0,-4 0,-16 94,14-152,-1 0,-2-1,-2 0,0-1,-2 0,-2 0,0-2,-2 0,-1 0,-2-2,0 0,-30 31,29-42,5-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">10478 2117,'4'0,"7"0,5 0,14 0,15 0,14 0,5 0,6 0,17 9,4 3,-10 0,-14-3,-14-2,-11 1,-13 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">10743 794,'286'-2,"306"5,-267 22,28 0,633-20,-528-8,1698 3,-2110 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">12119 1482,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1-1,-1 1,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 0,2 0,1 1,-1 0,0 0,1 0,-1 1,1-1,-1 1,0 0,0 0,1 0,-1 1,0-1,0 1,0-1,-1 1,1 0,0 0,-1 1,1-1,-1 0,4 5,45 57,-42-50,-1 1,0 0,-1 0,-1 0,0 1,-1 0,-1 0,-1 0,3 22,-3 15,-4 85,-1-50,-12 57,1 1,13-141,-1 5,1 0,0 1,1-1,0 0,1 0,4 14,-5-21,0 0,1-1,-1 1,1 0,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,0 1,-1-1,1-1,0 1,0 0,0-1,1 1,5-1,15 2,1-1,-1-1,1-1,0-1,40-9,-59 9,0-1,0 0,-1 0,1 0,-1-1,0 0,0 0,0 0,0-1,-1 1,0-1,0 0,0-1,-1 1,1 0,-1-1,-1 0,3-7,3-9,-1-1,-1 0,5-35,42-173,-3 18,5-60,-69 475,10-174,-1-1,-1 1,-19 52,16-56,1 0,1 0,1 1,2 0,-3 33,10 337,-4-387,2 0,-1 0,1 0,0-1,1 1,0 0,0-1,5 11,-5-14,0-1,0 1,0-1,1 0,0 1,-1-1,1-1,0 1,0 0,0-1,1 1,-1-1,1 0,-1 0,1 0,0-1,7 3,11 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">13045 2355,'-2'50,"0"-20,3 47,-1-71,1 0,0 0,0 0,0 0,1 0,0-1,0 1,0 0,1-1,-1 0,1 0,1 0,6 9,-7-11,-1-1,0 0,1 1,0-1,-1 0,1 0,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0-1,0 1,1-1,-1 0,1 0,-1 0,5-1,-3 0,-1-1,1 0,-1 0,1 0,-1-1,0 1,0-1,0 0,0 0,-1-1,1 1,-1-1,3-3,5-9,0 0,-1 0,-1-1,-1 0,-1-1,7-21,-14 39,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,2 19,-4 33,-7 29,-4 1,-4-2,-39 119,51-186,-1 1,0-1,-1-1,0 1,-1-1,0 0,-1 0,0-1,-1 0,-1-1,-16 15,18-19,0 0,-1 0,0-1,0 0,0-1,-1 0,1-1,-1 0,0 0,0-1,0 0,0-1,0 0,0 0,-1-1,-12-2,18 1,1 0,0 0,-1 0,1-1,0 0,0 0,0 0,0 0,0 0,1-1,-1 0,1 0,-1 0,1 0,0 0,0-1,1 1,-1-1,1 0,0 0,0 0,0 0,0 0,1 0,-1-1,0-7,-1 2,1-1,1 1,0-1,0 0,1 1,0-1,1 0,0 1,1-1,4-14,-4 20,1-1,0 1,0 0,0 0,1 0,0 0,0 1,0-1,1 1,6-5,-3 1,13-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">13733 1561,'0'76,"2"14,-4-1,-25 160,14-172,3 0,4 0,3 1,9 96,-6-167,1-1,0 0,0 1,1-1,-1 0,1 0,1 0,-1 0,1 0,7 10,-9-14,1 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,-1-1,1 1,0-1,0 1,-1-1,1 0,0 0,0 0,0-1,-1 1,1-1,4-1,10-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">14077 2196,'-1'-20,"2"0,0 0,1 1,1-1,1 0,12-36,-13 50,-1 1,1-1,0 0,1 1,-1 0,1 0,0 0,0 0,1 1,-1-1,1 1,0 0,0 1,0-1,1 1,0 0,-1 0,1 1,0 0,0 0,0 0,0 1,0-1,1 2,11-1,-11 1,0 0,0 1,0 0,0 1,0 0,0 0,0 0,-1 1,1 0,-1 0,1 0,-1 1,0 0,-1 1,1-1,-1 1,0 0,9 11,6 10,-1 0,30 57,-29-48,13 25,-2 1,30 89,-57-138,1 0,0 1,0-1,1-1,12 18,-17-28,0 0,0 1,-1-1,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,0 0,2-2,23-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">14818 1932,'0'-4,"-9"-2,-8 4,-10 13,-13 12,-32 26,-21 17,-5 2,2 4,8-7,14-5,15-13,18-14</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">14976 2567,'0'5,"0"5,0 6,0 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">15241 1561,'4'1,"0"0,1 0,-1 0,0 0,1 1,-1 0,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0 0,1 0,-1 0,3 5,9 12,24 40,-28-42,15 26,-3 2,-2 0,-2 2,-1 0,-3 1,-2 1,10 84,-9 12,-5 205,-9-335,-1 1,-1 0,0 0,-1-1,-1 1,0-1,-1 0,-1 0,0-1,-1 0,-1 0,-1 0,0-1,0 0,-2-1,1 0,-2-1,0 0,-14 11,2-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29">15876 1667,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 2,2 3,85 316,72 310,-152-595,-4-18,0 0,1 0,2 0,-1-1,17 34,-21-51,0 0,-1 0,1 1,0-1,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,0-1,0 1,1-1,0 1,-1-1,0 0,0 0,0 0,0 0,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0-1,-1 0,1 1,-1-1,1 0,-1 0,1 0,4-8,-1 0,0-1,-1 1,3-12,-3 10,22-74,106-331,-88 299,87-168,-103 231,-6 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30">16564 2858,'-1'-21,"2"0,1 0,0 1,10-39,-10 54,-1 0,1 0,0 0,0 0,0 1,1-1,-1 0,1 1,0 0,1 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,1 0,-1 1,1 0,0-1,0 2,0-1,10-2,-10 4,0 0,1 0,-1 1,0 0,0 0,0 0,0 1,0-1,0 1,0 0,0 1,-1-1,1 1,-1 0,0 0,0 0,0 1,0-1,0 1,-1 0,0 0,5 7,8 12,0 1,21 46,-32-59,9 16,-2 1,0 0,-2 0,-1 1,-1 1,-2 0,3 38,-9-64,1-1,-1 1,0 0,1 0,0 0,0-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1-1,1 1,0-1,1 0,-1 1,0-1,1-1,-1 1,1-1,-1 1,1-1,0 0,-1 0,1 0,7 0,22-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31">17146 2620,'-5'0,"-5"5,-7 1,-8 8,-9 7,-13 9,-12 8,-8 7,-12 8,3-3,1 2,9-7,11-7,6-6,12 1,7 0,4-2,7-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32">17596 1747,'-2'1,"1"-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 2,-14 36,10-26,-107 305,93-263,1 2,4 0,2 0,2 2,3-1,1 74,5-58,5 308,-4-378,0-1,0 1,1-1,-1 0,1 1,-1-1,1 1,0-1,0 0,1 0,-1 1,1-1,0 0,-1 0,6 5,10 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33">18072 2408,'-2'0,"1"-1,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,-1 1,1 0,0-3,-3-41,3 39,1-1,0 0,0 1,1-1,-1 1,1-1,1 1,-1 0,1 0,1 0,-1 0,1 0,0 1,7-9,-9 12,0 0,0 0,0 1,1-1,-1 1,0 0,0-1,1 1,-1 0,1 0,-1 1,1-1,-1 0,1 1,0 0,3-1,-2 2,-1-1,1 1,-1 0,0 0,0 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,0 1,-1-1,5 5,5 7,-2-1,1 2,-2-1,0 1,-1 1,0 0,7 22,30 125,-3-7,-39-148,3 9,0 0,2-1,16 30,-22-43,1 0,-1 1,1-1,-1 0,1 0,0 0,0-1,1 1,-1-1,0 1,1-1,-1 0,1-1,0 1,0-1,-1 1,1-1,0 0,0 0,0-1,0 1,9-1,1-3,0 0,0-1,0 0,0-2,-1 1,0-2,0 1,0-2,21-16,15-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34">18575 2064,'-9'0,"-26"0,-20 9,-10 12,-2 12,-13 22,-7 20,4 6,-8 12,4-1,6-2,14-8,17-9,18-17</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35">18575 2779,'9'0,"1"-1,-1-1,1 0,-1 0,0-1,0 0,0-1,0 0,0 0,15-11,7-7,41-37,-24 19,-11 17,-36 22,0 1,0 0,0-1,0 1,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 1,0-1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,-1-1,1 1,0-1,-1 1,1 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,1 14,0 1,-1-1,-1 1,0-1,-1 1,-7 30,-32 106,30-120,0-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36">18998 1905,'5'1,"0"0,1 0,-1 0,0 1,0 0,0 0,0 0,0 0,0 1,0 0,-1 0,0 0,1 1,-1-1,4 6,4 3,0 2,-1-1,11 20,-9-8,-2 0,-1 1,-1 0,-1 1,-2 0,7 52,-4-27,10 45,-5 1,-3 0,-6 193,-8-271,0 0,-2 0,0-1,-1 1,-1-1,-1 0,-1-1,-14 24,1-8,-1-1,-2-1,-35 36,40-49,-1-1,0-1,-1 0,-1-2,0-1,-1 0,-43 16,31-18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1588 1266,'1'-9,"0"-1,1 2,1-2,0 1,1 1,0-1,4-8,10-21,-12 19,1 0,2 1,0 0,0 0,3 1,-1 0,2 1,-1 1,3 0,0 1,-1-1,3 2,19-13,-33 24,-2 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 1,1-1,0 1,1 0,-1-1,0 1,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,1 0,-2-1,1 1,0 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 0,0 0,0 1,0-1,0 1,0 0,0-1,1 1,-1 2,4 8,-1-1,0 1,-1-1,0 1,2 18,4 98,-11 162,-1-93,1-88,4 113,-1-211,0 1,1-1,0 1,0 0,1-1,1 1,1-2,5 13,-8-21,0 1,1 1,-1-1,1 0,1 0,-1-1,0 1,0-1,0 1,0-2,1 1,0 0,0 0,0-1,-1 1,1-1,0 0,1 0,-1 0,0 0,0-1,0 0,0 0,1 0,-1 0,0 0,0-1,4-1,-4 1,-1 1,0-1,0 0,-1 0,1-1,0 1,-1-1,2 1,-2-1,1 1,-1-1,0 0,1 0,-1 0,0-1,-1 1,1-1,0 1,-1-1,3-2,13-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">2002 397,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">2913 729,'14'0,"0"-2,1 0,-1 0,18-5,22-5,256-15,-605 59,173-18,96-9,44-2,49-2,-63-1,172-2,-125 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">4155 729,'7316'0,"-7282"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">4514 1444,'5'0,"0"-1,1 0,-1 0,0 0,0-1,0 0,1 1,-1-1,0-1,-1 0,1 1,0-2,-1 1,0 0,0-1,0 1,-1-1,5-4,31-26,-33 30,3-2,0-1,1 1,-1 0,2 1,13-4,-22 8,-1 1,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,2-1,-2 1,0-1,0 1,0-1,2 2,-1 0,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 1,-1-1,0 0,0-1,0 2,-1 1,-1 22,-10 45,-1 6,7-39,-1-2,-2 1,-28 68,32-90,-2 1,2 0,1 1,0 0,1 1,0-1,2-1,0 2,2-1,0 0,6 29,-6-42,1-1,-1-1,1 1,-1 0,1 0,0 0,0 0,0 0,2-1,-2 1,1-1,-1 1,1-2,0 1,0 0,0 0,5 2,0-1,-1-1,2 1,-2-1,1 0,1-1,-1 0,13 0,-3-1,0-1,0-1,1 0,-1-1,-1-1,25-9,-33 12,0-2,0 0,-1-1,1 0,-1 0,1-1,-2 0,0 1,0-2,1 0,-2 0,1 0,0 0,-2-1,1 0,-2 0,1 0,7-14,9-29,24-95,-30 88,31-72,-38 106,1 0,-2-1,6-43,-31 229,6-82,7-43,-18 50,15-59,1 1,0 0,-1 42,8-64,-1 2,1 0,0 0,0 1,1-1,1 0,2 10,-3-16,0-1,1 1,0-1,-1 1,1-1,0 1,0-1,-1 0,1 0,1-1,-1 1,0 0,0 0,1-1,0 1,0-1,-1 0,1 0,0 0,-1 0,1 0,0 0,0-1,5 1,54 3,-33-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">5452 2032,'-1'-9,"1"1,1-2,0 1,0 0,1 0,0 0,3-9,-3 15,-1 0,1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,0 0,0 0,1 0,-1 0,0 1,0-1,1 1,-1-1,1 2,0-1,5 0,1-1,0 0,-1 1,2 0,-2 1,19 1,-24-1,-1 1,1 0,-1-1,0 1,0 1,0-1,0 0,0 0,0 0,1 1,-1 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,-1 1,4 3,7 18,-1 2,-1 0,-2 0,-1 0,4 30,9 33,-18-85,-1 1,2 0,-1 1,0-1,1-2,1 2,-1 0,1-1,7 9,1-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">5839 1930,'-6'8,"-5"4,-1 3,-3 9,-4-1,-13 6,-6 1,0 0,5-2,4-3,7-3,8-1,0-4,4 4,3-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">6225 1188,'-2'61,"-2"0,-3-1,-19 72,16-63,1-2,4 2,8 119,1-47,-5-132,1 1,1 0,-1-1,2 1,-1-1,3 0,-2 1,1-1,0-1,1 2,0-1,1-1,1 0,-1 0,1 0,14 14,-3-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">6501 1520,'0'-3,"0"-1,1 0,0 0,0 0,0 1,0-1,1 1,0-1,-1 1,2-1,-1 1,1-1,-1 1,1 0,-1 0,1 1,0-1,0 1,1-1,0 1,-1-1,1 1,5-2,2-1,-1 2,2-1,-2 0,2 1,-2 1,2 0,17-1,-20 3,0 1,0 0,-1 0,2 1,-2 0,0 1,2 0,-2 0,-1 0,2 1,-1 0,-1 0,1 1,-1 1,0-1,0 0,-1 1,0 0,0 1,7 9,12 17,-3 0,-1 1,17 39,-24-46,26 45,64 85,-90-136</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">7191 1572,'-10'0,"2"1,-2-1,2 1,-1 0,0 0,0 2,1-1,-1 1,1 0,1 1,-2-1,-13 9,6 2,-1-1,1 2,-26 31,14-17,3 2,1 0,-21 41,-1-3,32-47</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">7356 1930,'0'5,"0"4,0 7,0 4,0 3,0 2,0 2,0-1,0 1,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">7578 1240,'0'11,"2"0,0-1,0 1,1-1,6 18,5 9,11 61,-5 1,-5 1,-4-1,-4 117,-7-141,1-26,-2-1,-8 53,7-88,0 0,-3 0,2 0,-2-1,0 1,0-1,-2 0,0-1,0 1,-1-1,0 0,-14 13,4-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12">8019 1368,'14'164,"-6"-109,-1 60,-7-48,15 108,-10-146,-3-2,2 0,2 0,1-1,0 0,2 0,18 34,-26-58,1 0,0 0,0 0,-1 0,1 0,0-1,0 1,0 0,0-1,0 1,0-2,1 1,-1 0,1 0,0 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,-1 0,2 0,-2 0,1 0,-1 0,1-1,-1 1,1-1,-1 0,1 1,0-1,-1 0,1-1,-1 2,3-3,4-2,2-1,-2 0,0 0,0 0,-1-1,1-1,8-10,-7 3,-2 1,0-2,0 1,-2 0,-1-1,0 1,0-2,-2 1,3-30,9-35,57-260,-63 299,-5 18,1-1,3 1,-1 1,2 0,1-1,19-30,-14 34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13">8543 2211,'-4'1,"1"-1,-1 0,1 1,-1 0,1 1,-1-1,1 0,-1 1,1 0,0 0,0 0,1 0,-2 0,1 1,1-1,-1 1,1-1,0 1,0-1,0 1,0 1,1-1,-1 0,1 0,0 1,-1-2,0 5,1-4,0 0,0 0,1 0,-1 0,1 0,-1-1,1 0,0 1,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0-1,0 0,0 1,1-1,0 1,0-1,-1 1,1-1,0 0,0 1,0-1,0 0,0-1,1 0,-1 1,2 0,-2-1,4 2,-2-1,-1-1,1 1,1-1,-1 0,-1 0,1-1,0 1,0-1,1 0,-2 0,1 0,0 0,0-1,0 1,1-1,-2 0,1 0,0 0,4-3,-3 1,-1-1,-1 2,1-1,-1-1,0 0,0 0,1 0,-2 0,1 0,-1 0,0 0,0-1,-1 0,3-7,-3 8,12-31,-13 35,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,2 28,-1 65,-4 171,3-256,-1-1,1 0,-1 0,-1 1,1-1,-1 1,0-2,-1 1,0 0,0 0,-4 5,4-7,0-1,0 0,-1 0,1-1,-1 1,1-1,-1 0,0-1,-1 1,1 0,0 0,0-1,0 0,0 0,-1 0,0 0,1-1,-5 1,-75 2,-87-6,50-1,120 4,-8 0,-1 0,2-1,-1 0,0 0,-13-4,20 5,1-1,0 1,0 0,-1-1,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,-1 0,2 0,-1-1,1 1,-1 0,1 0,0-1,-1 1,1-1,0 1,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,2 0,-1 0,-1 0,2-2,2-3,0 0,1-1,0 1,1 0,-1 1,0 0,1 0,1 0,11-8,-1 4,1-1,31-11,-14 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">9040 1393,'0'54,"-2"-1,-2 0,-22 97,5-76,-41 166,52-186,2-1,0 85,8-100,0-10,0 0,6 32,-4-51,1 0,0 0,-1 1,2-2,0 1,0 0,0-1,2 0,-1 0,10 10,36 32,-27-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">9123 2083,'1'-4,"2"1,-2 0,1-1,0 1,0-1,1 1,-1-1,1 1,0 0,-1 0,2 1,0-1,4-3,7-6,41-42,2 3,117-78,-173 128,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,2 1,-2-1,0 1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,0 1,1 0,-1 1,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-2,0 2,-1 0,0-1,0 1,0 0,0 0,0-1,0 5,7 27,-3 1,0 1,-2-1,-2 1,-4 36,3 75,3-127,1-2,1 1,1 0,2-1,16 33,-22-48,8 18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">9895 1827,'-32'18,"2"-1,-47 36,46-31,-8 8,0 1,3 2,1 2,2 0,-44 63,-8 20,71-99</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">9840 2364,'4'-4,"8"-6,-1 3,1 7,-4 12,-3 9,-2 5,-2 2,0 1,-1 0,-1-1,1-1,-1 0,1-1,0 0,4-5,3-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">10061 2133,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">10227 1291,'15'17,"-1"0,0 1,12 20,7 12,16 16,51 91,-86-131,0 2,-3 0,-1 0,-1 0,-1 1,6 54,-9 4,-4 1,-4 0,-17 91,15-147,-1-1,-3 0,-1 0,-1-1,-1 0,-3 0,1-2,-3 0,-1 0,-2-2,1 0,-33 30,32-41,4-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">10861 2057,'4'0,"8"0,5 0,14 0,16 0,14 0,6 0,6 0,18 9,4 2,-11 1,-14-3,-15-3,-11 2,-13 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">11138 780,'298'-2,"319"5,-277 21,28 0,660-19,-550-8,1771 3,-2201 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">12573 1444,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-2 0,2-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1 0,0 0,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1-1,-1 1,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,1 0,-1-1,0 1,0 0,0 0,0 0,0 1,0-1,0 0,0 1,1-1,-1 0,2 0,1 1,-1 0,1 0,0 0,-1 1,1-1,-1 1,0 0,0 0,2 0,-2 0,0 0,0 1,0-1,-1 1,1 0,1 0,-2 1,1-1,-1 0,4 5,47 54,-43-47,-2 0,0 1,0-1,-2 1,0 0,-1 1,0-1,-2 1,3 20,-3 15,-4 83,-1-49,-13 54,2 2,13-136,-1 5,1 0,0 0,1 0,0-1,1 1,4 13,-5-20,0 0,1-1,-1 1,1 0,1-1,-1 0,0 1,0-2,0 1,0 0,1 0,-1 0,1 0,-1-1,2 1,-1-1,0 0,0 1,-1-1,1-1,0 1,0 0,1-1,0 1,5-1,16 2,1-1,-1-1,1-1,0-1,42-9,-62 9,1-1,-1 0,-1 0,1 1,0-2,-1 0,0 0,0 0,1-1,-2 1,0 0,0-1,0-1,-1 1,2 0,-2 0,-1-1,3-7,3-8,0-1,-2 0,5-34,45-167,-4 17,5-57,-71 458,9-168,0-1,-1 1,-20 50,16-54,2 0,1 0,1 2,1-1,-2 32,10 325,-4-373,2-1,-1 1,1 0,0-1,1 0,0 1,1-1,4 10,-5-13,0-1,0 1,0-1,1-1,0 2,0-1,0-1,0 1,0 0,0-1,1 1,-1-1,1 0,0 0,0 0,0-2,7 4,12 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">13539 2287,'-2'48,"0"-19,3 45,-1-68,1 0,0 0,0-1,0 1,1 0,0-1,0 1,0-1,1 0,-1 0,2 0,0 0,6 8,-7-10,-1-1,1 0,0 1,0-1,-1 0,1 0,0-1,0 1,0-1,1 1,-1-2,0 1,1 0,-1 0,0-1,0 1,1-1,0 0,0 0,-1 0,5-1,-3 0,0-1,0 1,-1-1,1 0,-1-1,1 1,-1-1,0 0,0 0,-1-1,1 1,0 0,2-4,5-9,1 1,-2-1,0 0,-2 0,-1-2,8-19,-15 37,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,2 18,-4 33,-7 27,-5 1,-3-2,-42 115,54-179,-1 0,0 0,-2-2,1 2,-1-2,0 1,-2 0,1-2,-2 1,0-1,-17 14,19-19,-1 1,0 0,-1-1,1 0,0-1,-2-1,2 0,-2 0,1 0,0-1,-1 0,1-1,-1 0,1 0,-2-1,-12-2,19 1,1 0,0 0,-1 0,0-1,1 0,0 0,0 0,0 0,0 0,0 0,0-1,1 0,-1 0,1 0,0 0,0-1,1 1,-2-1,2 1,0-1,0 0,0 0,0 0,1 0,-1-1,0-6,-1 1,1 0,0 0,1-1,0 1,1 0,0-1,1 1,0 0,2 0,3-15,-4 21,1-2,0 1,0 0,0 0,2 1,-1-1,0 1,0-1,1 1,7-5,-4 2,14-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">14257 1520,'0'74,"2"13,-4-1,-27 154,16-166,2 1,5-1,3 1,9 93,-6-161,1-1,0-1,0 2,1-1,0 0,0 0,1-1,-1 1,1 0,7 9,-9-13,1 0,1 0,-1 0,0 0,0-1,1 1,-1 0,0-1,1 0,-1 1,1-1,0 0,0 0,0 0,-1-1,1 1,0-1,0 0,-1 0,2 0,-1 0,0 0,0 0,-1 0,1-1,4-1,11-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">14615 2133,'-1'-19,"2"0,0-1,1 2,2-1,0-1,12-34,-12 49,-2 0,1-1,0 0,1 1,-1 1,1-1,1 0,-1 0,1 1,-1-1,1 2,1-1,-1 1,0-1,1 1,1 0,-2 0,1 1,0 0,1 0,-1 1,0 0,0-1,2 2,10-1,-10 1,-1 0,0 1,1 0,-1 1,0-1,1 1,-1 0,-1 1,1 0,0 0,0 0,-1 1,0 0,0 0,0 0,-1 1,0 0,10 10,6 10,-1 1,31 54,-30-47,13 25,-2 1,32 86,-60-133,1-1,1 2,-1-2,1 0,13 17,-18-27,0 0,0 1,-1-1,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 0,0 1,2-1,-2 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1-1,0 1,-1-1,0 1,0 0,1-1,-1 0,0 0,0 0,2-2,24-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">15388 1879,'0'-4,"-9"-2,-9 4,-10 13,-14 11,-33 25,-22 17,-5 1,2 5,8-7,15-5,15-13,20-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">15553 2491,'0'5,"0"5,0 5,0 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">15830 1520,'4'1,"0"0,1 0,-1 0,0 0,2 1,-2 0,0 0,0 0,0 0,1 1,-2-1,1 1,-1 0,0-1,1 1,-1 0,4 5,8 11,26 39,-30-40,17 24,-4 2,-3 1,-1 1,-1 0,-3 2,-3 0,11 81,-9 12,-6 198,-9-324,-1 2,-1-1,0 1,-1-2,-1 2,0-2,-2 0,0 1,0-2,-1 1,-2-1,0 1,-1-2,1 1,-2-2,0 1,-1-2,-1 1,-14 10,2-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29">16492 1623,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0-1,-1 1,1-1,-1 1,1 0,-1 0,0 0,2 0,-2-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 2,2 3,88 304,76 300,-158-574,-5-17,0-1,1 0,2 1,-1-2,18 33,-22-49,0 0,-1 0,2 1,-1-1,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,0-1,0 1,1-1,0 0,-1 0,0 0,0 0,0 0,1 0,-1 0,-1 0,1 0,0-1,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0-1,-1 0,1 1,-1-1,1 0,-1 0,1 0,4-8,-1 0,1 0,-2 0,3-11,-3 9,23-71,111-319,-92 288,90-162,-107 223,-6 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30">17210 2772,'-1'-20,"2"0,1-1,0 2,10-38,-10 52,-1 1,1-1,1 0,-1 0,0 1,1-1,-1 1,1 0,0 0,1 0,0 0,0 0,0 0,0 2,0-2,0 1,1 0,0 0,-1 1,1 0,0-1,1 2,-1-1,10-2,-9 4,-1 0,1 0,-1 1,1 0,-1 0,0 0,0 1,0-1,1 1,-1 0,0 1,-1-1,1 1,0 0,-1 0,0-1,0 2,0-1,0 1,0 0,-1 0,5 6,9 13,-1 0,23 44,-34-56,10 15,-3 1,1 0,-3 0,0 1,-2 1,-2 0,4 37,-10-63,1 0,-1 1,0 0,1 0,0 0,0-1,0 1,0-1,1 0,-1 1,1-1,0 1,0-1,0 0,2 0,-2 0,1-1,0 1,-1-1,1 1,0-1,1 0,0 1,-1-1,1-1,-1 1,1-1,-1 1,1-1,1 0,-2 0,1 0,7-1,24 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31">17817 2543,'-6'0,"-4"4,-8 2,-8 8,-9 6,-14 9,-13 8,-8 6,-12 8,3-3,0 3,11-8,10-6,7-6,12 0,8 1,4-2,7-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32">18286 1700,'-2'1,"1"-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 1,1-1,-1 0,0 2,-15 35,11-26,-112 295,98-254,0 2,4 0,3 0,1 2,4-1,1 72,5-57,5 298,-4-365,0-1,0 0,1 0,-1 0,1 1,-1-1,1 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1 0,7 5,9 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33">18783 2338,'-3'0,"2"-1,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,1 1,-1-2,1 1,-1 0,1-1,0 1,0-1,-1 1,1 0,0-3,-4-39,4 37,2-1,-1 0,0 2,1-2,-1 1,1-1,1 1,-1 1,1-1,1 0,-1 0,2 0,-1 2,7-10,-9 12,0 0,1 0,-1 1,1-1,-1 1,0 1,0-2,1 1,-1 0,1 0,-1 1,2-1,-2 0,1 1,0 0,3-1,-2 2,0-1,0 1,-1 0,0 0,0 0,1 1,-1-1,0 0,1 0,-1 1,-1 0,1 0,0 1,-1-1,5 5,6 6,-3 0,2 1,-3 0,1 0,-2 2,0-1,8 22,31 120,-3-6,-41-144,3 10,0-1,3 0,16 28,-23-41,1 0,-1 1,1-1,-1 0,1-1,1 1,-1-1,1 1,-1-1,0 1,1-1,-1 0,2-1,-1 1,0-1,-1 1,1-1,0 0,1 0,-1-1,0 1,10-1,0-3,1 0,-1-1,1 0,0-2,-2 1,1-1,-1 0,1-2,21-15,16-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34">19307 2006,'-9'0,"-28"0,-20 9,-11 11,-2 12,-13 21,-8 19,5 6,-9 12,4-1,6-2,15-8,18-9,19-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35">19307 2696,'10'0,"0"-1,-1-1,2 0,-2 0,1-1,-1 0,0 0,1-1,-1 0,16-11,8-6,42-36,-25 19,-12 15,-37 22,0 1,0 0,1-1,-1 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,-1-1,1 1,0-1,-1 1,1 0,-1-1,2 1,-2 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 2,1 13,0 2,-1-2,-1 1,0 0,-1 0,-7 29,-34 103,31-116,1-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36">19748 1852,'6'1,"-1"0,1 0,-1 0,1 1,-1 0,0 0,0 0,0 0,1 1,-1 0,-1 0,0 0,1 0,0 0,3 6,5 3,-1 1,-1 0,12 18,-9-6,-3-1,0 1,-2 0,0 1,-3 0,7 50,-3-26,10 44,-6 1,-2-1,-7 187,-8-262,0 1,-3-1,1-1,-1 2,-1-2,-2 0,0 0,-15 22,1-7,-1-1,-2-1,-37 34,43-46,-2-2,0 0,-1-1,-1-2,0 0,-1-1,-45 16,32-17</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7512,11 +7640,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1536 0,'-21'24,"2"1,0 0,2 2,1 0,1 0,-12 34,-1 21,3 0,-14 91,34-150,-9 55,-7 151,20 81,2-281,0-19,0-1,0 0,1 0,1-1,-1 1,2 0,-1-1,1 0,0 0,1 0,0 0,10 12,-4-6,1-1,1-1,0 0,0-1,24 16,-9-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">1695 556,'0'0,"0"-1,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,2 0,37 11,-37-12,14 8,0 0,0 1,-1 1,-1 0,1 1,-2 0,0 1,21 24,1 7,44 70,-71-101,9 13,-1 0,-1 1,-1 0,-1 1,-2 0,9 31,-19-50,1-1,1 1,-1-1,1 0,1 0,-1 0,7 9,-9-14,1 0,-1-1,1 1,-1 0,1 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,1 0,-1-1,0 0,1 1,-1-1,1 0,-1 0,0 0,1-1,4 0,20-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">2356 423,'-18'5,"-15"15,-11 12,-11 11,-6 6,-5 5,3-3,4 3,7-7,9-7,6-2,10 2,9-1,8 1,1-5,3-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">2647 979,'-5'0,"4"0,6 0,2 9,9 8,2 5,-2 3,-5 2,-3 2,-3-1,-3 0,-1 0,-1-1,-1 0,0 4,1 1,-1 5,1-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">2938 106,'10'1,"0"-1,0 1,0 1,0-1,0 2,-1-1,1 2,-1-1,1 1,-1 0,0 1,-1 0,1 1,-1 0,0 0,0 1,-1 0,0 0,0 0,-1 1,0 0,0 1,-1-1,6 12,7 19,-2 1,-2 1,-1 0,10 60,-8-33,-2-7,-2 0,-3 1,-3 0,-3 0,-8 96,3-141,0-1,-1 0,-1-1,0 1,-1-1,-1 0,-13 22,-67 92,71-108,-1 4,-1 0,-1-2,-1 0,-1-2,-41 34,37-39</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1547 0,'-22'23,"3"1,-1 0,2 2,1 0,2 0,-13 32,-2 21,4-1,-14 88,35-144,-10 53,-7 144,21 79,2-271,0-17,0-1,0-1,1 1,1-1,-1 0,3 1,-2-2,1 1,0 0,1-1,1 1,9 11,-3-5,0-2,2 0,-1-1,1 0,24 15,-9-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">1713 533,'0'0,"0"-1,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,-1-1,1 1,0 0,1 0,-1 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,-1 1,2 0,39 11,-39-12,14 8,1-1,0 2,-2 0,0 1,1 1,-3-1,1 2,21 22,2 7,45 68,-74-98,10 13,-1 0,-2 1,0 0,-2 1,-1 0,9 29,-20-47,1-1,1 0,-1 0,1 0,1-1,0 1,6 9,-9-15,1 1,-1-1,1 1,-1 0,1 0,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,1 0,0-1,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,5-1,20-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">2402 405,'-19'5,"-15"14,-12 12,-12 10,-5 6,-6 5,3-3,5 3,7-7,9-7,6-1,11 1,10-1,7 2,2-6,2-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">2705 938,'-5'0,"4"0,6 0,2 9,10 7,2 5,-3 3,-4 2,-4 2,-3-1,-3 0,-1 0,-1-1,-1-1,0 5,1 1,-1 4,1-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">3008 102,'11'1,"-1"-1,0 1,1 0,-1 0,1 2,-2-1,2 2,-2-1,1 1,0 0,-1 0,-1 1,2 1,-2 0,1-1,-1 2,-1 0,0 0,1-1,-2 2,0 0,0 0,0 0,5 11,8 18,-2 2,-3 0,0 0,10 58,-9-32,-1-6,-3-1,-2 2,-4-1,-3 1,-8 91,3-135,-1 0,0-1,-1-1,0 2,-1-2,-2 1,-13 20,-69 89,73-104,-1 4,0 0,-2-2,-1 0,-1-2,-42 33,37-38</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7597,14 +7725,14 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">79 1005,'0'2,"0"-1,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,0 1,1-1,1 0,40 5,-38-5,3 0,0 0,0 1,0-1,0 1,0 1,0 0,-1 0,11 3,-16-3,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,-1 0,0 6,1 1,-1-1,1 0,-2 0,1 0,-2 0,1 0,-1 0,0 0,-1 0,0 0,0-1,-1 1,0-1,-1 0,1 0,-2-1,1 1,-1-1,0-1,-1 1,1-1,-1 0,0 0,-1-1,-8 6,-24 11,-30 19,65-38,1 0,-1 1,1 0,-1 0,1 0,1 1,-1-1,0 1,1 0,-4 8,6-11,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0 0,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,-1 0,4 1,7 3,0-1,0 0,0 0,19 2,-14-3,8 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">397 793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">2963 0,'-13'32,"2"1,1-1,1 2,3-1,0 1,-1 50,-3 7,-16 68,-7 70,29-187,2-1,2 1,8 61,-6-89,2 0,-1 0,2-1,-1 1,2-1,0 0,1-1,13 20,2-2,2-1,27 25,-28-30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">3254 820,'0'-18,"-1"-10,7-50,-5 71,0 0,1 0,0-1,0 1,0 0,1 0,0 1,1-1,0 1,0 0,8-11,-9 14,0 0,1 1,-1-1,0 1,1 0,0 0,-1 0,1 0,0 1,0-1,0 1,0 0,0 0,0 1,0-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 1,0 0,0 0,0 1,0-1,0 1,4 2,7 4,0 1,0 0,-1 1,-1 0,18 18,1 4,-2 2,-1 0,31 51,57 120,-44-39,-51-113,-11-33,-1-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3837 476,'-5'14,"-5"13,-11 11,-6 12,-12 12,-4 9,-12 5,3 4,5-8,7-16,10-12,11-11,7-5,7-3,3-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">4207 1111,'4'0,"2"5,0 5,-2 11,-1 6,-1 3,-1 0,0 1,-1-2,0 0,-1-1,1-1,0-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">4154 846,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">4419 211,'10'1,"0"-1,0 1,0 1,0 0,0 0,0 1,0 0,-1 1,1 0,-1 1,16 10,-12-6,-1 1,1 1,-2 0,0 1,0 0,16 26,-7-5,-1 2,-2 0,-2 1,-1 1,13 52,-4-3,-3 1,-4 1,8 166,-23-208,-8 54,4-83,0 0,-2 0,1 0,-2-1,0 1,-12 20,2-12,0-2,-2 0,-1-1,0 0,-26 21,-33 36,59-58,2-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">82 968,'0'2,"0"-1,1 0,0 0,-1-1,1 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,1 0,-1 1,1-1,1 0,41 5,-39-5,4 0,-1 0,0 1,1-1,-1 1,0 1,0 0,0-1,10 4,-16-3,1 0,-1 0,1 0,0 0,-1 0,0 0,0 0,0 1,-1-2,1 2,-1-1,1 1,-1 0,0 0,0 0,0-1,0 1,0 0,-1-1,1 1,-1 0,0 6,1 1,-1-2,1 1,-2 0,1-1,-2 1,1 0,-1-1,0 1,-1 0,0-1,0 0,-1 1,0-2,-2 1,2 0,-2-2,1 2,-1-1,-1-1,0 0,1 0,-1 0,0 0,-2-1,-7 5,-26 11,-30 19,67-37,1 0,-2 0,2 1,-1 0,1 0,1 1,-1-1,0 0,0 1,-3 8,6-11,0 0,1 0,-1-2,1 2,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 0,-1 1,1 0,0 0,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,2 0,-2 1,1-1,-1 0,1 0,0 0,-1 0,4 0,7 4,1-1,-1 0,1 0,19 2,-15-4,9 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">411 764</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">3066 0,'-13'31,"1"1,2-2,1 3,3-1,-1 1,0 48,-3 6,-17 66,-7 68,30-181,2 0,2 0,8 59,-6-85,2-1,-1 1,2-2,-1 2,3-2,-1 1,1-2,14 20,2-2,1-1,29 24,-29-29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">3367 790,'0'-18,"-1"-9,8-48,-6 68,0 1,1-1,0-1,0 2,0-1,1 0,0 1,1 0,0 0,1 0,7-10,-9 13,0 0,1 1,-1-1,1 1,0 0,0 0,-1 0,1 0,0 1,0-1,1 2,-1-1,0 0,0 1,0-1,0 1,1 0,0 0,-1 0,0 1,0-1,0 1,0 0,0-1,1 2,-1-1,0 1,4 2,8 4,-1 1,1-1,-2 2,0-1,18 18,1 4,-2 2,-1 0,32 49,59 115,-45-37,-54-109,-10-32,-2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3971 458,'-5'14,"-6"12,-10 10,-7 13,-13 10,-3 10,-13 4,3 4,5-8,8-15,10-12,11-10,8-5,7-3,3-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">4354 1070,'4'0,"2"5,0 4,-2 11,-1 6,0 3,-2 0,0 1,-1-2,0 0,-1-1,1-1,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">4299 815,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">4573 203,'10'1,"1"-1,-1 1,0 1,1 0,-1 0,1 1,-1 0,-1 1,2-1,-2 2,17 10,-13-7,0 2,0 1,-2-1,1 2,-1-1,17 26,-7-5,-2 1,-1 1,-2 1,-2 0,14 51,-4-3,-3 1,-5 0,9 161,-24-201,-8 52,4-79,0-1,-3 1,2-1,-2-1,0 2,-13 18,3-11,-1-1,-2-1,0-1,-1 0,-26 20,-35 36,61-57,3-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7631,7 +7759,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">35 175,'0'639,"0"-633,0-1,0 1,1 0,0-1,1 1,-1-1,1 1,0-1,0 0,0 0,1 0,0 0,0 0,0-1,1 1,-1-1,1 0,0 0,1 0,-1 0,0-1,1 0,0 0,0 0,0 0,0-1,0 0,1 0,-1 0,1-1,-1 0,1 0,-1 0,1-1,0 1,-1-1,1-1,0 1,8-3,-8 2,1-2,-1 1,1-1,-1 1,0-2,0 1,0-1,0 0,-1 0,1-1,8-9,5-7,26-39,-13 17,189-252,-193 256,-8 12,-1-1,-1-1,-1-1,16-40,-20 32,-1 0,-2 0,7-60,-16 94,0 1,0-1,0 1,0 0,1-1,-1 1,1 0,2-5,-3 8,-1 0,0 0,0-1,0 1,0 0,1 0,-1-1,0 1,0 0,1 0,-1-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 0,1 0,8 25,1 78,-4 170,-6-165,2-12,-4 0,-5-1,-33 170,-119 286,143-503,-3-1,-1-1,-3-1,-1-1,-52 70,72-108,-1 0,0 0,0-1,0 0,0 0,-1 0,0-1,0 1,0-1,-1-1,1 1,-1-1,0 0,0-1,0 0,0 0,-1 0,1-1,0 0,-1 0,1-1,-1 0,1 0,0-1,-1 0,1-1,0 1,0-1,-1 0,1-1,1 0,-1 0,-11-7,1-3,0 0,1-1,1-1,0 0,1-1,0-1,2 0,0-1,1 0,0-1,2 0,0-1,1 0,1 0,1-1,1 0,1 0,1 0,0 0,2-42,2 36</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">35 168,'0'612,"0"-606,0-1,0 1,1-1,0 0,1 1,-1-1,1 1,0-2,0 1,0 0,1 0,0-1,0 1,0-1,1 1,-1-1,1 0,0-1,1 1,-1 0,0-1,1 0,0 0,0 0,0-1,0 0,0 0,1 0,-1 0,1-1,-1 0,1 0,-1 0,1-1,0 1,-1-1,1-1,0 1,8-3,-8 2,1-2,-1 1,1-1,-1 2,0-3,0 1,0-1,0 0,-1 0,1 0,8-10,5-6,26-38,-13 17,189-242,-193 246,-8 11,-1-1,-1-1,-1 0,16-39,-20 30,-1 1,-2-1,7-57,-16 91,0 0,0-1,0 1,0 0,1-1,-1 1,1 1,2-6,-3 8,-1 0,0 0,0-1,0 1,0 0,1 0,-1-1,0 1,0 0,1 0,-1-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 0,1 0,8 24,1 75,-4 162,-6-157,2-12,-4 0,-5-1,-33 163,-119 274,143-482,-3-1,-1 0,-3-2,-1-1,-52 67,72-103,-1 0,0-1,0 0,0 0,0 0,-1 0,0-2,0 2,0-1,-1-1,1 1,-1-1,0-1,0 0,0 0,0 0,-1 0,1-1,0 0,-1 0,1-1,-1 0,1 0,0-1,-1 0,1-1,0 1,0-1,-1 0,1 0,1-1,-1 0,-11-7,1-2,0-1,1 0,1-2,0 1,1-1,0-2,2 1,0-1,1 0,0-2,2 1,0-1,1 0,1 0,1-1,1-1,1 1,1 0,0 0,2-40,2 34</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7658,31 +7786,31 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">4949 0,'-6'1,"0"0,0 0,0 0,0 1,0 0,1 0,-1 0,1 1,-1 0,1 0,0 0,0 1,1-1,-1 1,1 0,-1 1,1-1,1 1,-1 0,1 0,-4 7,-7 11,2 1,0 1,-11 38,-73 269,79-267,2 5,4 1,3 0,2 1,4-1,3 1,12 80,7-21,-16-114,0-1,1 0,1-1,1 1,16 27,-21-39,1-1,0 1,0 0,0-1,1 0,-1 0,1 0,0 0,4 2,11 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="781">5002 688,'0'-27,"1"1,2-1,12-52,-12 67,1 0,0 0,1 0,0 1,1-1,0 2,1-1,0 0,0 1,16-15,-21 23,1-1,0 1,0 0,0-1,0 1,0 1,1-1,-1 0,0 1,1 0,0 0,-1 0,1 0,-1 1,1-1,0 1,7 0,-5 1,-1 0,1 1,0-1,0 1,-1 0,1 1,-1-1,0 1,0 0,6 5,8 8,0 1,-2 1,0 1,17 24,-28-35,47 62,-4 3,-3 2,-3 2,53 131,-84-176,-1 0,1-1,2 0,1-1,1-1,26 35,-38-60,0-1,-1 1,1-1,1 0,-1 0,0 0,1-1,0 1,-1-1,1 0,0-1,0 1,0-1,0 0,0 0,9 0,20 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1376">6113 397,'-9'1,"0"0,1 1,-1 0,1 0,-1 0,1 1,0 1,0-1,-11 8,-67 48,78-52,-48 39,2 3,2 3,3 2,-49 67,-76 79,140-164</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2230">6140 1085,'8'0,"-1"-1,1 0,0-1,0 0,0 0,-1-1,0 0,9-4,-10 3,1 1,0 1,0-1,0 1,1 0,-1 0,12 0,-17 2,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,1 0,-1-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,-1 0,1 1,1 1,-1 1,0-1,0 1,0-1,-1 1,1 0,-1 0,0-1,0 1,-1 7,-3 7,0 1,-12 34,15-51,-31 74,19-48,-18 58,29-77,0 0,0 1,1-1,0 0,1 0,0 1,0-1,1 0,0 0,5 18,0-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2836">6404 926,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112894.77">6695 1350,'0'1,"1"-1,0 0,0 1,0-1,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,-1 0,1-1,0 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,1-1,-1 1,0 0,0 0,0 0,1 0,-1 0,0 0,0 1,1 29,-3-18,1 1,-2-1,0 0,-1 0,0 0,-1 0,0 0,-1-1,0 0,-1 0,0-1,-1 0,-1 0,1-1,-19 17,-11 5,-1-1,-83 49,83-56,4 0,5-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="114884.51">7119 344,'4'-5,"6"12,7 15,-9 3,-1 1,-2 0,0 1,1 41,3 15,27 100,-28-154,1 0,1-1,2-1,18 32,-27-54,0-1,0 1,0-1,1 0,-1 0,1 0,0-1,0 0,1 1,-1-2,1 1,-1 0,1-1,0 0,0 0,0 0,0-1,1 1,-1-1,0 0,0-1,1 0,-1 1,0-2,1 1,-1-1,0 1,1-1,-1-1,0 1,0-1,0 0,0 0,0 0,-1-1,1 0,-1 0,1 0,-1 0,0-1,0 0,-1 1,6-8,8-10,0 0,-2 0,0-1,-2-1,0-1,-2 0,-1 0,0-1,-2 0,-1-1,-1 0,-1 0,-1 0,0-42,-10-118,-8 317,5-59,-94 519,41-263,61-316,-1 1,0-1,-1 0,0 0,-1-1,-6 14,8-21,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,-1 0,1-1,-1 1,1-1,-1 1,0-1,0 0,0-1,0 1,0-1,-1 0,1 0,-8 1,-2 0,-1-1,1 0,-1-1,0-1,1-1,-1 0,1 0,0-2,0 0,0 0,0-1,1-1,-1 0,1-1,1-1,0 0,0 0,0-1,1-1,0 0,1 0,0-1,1 0,-10-17,8 10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="115435">7701 1482,'4'0,"2"5,0 10,-2 11,-1 7,-1 1,-1 0,0-1,-1-3,0-1,-1-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="116321">8018 185,'3'1,"0"-1,1 1,-1-1,0 1,1 0,-1 0,0 1,0-1,0 1,0-1,0 1,0 0,-1 0,1 0,-1 1,1-1,-1 0,0 1,0 0,0-1,0 1,0 0,2 5,4 10,-1 0,0 0,5 22,-9-28,35 138,37 299,-49 170,-26-564,0 23,-13 102,10-158,-2 0,0 0,-1-1,0 1,-2-1,-1-1,-1 1,0-1,-17 22,-13-2,21-26</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="117989.83">1 2276,'2'1,"1"-1,-1 0,1 1,-1 0,1-1,-1 1,1 0,-1 0,0 0,1 1,-1-1,0 1,0-1,0 1,0 0,0-1,-1 1,1 0,0 0,-1 0,1 1,-1-1,0 0,1 3,4 9,0 0,-1 0,3 17,1 0,29 66,5-2,67 109,-22-41,-53-93,-18-33,1-1,1-1,2-1,37 45,-57-77,1 0,-1-1,1 1,-1-1,1 0,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,0-1,0 1,0 0,0-1,0 0,0 1,0-1,1 0,-1 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,1-2,7-4,-1-1,-1-1,0 1,0-1,7-12,-14 20,22-32,-2 0,-2-1,22-50,36-119,-25 61,161-331,-206 460,-2-1,1 0,-2 0,6-28,-7 18</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120876.52">1271 2884,'0'5,"0"6,0 5,0 4,0 9,0 3,0 5,0 2,0-3,0-2,0 2,0 4,0 0,0-3,0-3,0-3,0-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120877.52">1800 2381,'4'0,"11"0,17 0,11 0,3 0,2 0,3 0,-3 0,-1 0,-4 0,0 0,-3 0,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120878.52">1827 2911,'4'0,"11"0,12 0,5 0,29 0,14 0,11 0,5 0,-4 0,-12 0,-20 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120879.52">3441 2117,'5'1,"0"0,1 0,-1 1,0-1,1 1,-1 0,0 0,0 1,-1 0,1 0,0 0,-1 0,0 1,0-1,0 1,0 0,-1 0,1 1,-1-1,0 1,0 0,3 7,6 12,-2 0,0 1,8 31,23 140,-31-136,35 115,-45-172,1 0,0 0,0-1,1 1,-1 0,0 0,1-1,0 1,-1-1,1 0,0 1,0-1,4 3,-6-5,1 0,-1 0,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0 0,-1-1,1 1,-1 0,1-1,17-20,3-20,-2 0,21-66,-6 15,15-38,-23 56,38-74,-62 145,0 0,-1 0,1 0,0 1,0-1,1 0,-1 1,1-1,3-2,11-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121428.05">4605 1879,'-2'47,"-1"0,-2 0,-2-1,-20 66,0-28,-53 113,-19 36,81-183,3 1,-16 89,17-50,4 0,2 137,8-218,1 0,0 1,0-1,1 0,4 11,-5-18,0 1,0-1,0 0,0 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,1 0,-1 0,4 0,13 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122368.58">5055 2408,'-1'1,"1"-1,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,0 0,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0 0,0-1,0 0,5-15,21-12,-15 22,0 2,1-1,-1 2,1 0,0 0,0 1,0 0,1 1,-1 1,21 1,-16 0,0 1,0 0,0 2,-1 0,0 0,1 2,18 9,-28-11,-1 0,0 1,1 0,-2 1,1-1,-1 1,1 0,-2 1,1-1,-1 1,0 0,0 0,5 14,2 10,15 65,-19-63,10 41,-10-40,1 1,1-1,2-1,1 0,24 45,-34-75,0 0,-1 0,1 0,0 0,0 0,1 0,-1-1,1 1,-1-1,1 0,0 1,0-1,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,1 0,-1 0,0-1,1 1,0-1,-1 0,1 0,-1 0,1 0,3-1,0-2,0 1,0-1,0 0,-1 0,1-1,-1 0,0 0,0-1,0 0,-1 0,0 0,9-12,16-23</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123038.28">5663 2143,'0'5,"-5"10,-5 16,-11 12,-10 12,0 6,-4 1,0-5,1-3,-3 7,1-3,2-1,-3 2,6-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="124055.99">6166 2911,'-5'5,"-1"10,1 7,-9 9,-1 3,-3 6,-3 4,2 0,0-4,4-3,-2-9,4-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="125148.68">6034 2699</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="127216.75">5954 2699,'4'0,"7"0,5 0,0 5,3 5,-4-3,-3-7,-3-8,-9-3,-8 0,-8 3,-5 6,1 9,3 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="128095.49">6907 3281,'-5'0,"-10"0,-12 9,-5 8,-2 9,-14 19,2 6,0-1,7-5,11-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="129257.54">7277 2328,'-14'382,"2"-144,12-230,-1 0,2 0,-1 0,1 0,0 0,1-1,4 15,-5-20,0 0,0 0,0 0,0-1,0 1,1-1,-1 1,1-1,-1 1,1-1,-1 0,1 1,0-1,-1 0,1 0,0-1,0 1,0 0,0 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 0,1 0,3-2,0 0,0 0,0 0,0 0,-1-1,0 0,0 0,0-1,0 1,-1-1,1 0,5-10,5-8,20-43,-23 41,5-16,-14 32,1 0,0 0,0 0,0 1,1 0,1-1,7-7,-13 15,0 1,0 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,1 1,-1-1,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 1,0-1,1 0,-1 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,5 22,-6 20,-1-1,-1 1,-17 70,10-57,-33 140,37-177,-1 1,0-1,-1 0,-1-1,-1 1,-1-2,-20 27,26-39,-1 0,1 0,-1 0,1-1,-2 0,1 0,0 0,-1-1,1 0,-1 0,0-1,-10 3,3-2,0-1,0-1,0 0,-1-1,-18-2,4-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="130344.49">7912 3493,'0'-15,"4"-78,-3 86,0 0,0 0,1 1,0-1,0 1,1-1,-1 1,1 0,1 0,-1 0,5-5,-8 11,0 0,1 0,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,3 15,-3 20,-8-8,0 0,-1-1,-2 0,-1-1,-1 0,-21 31,-27 54,60-109,0 1,0 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,0 0,1 2,-1-3,-1-1,1 0,-1 1,1-1,0 0,-1 1,1-1,0 0,0 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0-1,0 1,-1 0,2-1,25-18,26-47,-27 31</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="130747.49">8150 2990,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="131713.5">8336 2381,'2'-2,"1"0,-1 0,1 1,0-1,0 0,0 1,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-1 0,0 0,0-1,1 2,-1-1,0 0,0 1,1-1,-1 1,0 0,0 0,0 1,0-1,0 0,4 4,2 0,-1 0,1 1,-1 0,-1 0,1 1,-1 0,0 1,6 8,0 5,-1 1,0 0,-2 1,0 1,-2-1,-1 1,0 1,-2-1,2 32,1 34,-6 108,-2-183,0 95,-10 173,7-264,-1 0,-1 0,-1-1,0 0,-2 0,0 0,-1-1,0 0,-19 23,-10 28,28-48,-1-1,0 0,-20 24,-36 33,53-60</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5145 0,'-7'1,"1"0,0 0,0 0,-1 1,1 0,1 0,-1-1,0 2,0 0,1 0,0 0,0 1,0-1,0 0,1 1,-1 1,1-1,1 1,-2-1,2 1,-4 7,-7 10,1 1,1 1,-12 36,-76 257,82-255,3 5,3 1,4 0,2 1,4-1,3 1,12 76,8-20,-17-108,0-2,1 0,2 0,0 0,17 26,-22-37,1-1,0 1,0-1,0 0,2 0,-2 0,1 0,0 0,4 2,12 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="781">5200 658,'0'-26,"1"1,2-1,12-49,-12 63,2 1,-1-1,1 1,0 0,1 0,1 1,0 0,0-1,0 2,17-15,-22 22,2-1,-1 1,0 0,0-1,0 2,0 0,1-1,-1 0,1 1,0 0,0 0,-1 0,1 0,-1 1,1-1,1 1,6 0,-5 1,-1 0,2 1,-1-1,0 1,-1 0,2 0,-2 0,0 1,0 0,7 5,7 7,1 1,-2 2,-1 0,19 23,-30-34,49 60,-4 3,-3 2,-3 2,54 125,-86-169,-2 1,2-2,1 1,2-1,1-2,26 35,-39-59,1 0,-2 1,1-1,1 0,-1 0,0 0,2-1,-1 0,-1 0,1 0,0-1,0 1,1-1,-1 0,0 0,10 0,20 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1376">6354 380,'-9'1,"0"0,0 0,0 1,1 0,-2 0,2 1,0 1,-1-1,-10 7,-71 47,82-51,-50 38,2 3,2 3,3 2,-51 63,-79 77,146-158</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2230">6383 1038,'8'0,"-1"-1,1 0,1-1,-1 0,0 0,0-1,-1 0,10-4,-11 4,1 0,0 1,1-1,-1 1,1 0,0 0,11 0,-17 2,-1 0,0 0,2 0,-2 0,0 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,1 0,-1-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,-1 0,1 1,2 1,-2 0,0 0,0 1,0-1,-1 1,1 0,-1-1,0 0,0 1,-1 7,-3 6,-1 1,-11 33,15-49,-33 70,21-45,-19 55,30-73,0 0,-1 0,2 0,0-1,1 1,0 0,0 0,1 0,0-1,6 18,-1-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2836">6657 886,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112894.77">6959 1291,'0'1,"2"-1,-1 0,0 1,0-1,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,-1 0,1-1,0 1,-1 0,1-1,-1 1,0 0,1-1,-1 1,1-1,-1 1,0 0,0 0,0 0,1 0,-1 0,0 0,0 1,1 28,-3-18,1 2,-2-2,0 0,-1 1,-1-1,0 1,0-1,-1 0,0-1,-2 1,1-2,-1 1,-2-1,2 0,-20 15,-12 6,0-1,-87 46,87-53,3 0,6-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="114884.51">7400 329,'4'-5,"7"12,6 14,-8 3,-2 1,-2 0,0 0,2 40,2 15,28 95,-28-147,0-1,2 0,1-1,19 30,-28-51,0-1,1 1,-1-2,1 1,-1 0,1 0,0-1,0 0,2 1,-2-3,1 2,-1 0,1-1,1 0,-1 0,0 0,0-1,1 1,0-1,-1 0,0-1,1 0,-1 1,1-2,0 1,-1-1,0 1,1-1,0-1,-1 1,0-1,0 0,0 0,1 0,-2-1,1 0,-1 1,1-1,0 0,-1-1,0 0,-1 1,6-7,9-10,0 0,-3 0,1-2,-3 0,1 0,-3-1,0 0,-1-1,-2 0,0-1,-2 0,-1 0,-1 0,0-40,-10-113,-8 304,4-57,-97 496,43-252,63-301,-1 0,0 0,-2-1,1 1,-1-2,-6 14,8-20,0 0,-2-1,2 1,-1-2,0 2,0-1,0 0,-1 0,1-1,-1 1,0-1,0 0,0 0,0 0,0-1,0 1,-1-1,0 0,1 0,-8 1,-3 0,-1-1,2 0,-2-1,1-1,0-1,0 0,0 0,0-2,1 0,-1 1,1-2,0-1,0 0,0 0,2-2,-1 0,1 1,-1-2,2-1,-1 1,2-1,0 0,0-1,-9-15,7 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="115435">8005 1417,'4'0,"3"5,-1 9,-2 11,-1 7,-1 0,-1 1,0-2,-1-2,0-1,-1-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="116321">8335 177,'3'1,"0"-1,1 1,-1-1,0 1,2 0,-2 0,0 1,0-1,0 0,0 0,0 1,0 0,-1 0,2 0,-2 1,1-1,-1 0,0 1,0 0,0-2,0 2,0 0,2 5,5 9,-2 0,0 0,6 22,-10-28,36 133,39 285,-51 163,-27-539,0 21,-13 98,10-151,-2 0,-1 0,0-1,0 2,-2-2,-2-1,0 1,-1-1,-17 21,-13-2,21-24</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="117989.83">1 2177,'2'0,"1"0,-1 0,1 1,-1 0,2-1,-2 1,1 0,-1 0,0 0,1 1,-1-1,0 1,0-1,0 1,0 0,1-1,-2 1,1 0,0-1,-1 1,1 1,-1-1,0 0,1 3,4 8,0 1,0-1,2 17,1-1,31 64,5-2,69 104,-23-39,-54-89,-20-32,2 0,1-2,2 0,38 42,-59-73,1 0,-1-1,1 1,-1-1,1 0,0 1,-1-1,2 0,-1 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,0 1,0-1,2 0,-2 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 0,0 1,0-1,1 0,-1 0,0 0,1-2,7-4,0-1,-2 0,0 0,0 0,8-12,-15 19,23-31,-2 0,-2 0,22-48,38-115,-26 60,168-318,-215 441,-2-1,1-1,-1 1,5-27,-7 17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120876.52">1321 2758,'0'5,"0"5,0 6,0 3,0 8,0 4,0 4,0 3,0-4,0-1,0 1,0 4,0 1,0-4,0-3,0-2,0-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120877.52">1871 2277,'4'0,"12"0,17 0,12 0,3 0,2 0,3 0,-4 0,0 0,-4 0,0 0,-4 0,-7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120878.52">1899 2784,'4'0,"12"0,12 0,5 0,31 0,14 0,11 0,6 0,-5 0,-12 0,-21 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="120879.52">3577 2024,'5'1,"0"0,2 0,-2 1,0-1,1 1,-1 0,1 0,-1 1,-1 0,1 0,0-1,-1 1,1 1,-1-1,0 1,0 0,-1-1,1 2,0-1,-1 1,0 0,3 6,6 12,-1 0,-1 1,9 29,24 135,-33-131,37 111,-47-165,1-1,0 1,0-1,1 1,-1 0,0 0,1-1,0 1,-1-2,1 1,0 1,0-1,5 3,-7-5,1 0,-1 0,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0 0,-1-1,1 1,-1 0,1-1,18-19,3-19,-2 0,21-64,-6 15,16-36,-24 53,40-70,-65 138,0 0,-1 0,1 0,0 1,0-1,2 0,-2 2,1-2,3-2,12-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121428.05">4787 1797,'-2'45,"-1"0,-2 0,-3-1,-20 63,0-27,-55 109,-20 33,84-174,4 1,-17 85,17-48,5 0,1 131,9-208,1-1,0 2,0-2,1 1,5 10,-6-17,0 1,0-1,0 0,0 1,1-1,-1-1,1 1,-1 0,1 0,0 0,0 0,0-1,1 1,-1 0,0-1,0 0,1 1,-1-1,0 0,1-1,-1 1,4 0,14 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122368.58">5255 2303,'-1'1,"1"-1,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-2 0,2 0,0-1,-1 1,1 0,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0-1,-1 1,1 0,0 0,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0 0,0-1,0 0,5-14,22-12,-15 21,-1 2,2 0,-2 1,2 0,-1 0,1 1,-1 0,2 1,-2 1,22 1,-16 0,0 1,-1 0,1 2,-1 0,-1-1,2 3,18 9,-28-12,-2 1,0 1,1 0,-1 1,0-2,-1 2,1 0,-2 0,2 0,-2 1,0 0,0-1,5 14,3 10,15 62,-20-61,11 40,-11-38,2 0,0 0,2-2,2 1,24 42,-35-71,0 0,-1 0,1 0,1 0,-1 0,1-1,-1 0,1 1,-1-1,1 0,0 1,0-1,0 0,1-1,-1 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1-1,1 1,0-1,-1 0,1 0,-1 0,2 0,2-1,0-2,0 2,1-2,-1 0,-1 0,1-1,0 0,-1 0,0 0,0-1,0 0,-1 0,9-11,17-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123038.28">5887 2049,'0'5,"-5"9,-6 16,-11 11,-10 12,0 5,-5 1,1-4,1-3,-4 6,2-3,2 0,-4 1,7-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="124055.99">6410 2784,'-6'5,"0"9,1 7,-10 9,0 2,-4 6,-3 4,3 1,-1-5,4-3,-1-8,3-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="125148.68">6272 2581</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="127216.75">6189 2581,'4'0,"8"0,4 0,1 5,3 4,-5-2,-2-7,-4-8,-9-2,-8-1,-9 4,-5 5,2 9,2 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="128095.49">7180 3138,'-5'0,"-11"0,-12 8,-5 8,-3 9,-13 18,1 6,0-1,7-5,12-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="129257.54">7564 2226,'-14'366,"1"-139,13-219,-1-1,2 1,-1 0,2-1,-1 1,1-1,4 14,-5-19,0 0,0 0,0-1,0 0,0 1,1-1,-1 1,1-1,-1 1,1-1,-1 0,2 1,-1-1,-1 0,1 0,0-1,0 1,0 0,0 0,0-1,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 0,1 0,4-2,-1 0,0 0,0 0,1 0,-2 0,0-1,0 0,0-1,1 1,-2 0,1-1,5-10,6-7,20-41,-23 39,4-15,-13 31,0-1,0 0,0 1,0 0,1 1,2-2,6-6,-13 14,0 1,0 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0 0,1 1,-1-1,0 0,1 0,-1 0,0 0,2 0,-2 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 1,0-1,1 0,-1 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,5 21,-6 20,-1-2,-1 1,-18 67,10-55,-33 135,38-170,-2 1,1-1,-1 1,-2-2,0 1,-2-2,-20 26,27-37,-1 0,1 0,-2-1,2 0,-2 0,1 0,-1 0,0-1,1-1,-1 1,-1-1,-9 3,2-2,1-1,-1-1,0 0,0-1,-19-2,3-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="130344.49">8225 3340,'0'-14,"4"-75,-3 82,0 1,0-1,1 1,0 0,0 0,1-1,-1 1,1 1,2-1,-2 0,5-4,-8 10,0 0,1 0,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,3 14,-3 19,-8-7,0 0,-2-1,-1 0,-1-1,-2 0,-21 29,-29 52,63-104,0 1,0 0,0 0,0-1,1 1,-1 0,0 0,1 0,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,0-1,1 3,-1-3,-1-1,1 0,-1 1,1-1,0 0,-1 1,1-1,0 0,0 0,-1 1,2-1,-1 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0-1,0 1,-1 0,2-1,26-17,27-45,-28 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="130747.49">8472 2859,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="131713.5">8665 2277,'2'-2,"2"0,-2 0,1 1,0-1,0 0,0 1,0 1,0-1,0 0,1 0,-1 0,0 0,1 1,-1 0,0 0,0-1,1 2,0-1,-1 0,0 1,1-1,-1 1,0 0,0 0,0 0,1 0,-1 0,4 4,2 0,0 0,0 0,-1 1,0 0,0 1,-1-1,0 2,7 7,-1 5,0 1,-1 0,-1 1,-1 1,-1-1,-2 1,0 1,-2-1,3 31,0 32,-6 103,-2-175,0 92,-10 164,6-252,0 1,-1-1,-1-1,0 0,-3 0,1 1,-1-2,-1 0,-19 22,-10 27,28-45,0-2,-1 0,-20 23,-37 32,54-58</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7793,7 +7921,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 186,'0'-3,"1"0,0 0,0-1,0 1,0 0,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,4-3,35-33,-36 35,7-7,1 0,0 1,0 1,1 1,0-1,1 2,0 0,0 1,0 1,1 0,26-5,-39 10,0 0,0 0,0 1,0-1,0 0,0 1,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,-1 0,1-1,-1 1,0 1,1-1,-1 0,0 0,0 1,-1-1,1 1,0 0,-1-1,0 1,1 0,-1 0,0 0,0 0,-1 0,1 4,3 12,-1 1,-1-1,-1 1,-1 20,0-26,-18 255,5-120,12-142,1-1,0 1,0-1,0 1,1-1,0 1,1-1,-1 1,1-1,0 0,1 0,-1 0,1 0,5 6,-6-9,1 0,-1-1,1 0,0 1,0-1,0 0,0 0,0-1,0 1,1-1,-1 1,0-1,1 0,-1-1,1 1,0 0,-1-1,1 0,-1 0,1 0,0 0,-1-1,1 1,-1-1,1 0,-1 0,7-3,15-5,-1-2,0 0,0-2,-1-1,35-27,-8 1,53-57,-90 83,-1-1,-1 0,-1-1,0 0,-1-1,0 0,-2-1,0 1,-1-1,-1-1,4-23,0-12,-3 0,-1-88,-9 123,-4 34,-6 36,-65 366,54-324,17-70,1 0,1 1,2-1,-4 48,8-61,0 0,0 1,1-1,1 0,0 1,0-1,1 0,0 0,1-1,0 1,0-1,1 1,0-1,1-1,0 1,0-1,1 0,0-1,1 1,-1-1,12 7,5 5,-5-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 178,'0'-3,"1"0,0 0,0 0,0 0,0 0,1 0,0 0,-1 0,1 0,0 2,0-2,1 0,3-3,39-31,-39 33,7-7,1 1,0 0,0 2,2 0,-1-1,1 3,1-1,-1 1,1 1,0 1,29-6,-43 10,1 0,-1 0,0 1,0-1,1 0,-1 1,0 0,1 0,-1 0,0 0,0 0,0 1,0-1,0 0,-1 1,2-1,-2 1,0 1,1-1,0 0,-1 0,0 1,-1-1,1 1,0-1,-1 0,1 1,0 0,-1 0,0 0,0 0,-1 0,1 3,4 12,-2 2,-1-2,-1 1,-1 19,0-24,-20 243,6-114,13-136,1-2,0 2,0-1,0 1,1-2,0 2,1-1,0 0,0 0,0 0,1 0,-1-1,2 1,4 6,-5-9,0-1,-1 0,1 0,1 1,-1-1,0 0,0 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0-1,0 1,0-1,0 0,0 0,-1 0,2 0,-1 0,-1 0,2 0,-2-1,1 0,0 0,7-3,16-5,-1-1,1-1,-1-1,-1-2,38-25,-8 1,58-55,-99 79,-1 0,-1 0,-1-2,0 1,-1-1,0-1,-3 0,1 1,-1-1,-2-1,5-23,0-10,-4-1,0-84,-10 118,-5 32,-7 35,-70 350,59-310,18-67,1 0,2 1,1-1,-3 46,8-58,0-1,0 2,1-1,1-1,0 2,0-2,1 1,1-1,0 0,1 1,-1-2,1 2,1-2,0 0,1 1,0-2,0 1,1-1,1 0,-2 0,14 7,5 4,-5-3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7820,7 +7948,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'1'1,"0"-1,0 0,0 1,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,2 1,11 29,-9-20,26 63,37 148,-10-26,-24-76,-22-73,18 47,-27-90,-1 0,1 0,0 0,-1 0,2 0,-1 0,0-1,1 1,0-1,0 1,0-1,0 0,0-1,1 1,-1 0,1-1,-1 0,1 0,0 0,0 0,0-1,0 1,1-1,4 1,-2-2,-1 0,1-1,0 1,0-1,-1-1,1 1,-1-1,1-1,-1 1,0-1,0 0,0 0,0-1,0 1,7-7,12-12,-1 0,-1-1,30-38,53-87,-66 91,33-45,65-96,-114 158</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'1'1,"0"-1,0 0,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,-1 0,2 0,-2 0,2 1,12 28,-10-20,29 61,40 140,-11-24,-26-73,-24-69,19 44,-29-85,0 0,0 0,0 0,-1 0,2-1,-1 1,1-1,0 1,0-1,0 0,1 0,-1 0,0-1,2 1,-2 0,1-1,-1 0,2 0,-1-1,1 1,-1-1,0 1,2-1,3 1,-1-2,-1 0,0-1,1 1,-1-1,0-1,1 1,-2-1,2 0,-2 0,1-1,-1 0,1 0,-1-1,1 1,7-6,13-12,-1 0,-1-1,33-36,58-83,-73 87,37-44,70-90,-124 150</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7846,25 +7974,25 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1116 476,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1011">931 476,'-2'15,"1"-1,-2 0,0 0,0 0,-1 0,-1-1,0 0,-1 0,-1 0,0 0,0-1,-1-1,-1 1,0-1,0 0,-1-1,-14 11,-20 16,-2-3,-93 54,135-86,-74 41,36-20,-70 48,100-61,1-1,-1 2,2-1,0 2,0-1,1 1,0 1,1-1,-12 27,10-16,1 1,1 1,-8 41,14-59,1-1,0 1,1 0,-1 0,1 0,1 0,-1-1,1 1,1 0,-1 0,1-1,0 1,0-1,1 1,0-1,0 0,0 0,7 8,7 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13160.62">852 0,'1'31,"-1"-1,-1 0,-2 0,0 0,-2 0,-2-1,-18 52,21-72,-16 37,-24 82,30-74,2 0,2 1,3 1,2-1,3 80,3-127,0-1,1 0,-1-1,2 1,-1 0,1 0,0-1,0 0,0 1,1-1,0 0,0-1,1 1,0-1,6 6,-6-7,-1 0,1-1,0 1,0-1,0 0,0-1,0 1,0-1,1 0,0 0,-1-1,1 1,0-1,-1-1,1 1,0-1,0 0,11-2,-13 1,0 0,0 0,0-1,-1 0,1 0,-1 0,1 0,-1 0,0-1,0 1,0-1,0 0,0 0,0 0,-1-1,0 1,1 0,-1-1,2-7,4-8,-1 0,9-37,-7 20,0 8,1-4,-1 0,-2 0,5-44,-7 45,2 0,0 0,2 1,2 0,27-56,-14 33,-2 7,13-29,-33 69,1-1,-1 0,0 0,-1 0,0 0,0 0,0 0,-1-9,-23 52,-22 54,-37 106,73-175,0 1,2 0,0 1,1 0,2 0,0 0,0 34,3 34,-1-46,2 0,2-1,13 76,-14-113,1-1,-1 1,1-1,1 1,-1-1,1 0,0 0,0 0,1 0,0 0,0-1,0 0,1 0,-1 0,1 0,0-1,1 0,-1 0,1 0,0-1,0 0,0 0,0 0,12 3,7-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16322.19">4053 1137,'0'5,"0"15,-5 26,-10 19,-7 8,-4 4,-8-1,4-10,1-6,-3-10,4-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13814.63">2148 0,'-20'13,"1"0,1 2,1 0,0 1,-28 33,29-28,0 1,1 1,2 0,0 1,1 0,2 1,-14 48,-31 192,54-258,-36 298,34-250,2 0,3 0,13 86,-9-112,1-1,14 35,-18-55,0 1,1 0,0-1,1 0,0 0,0 0,1-1,0 0,0 0,0 0,8 5,13 0,0-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14532.15">2333 582,'0'-11,"2"0,0 0,0 1,1-1,0 0,1 1,0 0,1 0,0 0,0 0,1 1,1 0,-1 0,1 0,1 1,0 0,0 1,0 0,1 0,0 1,0 0,1 0,0 1,0 0,0 1,0 0,1 1,0 0,-1 0,21-1,-24 5,1 0,-1 0,1 0,-1 1,0 1,0-1,1 1,-2 0,1 1,0-1,-1 1,0 1,0-1,0 1,0 0,-1 0,0 1,0 0,8 12,6 9,-2 1,-2 1,15 34,-7-6,-3 1,-2 0,-3 2,-2 0,8 98,-20-145,1-1,0 1,5 16,-6-27,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,4 2,-4-4,0 1,-1-1,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1-1,1 1,0 0,0-1,0 0,-1 1,2-2,16-15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14968.15">3180 158,'-5'9,"-23"26,-26 33,-30 33,-19 21,-14 13,-10 5,7-7,20-17,18-20,19-21,19-23</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15673.22">3286 899,'0'9,"0"12,0 12,-5 13,-1 4,-4 2,-1 5,2-1,-2-7,1-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23624.15">3921 2990,'4'0,"2"5,-1 5,0 11,-6 10,-3 4,-10 6,-2 1,2-4,-2-2,2 0,-1-5,2-3,-1-3,-3 0,1-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20187.15">481 2540,'1'44,"3"-1,1 0,17 64,47 124,-33-121,54 140,-89-247,0 0,1 0,-1 0,1 0,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,1 1,-1-1,1-1,0 1,3 2,-3-4,0 1,-1-1,1 1,0-1,0 0,-1 0,1 0,0-1,0 1,-1-1,1 1,0-1,-1 0,1 0,-1 0,1 0,-1-1,1 1,-1-1,0 1,3-3,34-27,-1-1,-2-2,33-40,93-127,-92 112,-8 10,73-124,-124 183</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21067.15">2095 2249,'-3'20,"0"-2,-1 1,0 0,-2-1,0 0,-1 0,-19 34,4-8,-3 11,3 0,2 2,2 0,-19 116,30-117,2 1,3 0,2 0,9 61,-6-98,0 0,1-1,1 1,1-1,1 0,1-1,0 0,1 0,1-1,1 0,0 0,1-1,1-1,0 0,18 15,-9-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21871.15">2360 2857,'-1'-15,"2"1,0-1,0 0,2 0,0 0,0 1,1 0,1 0,1 0,0 0,0 1,2 0,-1 0,2 0,17-20,-20 26,0 1,1-1,0 1,0 1,0-1,0 1,1 1,0-1,0 1,0 0,0 1,1 0,-1 1,16-3,-19 4,1 1,0 0,0 0,0 1,0 0,0 0,-1 0,1 1,0 0,-1 0,1 0,-1 1,0-1,0 1,0 1,0-1,-1 1,1-1,-1 2,0-1,0 0,0 1,4 6,8 14,-1 1,0 1,-3 1,0 0,-1 0,-2 1,7 35,-16-60,1-1,0 1,-1-1,2 0,-1 1,0-1,1 0,-1 0,1 0,0 0,0 0,0-1,5 5,-5-5,0-1,0 0,1 0,-1 0,0-1,0 1,1-1,-1 1,1-1,-1 0,0 1,1-1,-1 0,1-1,-1 1,0 0,1-1,-1 1,0-1,4-1,24-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22419.15">3074 2381,'-4'23,"-1"-1,-1 0,0 0,-2 0,-20 39,16-34,-123 236,44-94,42-73,36-67</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23080.15">3180 2910,'4'0,"7"0,5 9,0 26,-2 11,-4 11,-4 5,-2-3,-2-8,-2-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17736.15">4715 370,'-43'534,"42"-527,0 4,-1-1,1 1,1-1,0 1,3 16,-3-25,1 1,-1-1,1 1,0-1,0 1,0-1,1 0,-1 1,0-1,1 0,0 0,-1 0,1 0,0-1,0 1,0 0,0-1,0 1,0-1,1 0,-1 0,0 1,1-2,-1 1,1 0,-1 0,1-1,2 1,2 0,0 0,0 0,-1 0,1-1,0 0,0 0,0-1,0 0,-1 0,1 0,0-1,-1 0,1-1,-1 1,0-1,0 0,0-1,0 1,-1-1,1-1,-1 1,0-1,0 1,0-2,-1 1,0 0,0-1,0 0,-1 0,5-9,20-45,-2-1,31-113,-18 51,-38 117,2 0,-1 0,1 1,0-1,0 0,0 1,6-7,-9 12,0-1,1 1,-1 0,0 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,1 0,-1 0,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 1,1 2,-1-1,0 1,0-1,0 1,0 0,0-1,0 1,-1 0,1 0,-1 3,8 99,-4 0,-5 1,-26 185,20-244,-3-1,-19 59,21-84,0-1,-1 1,-1-1,-1-1,-1 0,-28 34,35-48,0 0,-1-1,1 1,-1-1,-1 0,1-1,0 0,-1 0,0 0,1 0,-1-1,0 0,0-1,-1 0,-7 1,-6-1,0-1,0-1,-39-6,23 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18251.15">5429 1376,'4'0,"2"5,0 5,-1 6,-2 9,-1 5,-1 2,0-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24873.15">4582 2540,'-1'38,"2"0,1 0,2 0,16 65,-19-100,0 1,1 0,-1 0,1-1,0 1,0-1,0 0,0 1,1-1,-1 0,1 0,0-1,0 1,0 0,0-1,1 0,-1 0,0 0,5 2,-2-2,1 0,-1-1,1 0,-1 0,1 0,-1-1,1 0,0 0,-1-1,11-1,8-5,0 0,0-1,-1-2,36-19,-35 16,0-1,-1-1,-1-1,28-25,-41 32,-1 0,0-1,0-1,-2 1,1-2,-1 1,-1-1,0 1,0-2,-1 1,3-15,1-4,-2 23,-3 19,-1 22,-25 117,5-50,-44 284,58-364,-1 0,-1-1,-1 0,-1 0,0 0,-2 0,0-1,-1-1,-13 18,14-23,-1-1,0 0,-1 0,-1-1,1-1,-1 0,-1-1,0 0,0 0,-1-2,1 0,-26 8,8-5,-44 6,65-13,1-1,-1 0,1-1,-1 0,1 0,-1-1,0-1,1 1,-10-4,18 5,-1-1,1 1,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,1-1,1-1,0 0,0 0,0 0,0 0,1 1,-1-1,1 1,0-1,-1 1,1 0,0 0,4-1,26-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25342.15">5482 3386,'0'9,"-9"26,-8 20,0 14,-7 9,-4 1,4-5,4-33,7-36,5-20</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28544.15">270 4418,'-13'14,"2"1,0 0,-12 23,-10 13,10-19,1 1,2 1,2 1,1 1,1 0,2 1,2 1,2 0,1 0,1 1,-1 46,9-75,0-1,1 1,0-1,1 1,0-1,0 0,1 0,0 0,1 0,0 0,0-1,1 0,0 0,0 0,1 0,0-1,1 0,-1 0,1-1,1 0,-1 0,1 0,14 6,-3-1,0-2,1 0,0-2,1 0,0-1,0-1,0-1,0-1,33 0,-5-1,-6 0,0-2,0-1,0-2,77-16,-112 16,0 0,0 0,0-1,-1 0,0 0,1-1,-2 0,1 0,0 0,-1-1,0 0,6-8,-3 2,-1-1,0 0,-1 0,0-1,-1 0,6-18,0-14,-2-1,-2 0,3-58,-11 100,0-1,-1 1,1 0,-1 0,0 0,-4-10,5 14,0 1,0-1,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1 0,0 0,0-1,0 1,0 1,0-1,0 0,0 1,0-1,1 1,-1-1,0 1,0-1,0 1,1 0,-1-1,0 1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 2,-6 12,1 1,1-1,1 1,0 0,1 1,-2 29,3 105,2-142,1 0,0 0,0 0,1 0,0 0,0 0,1 0,0 0,7 12,-7-17,0 0,1 0,-1 0,1 0,0-1,0 1,0-1,1 0,-1 0,1-1,-1 1,1-1,0 0,0 0,0-1,0 1,9 0,24 4,0-2,0-1,1-2,61-7,-81 4,-1-1,1-2,-1 0,0 0,-1-2,1 0,-1-1,-1-1,0 0,0-2,0 1,-2-2,1 0,-1-1,-1 0,-1-1,13-17,-11 10,-1 0,0-1,-2 0,0-1,-2 0,0-1,-2 0,0 0,-2-1,-1 0,-1 0,0-32,-6-125,3 153</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1168 457,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1011">974 457,'-2'14,"1"0,-2-1,0 1,0-1,-2 1,0-2,0 1,-1-1,-2 1,1-1,0 0,-2-2,0 2,-1-2,1 1,-1-2,-16 12,-20 14,-2-2,-97 51,141-82,-78 39,38-18,-73 45,104-59,2 0,-2 2,3-2,-1 3,1-2,0 2,1 0,1 0,-13 25,10-15,2 1,0 1,-7 40,14-58,1 0,0 1,1 0,-1-1,1 1,1 0,-1-1,1 0,1 1,-1 0,1-2,0 2,0-1,1 1,0-2,0 1,1 0,6 7,8 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13160.62">891 0,'1'30,"-1"-1,-1-1,-2 1,0 0,-2 0,-2-1,-20 49,23-68,-17 35,-25 79,32-71,1 0,3 1,2 0,3 0,3 77,3-122,0-2,1 1,-1-1,2 0,-1 1,2 0,-1-1,0-1,0 2,1-1,0 0,1-2,0 2,0-1,7 6,-7-8,-1 1,1-1,0 1,1-1,-1 0,0-1,0 1,1-2,0 1,0 0,-1-1,2 1,-1-1,-1-1,1 1,1-1,-1 0,12-2,-14 1,0 0,0 0,0-1,0 0,0 1,-1-1,1 0,-1 0,0-1,1 1,-1-1,0 0,0 0,0 0,-1 0,0 0,1 0,0-1,1-7,4-7,-1 0,10-36,-7 20,-1 7,1-4,0 0,-3 1,6-43,-8 43,2 0,1 0,1 1,3 1,27-55,-14 32,-2 7,14-28,-35 66,1 0,-1-1,0 0,0 0,-1 1,0-1,0 0,-1-8,-24 49,-23 53,-39 101,76-168,1 1,2 0,-1 2,2-1,2 0,0 0,-1 33,4 32,-1-44,2 0,2 0,14 72,-15-108,1-2,-1 2,1-1,1 0,0 0,0 0,0 0,0 0,1-1,0 1,1-1,-1 0,1-1,-1 1,1 0,1-1,0 0,-1 0,1-1,1 0,-1 0,0 0,1 0,11 3,8-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16322.19">4241 1092,'0'5,"0"14,-5 25,-11 18,-7 8,-4 4,-9-1,5-9,0-7,-2-9,4-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13814.63">2247 0,'-20'12,"0"1,1 1,1 1,0 0,-29 32,30-27,1 1,0 2,2-1,1 1,0 0,3 1,-15 46,-33 184,57-247,-38 286,36-240,2-1,3 1,14 83,-10-108,2-2,14 35,-19-53,0 0,1 1,0-1,1-1,1 1,-1 0,1-2,0 1,1 0,-1-1,9 6,13 0,0-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14532.15">2441 559,'0'-11,"2"1,0-1,0 2,1-2,1 0,0 2,0-1,1 1,0-1,1 0,0 2,1-1,0 0,0 1,1 0,1 0,-1 2,0-1,2 0,-1 2,1-1,0 0,1 1,-1 0,0 2,1-1,0 1,1 0,-2 0,23-1,-26 5,2 0,-2 0,1 0,0 1,-1 1,0-1,2 1,-3 0,1 0,1 0,-2 1,0 1,0-1,1 1,-1-1,-1 1,0 1,1 0,7 11,7 9,-2 1,-2 1,15 32,-7-5,-3 1,-2-1,-4 3,-1-1,8 95,-21-139,1-2,0 2,6 15,-7-27,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0-1,1 1,-1 0,4 2,-4-4,0 0,-1 0,2 1,-1-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0 0,0-1,0 0,-1 1,3-2,15-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14968.15">3327 152,'-5'8,"-24"26,-28 31,-31 32,-19 20,-16 13,-10 4,8-6,20-16,19-20,20-20,20-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15673.22">3438 863,'0'9,"0"11,0 12,-5 12,-1 4,-5 2,0 5,1-2,-1-6,0-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23624.15">4103 2871,'4'0,"2"5,-1 4,1 12,-7 8,-4 5,-9 5,-3 2,2-5,-1-1,1-1,-1-4,3-3,-2-3,-3 0,1-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20187.14">503 2439,'1'42,"3"-1,2 1,17 60,49 120,-34-116,56 134,-93-237,0 0,1 0,-1-1,1 1,0 0,0-1,0 1,0-1,1 1,0-1,-1 0,1 1,-1-2,1 0,0 1,4 2,-4-4,0 1,-1-1,1 1,0-1,0 0,-1 0,2 0,-1-1,0 1,-1-1,1 1,0-1,-1 0,1 0,0 0,0 0,-1-1,1 1,-1 0,0 0,3-3,36-26,-1-1,-2-1,34-39,97-122,-95 107,-10 10,78-119,-131 176</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21067.15">2192 2159,'-3'20,"0"-3,-1 1,-1 0,-1 0,0-1,-2 0,-19 33,4-8,-3 11,3 0,2 2,2 0,-19 111,30-113,3 2,3 0,2 0,9 58,-5-94,-1 0,1 0,1 0,1-1,2 0,0 0,0-1,2 0,0-1,2 1,-1-1,2-1,0 0,1-1,19 15,-10-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21871.15">2469 2743,'-1'-14,"2"0,0 0,0 0,3-1,-1 1,0 0,1 1,1-1,2 1,-1 0,0 0,2 1,0-1,1 1,18-20,-20 25,-1 1,1 0,1 0,-1 1,0-1,1 2,0 0,0-1,1 1,-1 0,0 1,2 1,-2 0,17-3,-19 4,0 1,0 0,0 0,1 1,-1 0,0 0,-1 0,2 1,-1 0,-1-1,2 1,-2 1,0-1,0 1,0 1,1-1,-2 1,1-1,-1 1,0 0,1 0,-1 1,4 5,9 14,-1 1,-1 1,-2 1,-1 0,0 0,-3 1,8 33,-17-57,1-1,0 1,-1-1,2 0,-1 0,0 0,1 0,0 0,0 0,0 0,0 0,0-1,5 4,-5-4,0-1,0 0,2 0,-2 0,0-1,0 1,1-1,-1 1,1-1,-1 0,0 1,2-1,-2 0,1-1,-1 1,0 0,1-1,-1 1,0-1,5-1,24-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22419.15">3216 2286,'-4'22,"-1"-1,-1 1,-1-1,-1 0,-21 37,16-32,-128 227,46-91,43-70,39-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23080.15">3327 2794,'4'0,"8"0,5 9,-1 24,-1 12,-4 9,-5 6,-2-4,-2-7,-2-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17736.14">4933 355,'-45'513,"44"-506,0 3,-1 0,1 0,1 0,0 1,3 15,-3-25,1 2,-1-1,1 1,0-1,1 1,-1-1,1 0,-1 1,0-1,1 0,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,1 1,-1-1,1 0,-1 0,0 1,1-2,-1 1,1 0,-1 0,2-1,1 1,2 0,0 0,1-1,-2 1,1-1,1 0,-1 0,0-1,1 1,-2-1,1 0,1-1,-2 0,1-1,-1 1,1-1,-1 0,0-1,1 1,-2 0,1-2,-1 1,1-1,-1 1,0-1,-1 0,0 0,1-1,-1 0,-1 1,5-10,22-42,-3-2,32-108,-18 49,-40 112,2 0,-1 1,2 0,-1-1,0 0,0 2,6-8,-9 12,0-1,2 1,-2 0,0 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,1 0,-1 0,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 1,1 2,-1-1,0 1,0-1,0 1,0-1,0 0,1 1,-2 0,1 0,-1 3,8 95,-4-1,-5 2,-27 178,21-235,-4-1,-19 57,21-81,1-1,-1 1,-2-1,0 0,-2-1,-29 33,37-46,0-1,-2 0,2 1,-1-1,-1 0,0-1,1-1,-1 1,-1 0,2 0,-1-1,-1 0,1-1,-1 0,-8 1,-6-1,0-1,0-1,-41-6,25 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18251.14">5680 1321,'5'0,"1"5,0 5,-1 5,-1 9,-2 5,-1 2,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24873.15">4794 2439,'-1'36,"2"1,1-1,3 1,15 62,-18-96,-1 0,1 1,-1 0,1-1,0 1,0-1,0 0,0 0,1 0,-1 0,2 0,-1-1,0 1,0 0,0-1,1 0,-1 0,1-1,4 3,-2-2,2 0,-2-1,1 0,-1 0,2 0,-2-1,1 0,1 0,-2-1,12-1,8-5,0 1,0-2,-1-2,38-17,-37 14,0 0,0-2,-2 0,29-25,-43 32,0-1,-1 0,1-2,-3 1,1-1,0 0,-2 0,0 0,1-1,-2 0,3-14,2-3,-3 21,-3 18,-1 22,-26 112,5-48,-45 273,59-350,0 0,-1 0,-1-1,-2 0,1 0,-2 1,-1-2,0-1,-14 18,14-23,0 0,-1-1,0 1,-2-1,2-2,-2 1,0-2,-1 1,0 0,0-2,0-1,-27 9,9-6,-47 7,69-13,1-1,-2 0,2-1,-2 0,2 0,-2-1,1-1,0 1,-9-4,18 5,-2-1,2 1,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-2-1,2 1,0 0,0 0,0 0,0 0,0-1,0 1,2 0,-2 0,0 0,0 0,1 0,1-2,0 0,0 0,0 0,0 0,1 1,-1-1,1 1,1 0,-2 0,1 0,0 0,4-1,28-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25342.15">5736 3251,'0'9,"-9"24,-9 20,0 14,-7 7,-4 2,3-5,6-31,6-36,6-18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28544.15">282 4242,'-13'14,"1"0,1 0,-13 23,-11 12,11-18,1 0,2 2,2 0,2 2,0 0,2 0,3 2,1-1,2 1,0 0,0 45,9-73,0 0,1 1,0-2,1 2,0-2,0 1,2 0,-1-1,1 1,0 0,0-2,1 1,1 0,-1-1,1 1,0-1,2-1,-2 1,1-1,2 0,-2-1,1 1,15 6,-3-2,0-1,1 0,0-3,1 1,0-1,0-1,0-2,0 0,34 0,-4-1,-7 0,0-2,0-1,0-2,80-15,-116 15,-1 0,0 0,1-1,-2 1,0-1,2-1,-3 0,1 0,1 1,-2-2,0 0,7-7,-4 1,0 0,-1-1,-1 1,1-2,-2 1,6-18,1-13,-3-1,-1 0,2-56,-11 96,0-1,-1 1,1 1,-1-1,0 0,-4-9,5 13,0 1,0-1,-1 0,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1 0,-1 0,1-1,0 1,0 1,0-1,0 0,0 1,0-1,1 1,-1-1,0 1,0-1,0 1,1 0,-1-1,0 1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 1,-7 13,2 0,1 0,1 0,0 0,0 2,-1 27,3 101,2-137,1 1,0 0,0-1,1 1,0 0,0-1,2 1,-1 0,7 11,-7-16,0-1,2 1,-2 0,1 0,0-1,0 1,1-1,0-1,-1 1,1-1,-1 1,2-1,-1 0,0 0,0-1,1 1,8 0,26 3,0-1,-1-1,2-2,64-7,-85 4,-1 0,0-3,0 0,0 0,-1-2,1 1,-1-2,-2-1,1 1,0-3,0 2,-3-3,2 1,-1-2,-2 1,0-2,13-16,-11 10,-2 0,1-1,-3 0,1-1,-3 0,1-1,-3 0,0 0,-2-1,0 0,-2 0,0-31,-6-120,3 147</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7890,7 +8018,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 255,'2'-12,"0"-1,1 0,1 1,0 0,1 0,1 0,-1 0,15-20,-13 21,0 1,1 0,0 1,1-1,0 1,1 1,14-11,-17 14,1 0,-1 1,0 0,1 1,0-1,0 1,0 1,0 0,0 0,1 0,15 0,-21 2,1 0,-1 0,0 1,0 0,1-1,-1 1,0 0,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,4 5,-3-3,-1 1,1 0,-1 1,0-1,0 0,0 1,-1 0,3 9,1 9,-2 0,0 0,-1 40,-2-49,-1 31,-3 0,-1 0,-3-1,-18 67,22-97,-3 10,2 0,0 0,2 1,1-1,1 1,5 46,-4-64,1 0,-1 0,2 0,-1 0,1 0,0 0,0 0,1-1,0 0,1 1,-1-2,1 1,1 0,-1-1,1 0,0-1,1 1,-1-1,1 0,0-1,0 1,1-1,-1-1,13 5,-16-7,1 1,-1-1,1 0,-1 0,1 0,-1-1,1 1,0-1,-1-1,1 1,-1 0,1-1,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,0 0,-1 0,1 0,4-6,2-5,0 0,-1-1,-1-1,0 0,9-28,11-20,-1 6,-3-2,31-120,-43 137,-8 26,-3 11,1 0,-1 0,1 0,0 0,0 1,0-1,1 1,0-1,5-6,-7 12,-1 0,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,-1 0,1 1,0 18,-33 148,19-106,3 0,-7 114,17-106,-1-22,2-1,10 84,-8-121,1 0,0-1,0 1,0 0,1-1,1 0,-1 0,1 0,9 10,-2-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 246,'2'-12,"0"0,2-1,0 2,1-1,0 1,2-1,-2 0,17-18,-14 19,0 1,1 1,0 0,1-1,0 2,1 0,15-10,-18 13,1 0,-1 1,-1 0,2 1,0 0,0 0,0 1,0 0,0 0,1 0,16 0,-23 2,2 0,-2 0,1 1,-1 0,1-1,0 1,-1 0,0 0,1 1,-1-1,0 1,1-1,-2 1,1-1,0 1,5 5,-3-3,-2 1,1 0,0 0,-1 0,0 0,1 1,-2 0,3 8,2 9,-3 0,1 1,-2 37,-2-46,-1 29,-3 1,-1-1,-4-1,-20 65,25-93,-4 9,3 0,-1 0,3 1,1-1,1 2,6 43,-5-61,1-1,-1 1,2 0,-1 0,2-1,-1 1,0 0,2-2,-1 1,2 1,-2-2,2 0,0 1,0-1,1 0,-1-1,2 0,-1 0,0 0,1-1,0 1,1-1,-1-2,14 6,-18-7,2 1,-2-1,2 0,-2 0,2 0,-2-1,2 1,-1-1,0-1,0 1,0 0,0-1,0 0,0 0,-1-1,2 1,-2-1,1 0,-1 0,1 0,-1 1,1-2,-1 0,-1 0,2 0,4-6,2-4,0-1,-1 0,-1-2,-1 1,11-28,12-18,-1 5,-3-2,34-116,-48 133,-9 24,-2 12,0-1,-1 0,1 0,0 0,1 2,-1-2,1 1,0-1,6-5,-8 11,-1 0,0 0,1 0,-1 0,0 0,0 0,2 1,-2-1,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,-1 0,1 1,0 18,-37 142,22-102,3-1,-8 111,19-102,-2-22,3 0,11 80,-8-116,0-1,0 0,1 1,-1-1,1 0,2 0,-2 0,2-1,9 11,-1-3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7971,15 +8099,15 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 476,'0'-5,"1"-1,1 1,-1 0,1-1,0 1,0 0,1 0,0 0,-1 0,1 1,1-1,3-4,49-48,-49 52,1 1,0-1,0 1,0 1,1-1,-1 1,1 1,-1 0,1 0,0 0,15 1,15-1,53 6,-58-2,-2 1,0 1,-1 1,0 2,0 1,0 1,-1 2,-1 1,1 1,-2 2,0 1,-1 1,-1 1,0 1,-2 1,0 2,-1 0,-2 2,30 40,-19-14,35 76,-44-77,3-1,34 48,-57-92,1 0,-1 1,1-1,-1-1,1 1,0 0,0-1,1 0,-1 0,1 0,0 0,0-1,-1 0,1 0,7 1,-5-2,-1 0,1-1,-1 0,1 0,-1-1,1 0,-1 0,1 0,-1-1,0 0,0 0,7-4,20-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="534">1324 0,'-5'5,"-6"10,-9 16,-7 12,-12 17,1 7,2 1,-6 2,4-6,4-5,8-7,3-10,6-5,6-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2659">1244 80,'-1'4,"0"-1,0 1,0-1,0 0,0 0,-1 0,0 0,1 0,-4 5,-5 8,-31 68,-4 14,-109 169,73-143,45-65,-85 104,106-147,1 0,1 1,0 1,-17 32,18-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3799">1721 953,'-5'5,"-1"5,0 11,1 15,-2 1,-1-1,1-2,2-3,2-1,-4 2,0 6,1 0,-2-6,-1-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4207">1694 715,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4813.64">1985 767,'0'14,"0"13,0 7,0 11,0 6,0 9,0 3,9 4,3 0,-1-8,-2-8,-2-9,-3-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5549.17">1932 1138,'4'0,"7"0,5 0,5 0,3 0,2 0,10 0,4 5,-1 1,-3-1,-6 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6695.17">2620 1164,'0'-203,"0"809,0-583</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7725.17">2435 1138,'0'-4,"0"-7,4-5,7 0,0-2,9 2,4-1,3-1,2 1,-5 0,-2 3,-4-2,4-1,-2 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 457,'0'-5,"1"-1,1 1,-1 1,1-2,1 1,-1 0,1 1,0-1,-1 0,1 1,2-1,2-3,53-47,-53 50,2 1,-1 0,1 0,-1 1,2-1,-2 1,2 1,-2 0,2 0,-1 0,17 1,15 0,57 4,-62-1,-2 1,1 1,-2 1,-1 2,1 0,0 2,-1 1,-1 2,1 0,-2 3,0 0,-2 1,0 2,0 0,-3 1,1 2,-2 0,-1 2,31 39,-20-14,37 73,-46-74,2-1,37 46,-61-88,2 0,-2 0,1 0,-1-1,1 1,1 0,-1-1,1 0,0 0,0-1,0 1,0-1,0 0,0 0,8 1,-6-2,0 0,0-1,-1 0,2 0,-2-1,2 0,-2 0,2 0,-2-1,0 0,1 0,7-4,21-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="534">1408 0,'-5'5,"-7"9,-9 16,-8 11,-12 17,0 6,3 1,-7 3,5-7,4-4,8-7,4-10,6-5,6-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2659">1323 77,'-1'4,"0"-1,0 0,0 0,0 0,0 0,-1 0,0 0,1 0,-5 4,-4 9,-34 64,-4 14,-116 163,78-138,48-63,-91 101,113-142,1 0,1 2,1 0,-19 31,19-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3799">1831 915,'-6'4,"0"6,0 10,0 15,-1 0,-2 0,2-3,2-2,1-1,-3 2,-1 5,2 1,-2-7,-2-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4207">1802 686,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4813.64">2111 736,'0'14,"0"11,0 8,0 10,0 6,0 9,0 2,10 5,3-1,-1-7,-3-8,-1-9,-4-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5549.17">2055 1092,'4'0,"8"0,5 0,5 0,4 0,2 0,10 0,4 5,0 1,-4-1,-6-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6695.17">2787 1117,'0'-195,"0"777,0-560</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7725.17">2590 1092,'0'-4,"0"-6,4-6,8 1,0-2,9 1,5 0,2-1,3 1,-5-1,-3 4,-4-3,5 0,-3 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8031,10 +8159,10 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">222 1220,'0'5,"-5"5,-5 11,-11 5,-1 4,-7 1,-2-5,-5-3,-1-4,6-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1212.65">725 2,'111'-1,"116"3,-223-1,-1-1,0 1,0 0,0 0,1 0,-1 0,0 0,0 1,0-1,-1 1,1 0,0 0,-1 0,1 0,-1 1,0-1,1 1,-1-1,-1 1,1 0,0 0,0 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,0 0,1 5,0 6,-1 1,0-1,-1 1,0-1,-2 1,-4 19,-2-7,-1 1,-1-2,-2 0,-24 39,-77 97,61-89,-27 33,33-45,-55 93,101-153,0 1,0-1,0 1,0-1,0 1,1-1,-1 1,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,0 0,-1-1,1 1,2-1,12 4,-1 0,1-2,-1 0,21 0,-23-1,315 0,-257-2,-32 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1715.65">1571 611,'0'18,"0"15,0 7,0 9,0 6,-5 11,-1 0,-8 1,-3-6,-2-4,2-8,4-7,4-16,3-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2073.65">1704 294,'-5'0,"-6"5,0 14,-4 27,1 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">233 1166,'0'5,"-5"4,-6 11,-11 5,-1 4,-7 1,-3-6,-5-2,0-3,5-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1212.64">761 2,'116'-1,"122"3,-233-1,-2-1,0 1,0 0,0 0,1 0,0 0,-1 0,0 1,0-2,-1 2,1 0,0 0,-1 0,2 0,-2 1,0-1,1 1,-1-1,-1 0,1 1,0 0,0 0,-1 0,0 0,1 0,-1 0,0-1,0 1,0 1,-1-1,0 0,1 4,0 7,-1 0,0 0,-1 0,0-1,-2 2,-5 17,-1-6,-2 1,0-2,-3-1,-25 38,-80 93,63-85,-28 31,35-42,-58 88,106-146,0 1,0-1,0 1,0-1,-1 1,2-2,-1 2,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,1-1,-1 0,0 1,1 0,-1-1,1 1,-1 0,2-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,-1-1,1 1,2-1,13 4,-1 0,0-2,0-1,22 1,-24-1,330 0,-270-2,-33 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1715.65">1648 584,'0'17,"0"15,0 6,0 9,0 5,-5 11,-1 1,-9 0,-3-6,-2-4,3-7,3-7,4-15,4-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2073.65">1788 281,'-5'0,"-7"5,1 13,-5 26,1 6</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8060,22 +8188,22 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">136 3968,'-4'53,"-1"0,-3-1,-24 85,7-29,1 24,5 2,7 0,6 169,7-258,6 43,-5-73,1 0,1 0,0-1,1 1,0-1,13 21,1-1,35 47,-36-59</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="855">639 4630,'-1'-15,"1"-1,1 0,1 0,0 0,1 1,6-22,-7 32,0 1,1-1,-1 1,1 0,0-1,0 1,0 1,0-1,1 0,-1 1,1-1,0 1,0 0,1 1,-1-1,0 1,1 0,0 0,-1 0,1 0,0 1,0 0,0 0,7-1,-1 2,-1 0,1 0,0 1,-1 0,1 1,-1 1,0-1,0 1,0 1,0 0,0 0,-1 1,16 11,-1 0,-1 2,0 1,35 38,-31-25,-1 1,-1 1,21 39,52 114,-85-160,17 37,34 61,-19-49,-26-47</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1398">1432 4497,'-5'0,"-5"0,-15 5,-8 6,-11 23,-4 15,-15 13,3 5,-2 4,5-1,3 2,11-8,8-10,6 0,3-5,6-7,6-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1926">1988 5106,'0'23,"0"16,-5 15,-14 11,-5 0,-2 3,-2-7,0-9,5-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3442">2597 5265,'0'9,"0"8,0 9,-5 10,-10 12,-12 11,-10 5,-3-4,-9 1,0-1,-1-5,4-4,9-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4749.52">2888 4524,'1'1,"0"0,0-1,0 1,0 0,0 0,0 0,0-1,-1 1,1 0,0 0,0 0,-1 0,1 1,0-1,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 1,4 42,-3-37,2 240,0 11,-3-255,1-1,-1 0,0 0,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 0,1 0,-1 0,0 0,0-1,1 1,0 0,-1-1,1 1,0-1,2 2,-1-1,1-1,-1 0,1 1,0-1,-1-1,1 1,0 0,-1-1,1 0,0 0,6-1,3 0,0-2,0 0,-1 0,1-1,-1-1,15-7,-12 3,-1 1,0-2,-1 0,0-1,-1 0,0-1,0 0,15-23,0-6,34-68,-59 106,20-36,-11 30,-6 15,-4 26,-1-31,-8 82,-3-1,-34 127,40-190,-1 1,-1-1,-1 0,-19 33,24-46,0-1,-1 0,0-1,0 1,0-1,0 1,-1-1,0 0,0-1,0 1,0-1,0 0,-1 0,1-1,-1 0,0 0,0 0,0-1,0 1,-6-1,10-1,-1 1,1-1,0-1,0 1,-1 0,1 0,0-1,0 0,-1 1,1-1,0 0,0 0,0 0,0 0,-3-2,-7-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5286.52">3470 5265,'0'5,"0"5,0 11,0 10,0 14,0 12,0 1,0 0,0-5,0-17,0-14</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="99169.54">4131 2831,'22'-1,"0"-2,0 0,-1-2,43-14,-7 2,277-62,-254 64,1 5,102-2,-180 12,0 0,0 0,0 0,-1 0,1 0,0 1,0-1,0 1,-1 0,1 0,0 0,-1 0,1 0,-1 1,0-1,1 1,-1-1,0 1,0 0,0 0,0 0,0 0,2 4,-2-2,0 0,-1 1,1-1,-1 1,0 0,-1-1,1 1,-1 0,0-1,0 1,0 0,-1-1,-1 7,-2 9,-1 0,-1 0,-1-1,0 0,-1-1,-2 1,0-1,0-1,-17 21,-16 13,-75 69,77-81,1 2,-49 66,79-93,0 2,1-1,1 1,0 1,1 0,1 0,1 0,0 1,-3 28,7-44,1 0,0 1,0-1,1 0,-1 1,0-1,1 0,0 0,-1 1,1-1,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,3 3,0-1,0 0,1 0,-1-1,1 0,0 1,-1-1,1-1,10 3,6 0,1-1,0-1,29-2,-48 0,432-5,-402 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="99683.53">5507 3360,'4'0,"2"5,0 19,-6 19,-3 11,0 10,-1-1,1-3,1-6,1-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100383.79">5586 2989,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="101765.79">4237 4762,'0'-1,"1"0,-1 0,1 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0 0,1-1,-1 1,0 0,1 0,37-4,-34 3,396-7,-273 10,-126-2,8 0,0 0,0 0,0 1,-1 1,17 3,-23-4,-1 0,1 1,-1-1,1 0,-1 1,1 0,-1 0,0-1,0 1,0 0,0 1,0-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,0-1,0 1,0 0,-1 0,2 5,0 9,0 1,0 0,-2 0,0-1,-1 1,-1 0,-1-1,0 1,-2-1,1 0,-11 23,-7 6,-2 0,-48 65,1 1,62-98,1 0,1 1,0 0,1 1,-7 25,12-38,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1-1,1 1,-1 0,0 0,1-1,-1 1,1 0,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 0,4 0,51 10,0-2,0-2,88-3,-102-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="102206.79">5295 5397,'0'5,"0"10,0 12,0 14,-5 1,-5 6,-6-4,-1-2,-1-7,3-5,3-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="102986.78">4025 5529,'0'5,"0"10,-5 7,-1 14,-8 5,-30 17,-15 0,-3-1,4-11,9-13,16-21,14-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="103987.77">5904 0,'-1'1,"0"-1,0 0,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 2,1 36,-1-35,29 222,-8-82,19 202,-6 393,-35-684,-2-1,-15 74,11-96,-1-1,-2 0,-1-1,-1 0,-23 38,11-27,-38 49,32-54</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="104773.82">5719 2434,'1'14,"1"-1,0 1,1-1,1 0,10 25,7 28,-7 6,-4 0,1 78,-12 150,-1-145,2-105,-3-1,-2 1,-17 78,16-105,-1 0,-1-1,-1 0,-1 0,0-1,-2 0,-1-1,0 0,-28 31,19-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="105663.82">5428 4497,'3'1,"1"-1,0 1,0-1,-1 1,1 0,-1 0,1 1,-1-1,1 1,-1-1,0 1,1 0,-1 1,5 4,37 44,-25-25,110 134,159 255,-278-398,-1 1,-1 0,0 0,-1 1,-2 0,1 1,-2 0,-1 0,0 0,-2 0,0 0,-1 1,-1-1,-1 1,-1-1,-7 31,2-21,-2-1,-1 0,-2-1,0 0,-2-1,-1 0,-1-2,-2 1,0-2,-25 26,-31 26,-125 101,198-177,-22 18,-52 30,41-28,10-2,6 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">142 3806,'-4'51,"-2"0,-2-1,-25 81,7-27,1 23,5 1,7 1,7 161,7-247,6 42,-5-71,2 1,0-1,0 0,1 0,0-1,14 21,1-1,36 44,-37-56</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="855">666 4441,'-1'-14,"1"-1,1-1,1 1,0 0,1 0,6-20,-6 30,-1 1,1-1,-1 1,1 1,0-2,0 1,0 1,0-1,2 0,-2 2,1-2,0 1,0 0,1 1,0-1,-1 1,1 0,0 0,-1 1,2-1,-1 1,0 0,0 0,8-1,-2 2,0 0,0 0,1 1,-2 0,1 1,0 1,-1-2,1 2,-1 1,1 0,-1 0,-1 1,17 10,-1 0,-1 3,0 0,37 36,-33-23,-1 1,-1 0,22 38,54 110,-88-154,17 35,36 59,-21-47,-26-45</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1398">1492 4314,'-5'0,"-6"0,-15 5,-8 5,-12 23,-4 14,-15 12,2 6,-2 3,6-1,3 2,11-8,8-9,7 0,3-5,6-7,7-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1926">2071 4898,'0'22,"0"16,-5 13,-15 12,-5-1,-2 3,-2-6,0-9,5-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3442">2706 5051,'0'8,"0"8,0 9,-5 10,-11 11,-12 11,-10 4,-4-3,-9 0,0 0,-1-6,4-3,9-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4749.52">3009 4340,'1'1,"0"0,0-1,0 1,0 0,1 0,-1-1,0 0,-1 1,1 0,0 0,0 0,-1 0,1 1,0-1,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 1,4 40,-3-35,2 229,0 12,-3-245,1-1,-1 0,0 0,1 0,-1 0,1 0,1 0,-2 0,1 0,0 0,0 0,1 0,-1 0,0 0,0-1,1 1,0-1,-1 0,1 1,0-1,2 2,0-1,0-1,-1 0,1 1,0-1,-1-1,1 1,1 0,-2-1,1 0,0 0,7-1,2 0,1-2,-1 0,0 0,0-1,0 0,15-8,-13 3,0 2,0-3,-2 1,1-2,-2 0,1 0,-1-1,16-21,1-6,34-66,-61 102,21-34,-11 28,-7 15,-4 25,-1-31,-9 80,-2-1,-36 121,42-182,-1 2,-2-2,0 0,-20 32,25-44,0-1,-2-1,1 0,0 1,0-1,0 1,-1-2,-1 1,1-1,0 1,0-1,0 0,-2 0,2-1,-1-1,0 1,-1 0,1-1,0 1,-7-1,11-1,-1 1,1-1,0-1,0 1,-1 0,1 0,0-1,-1 0,0 1,1-1,0 0,0 0,0 0,0 0,-3-1,-8-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5286.52">3616 5051,'0'4,"0"6,0 10,0 10,0 13,0 12,0 0,0 1,0-5,0-17,0-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="99169.54">4304 2716,'23'-1,"0"-2,0 0,-1-2,45-13,-8 2,289-60,-264 61,0 6,107-3,-188 12,0 0,0 0,0 0,-1 0,1 0,1 1,-1-1,0 1,-1 0,1 0,0 0,-1 0,1 0,-1 1,1-1,0 1,-1-1,0 1,0 0,0 0,0 0,0-1,2 5,-2-2,0 0,0 1,0-2,-1 2,0 0,-1-1,1 1,-1 0,0-2,0 2,0 0,-1-1,-1 6,-3 10,0-1,-1 0,-1-1,-1 0,0 0,-2 0,-1-1,1-1,-18 21,-17 12,-78 66,80-78,1 3,-50 62,81-88,1 1,1-1,0 2,1 0,1 0,0 1,2-1,0 1,-3 27,7-42,1 0,0 1,0-1,1 0,-1 1,0-1,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,3 3,0-2,1 1,0 0,-1-1,1 0,0 1,0-1,0-1,10 3,7-1,1 0,0-1,30-2,-50 0,451-5,-420 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="99683.53">5738 3223,'4'0,"3"5,-1 18,-6 18,-3 11,0 9,-1 0,0-4,2-5,1-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100383.79">5821 2867,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="101765.79">4415 4568,'0'-1,"1"0,-1 0,1 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,0 1,0 0,0 0,0-1,1 1,-1-1,0 1,0 0,0 0,1-1,-1 1,0 0,1 0,39-4,-36 3,413-7,-285 10,-131-2,9 0,-1 0,0 0,1 1,-2 1,18 3,-24-4,-1 0,2 1,-2-1,1 0,-1 0,1 1,-1 0,0-1,0 1,0 0,0 1,1-1,-1 0,-1 1,1-1,-1 0,1 0,-1 1,0-1,0 1,0 0,-1 0,2 4,0 10,0 0,0 0,-2 1,0-2,-1 1,-1 0,-1 0,0 0,-2-1,1 1,-12 21,-7 6,-2 0,-50 63,1 0,65-93,0-1,2 1,0 1,0 0,-6 24,12-36,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0-1,1 1,-1 0,1 0,0 0,-1 0,1-1,1 1,-1-1,0 1,1-1,-1 1,1 0,0-1,1 0,-1 1,0-1,0 0,0-1,1 1,-1 0,1-1,-1 1,1-1,1 1,-2-1,1 0,0 0,0 0,4 0,54 9,-1-1,1-2,91-3,-106-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="102206.79">5517 5177,'0'5,"0"9,0 12,0 14,-5 0,-5 6,-7-4,-1-2,0-6,2-5,3-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="102986.78">4194 5304,'0'5,"0"9,-5 7,-1 14,-9 4,-31 17,-15-1,-4 0,5-11,9-12,16-21,15-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="103987.77">6152 0,'-1'1,"0"-1,0 0,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,0 0,1-1,-2 1,1 0,1 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,1 0,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 2,1 34,-1-33,30 213,-8-79,20 194,-7 377,-36-656,-2-2,-15 72,10-92,0-1,-2-1,-2 0,0 0,-25 36,12-25,-40 46,34-52</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="104773.82">5959 2335,'1'13,"1"0,0 0,2 0,0-1,10 25,8 26,-7 6,-5 0,2 75,-13 144,-2-140,3-100,-3-1,-2 1,-18 75,17-101,-1 0,-2-1,0 0,-1 1,-1-2,-1 0,-2-1,1 0,-30 30,20-28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="105663.82">5656 4314,'3'1,"1"-1,0 1,1-1,-2 1,1 0,-1 0,1 1,-1-1,1 0,0 0,-1 1,1 0,-1 1,5 4,39 42,-26-24,115 128,165 245,-290-381,0 0,-2 0,0 0,0 2,-3-1,1 1,-2 0,0 0,-1 1,-2-1,0 0,-1 1,-1-1,-1 1,-1 0,-8 29,3-21,-2 0,-2 0,-1-1,-1 0,-1-1,-2-1,-1-1,-1 1,-1-2,-26 25,-32 25,-130 97,206-170,-23 17,-54 29,42-26,11-3,6 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8215,14 +8343,14 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 0,'-2'174,"4"187,-2-352,1 0,0 0,0 0,0-1,1 1,1 0,-1-1,7 14,-6-18,-1-1,0 0,1 0,0 0,-1-1,1 1,1-1,-1 1,0-1,0 0,1 0,-1 0,1-1,0 1,-1-1,1 0,0 0,0 0,0-1,0 1,6-1,9 2,1-2,0 0,-1-1,1-2,-1 1,24-8,-31 6,0 0,0-1,0 0,-1-1,0 0,0 0,-1-2,0 1,0-1,16-17,15-22,-2-2,-1-1,34-63,-60 93,-1-1,-1 0,-1-1,-1 0,-1-1,-1 1,-1-1,-1 0,0-1,-2 1,-2-36,0 257,-3-118,-8 295,-5 394,16-765,1 0,-1 1,-1-1,1 0,-1 1,1-1,-1 0,-1 0,1 0,0 0,-1 0,0 0,0 0,0 0,0-1,-1 1,0-1,1 0,-6 5,2-4,0-1,0 0,0 0,0 0,0-1,-1 0,1 0,-1 0,1-1,-1 0,-12 0,-6 1,1-1,-1-1,1-2,-44-6,62 6,1 1,-1 0,1-1,-1 0,1-1,0 1,0-1,0 0,0 0,0 0,1-1,0 0,-1 0,1 0,1 0,-1-1,1 1,-1-1,1 0,0 0,1 0,0-1,-1 1,2 0,-1-1,-1-5,-1-24,1 1,2-1,3-43,-2 78,1-26</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="699.99">876 1138,'0'9,"0"8,0 5,0 3,4 3,2 4,0 2,-1 0,-2-2,-1-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1202.99">956 847,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1751.99">1538 635,'4'0,"6"0,7 0,26 0,20 5,8 1,5 0,-5-1,-6-2,-10-1,-9-1,-8 4,-11 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2305.01">1538 953,'9'0,"34"0,24 0,18 0,8 0,2 0,-6 0,-10 0,-17 5,-20 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3487">2649 239,'-1'0,"1"0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0-1,0 1,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0-1,0 1,0 0,0 0,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0-1,0 1,0 0,1 0,-1 0,15-11,1 4,-1 1,1 1,1 1,-1 0,1 1,24-1,102 3,-134 1,0 1,0-1,-1 2,1-1,0 1,-1 1,0-1,1 1,-1 1,14 7,-18-7,0-1,0 1,0-1,0 1,-1 0,1 1,-1-1,0 0,0 1,-1 0,1 0,-1 0,0 0,0 0,-1 0,0 0,0 1,1 9,1 13,-2 0,-1 1,-1-1,-2 1,-1-1,-10 41,13-64,0-1,0 0,0 0,1 0,0 0,0 1,0-1,0 0,1 0,0 0,-1 0,2 1,-1-1,0 0,1-1,-1 1,1 0,0 0,1-1,3 6,6 4,0 1,1-2,24 20,13 12,-37-30,-7-9,1 1,-1 1,-1-1,1 1,-1-1,-1 2,1-1,-1 0,0 1,-1 0,0 0,0 0,-1 0,3 13,-5-21,2 18,0 0,-2 0,0 0,-2 18,1-31,0 0,0 0,0 0,-1-1,1 1,-1 0,0-1,0 0,-1 1,0-1,1 0,-1 0,-1 0,1-1,-1 1,1-1,-1 0,0 0,0 0,-4 2,-13 5,1-2,-1 0,-1-1,1-2,-1 0,-38 3,-141 0,164-7,-19-2,13 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3893">3549 900,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5452.99">5242 159,'0'6,"0"0,0 1,0-1,-1 0,1 0,-1-1,-1 1,1 0,-4 7,3-10,0 0,-1-1,1 0,-1 1,1-1,-1 0,0 0,0-1,0 1,0 0,0-1,0 0,0 0,0 0,-1 0,1 0,0-1,-1 1,-3-1,-99 10,-174-6,166-6,10 1,1-1,-112 13,200-9,1-1,0 2,-1 0,1 1,-14 6,25-9,0 1,-1 0,1 0,0 0,0 0,0 0,1 0,-1 1,0 0,1-1,0 1,-1 0,1 0,1 0,-1 1,0-1,1 0,-1 1,1-1,0 1,0-1,1 1,-2 6,2 1,-1 0,2 0,-1 0,1 0,1 0,0 0,1 0,0-1,0 1,1-1,0 0,1 0,0-1,1 1,0-1,1 0,-1-1,2 1,-1-1,1-1,0 1,1-1,0-1,0 0,0 0,1-1,0 0,0 0,0-1,0-1,1 1,0-2,-1 0,1 0,21 0,15-3,-21 0,50 3,-66 0,-1 0,1 0,0 0,-1 2,0-1,0 1,0 0,14 9,-6 0,-1 0,-1 1,0 0,-1 1,0 1,-1 0,-1 1,-1 1,10 18,-2 2,-1 1,-3 0,17 59,-31-93,4 13,0 0,-1 1,-2 0,2 32,-4-47,0 0,0 0,-1 0,1 0,-1 1,0-1,0 0,-1-1,1 1,-1 0,0 0,0-1,0 1,0-1,-1 1,1-1,-1 0,0 0,0 0,0 0,-1-1,1 1,0-1,-1 0,0 0,1 0,-6 1,-19 6,-1-1,1-2,-1-1,-37 2,-124-3,146-4,27 0,-201-5,180 2,0-1,0-2,-60-18,75 15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 0,'-2'170,"4"183,-2-345,1 1,0 0,0 0,0-1,1 0,2 1,-2-1,7 13,-6-17,-1-1,1 0,0 0,0 0,-1-1,1 1,1-1,0 1,-1-1,0 0,1 0,-1 0,1-1,1 1,-2-1,1-1,0 1,0 0,1-1,-1 1,6-1,11 2,0-2,0 0,-1-1,1-2,-1 2,25-9,-32 6,-1 0,1-1,0 0,-2-1,1 0,0 1,-2-3,1 1,-1-1,18-16,15-22,-2-2,-1-1,36-61,-63 90,-2 0,0-1,-2 0,0-1,-2 0,-1 0,0 0,-2-1,0 0,-2 0,-2-34,0 250,-3-115,-9 289,-5 384,17-747,2-1,-2 2,-2-1,2 0,-1 1,1-1,-1 0,-1 0,1 0,0 0,-1-1,0 1,0 0,0 0,0-1,-2 1,1-1,1 0,-6 5,1-4,1-1,0-1,-1 1,1 0,0-1,-2 0,2 0,-1 0,0-1,0 0,-13 0,-6 1,0-1,0-1,1-2,-47-6,66 6,0 1,0 0,1-1,-2 0,2 0,0 0,0-1,-1 0,1 0,0 0,1-1,-1 0,0 0,1 0,1 0,-1-1,0 2,0-2,1 0,0 0,1 0,0-1,-2 1,3 0,-1-1,-1-4,-1-24,1 0,2 0,3-42,-2 76,1-25</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="699.99">923 1111,'0'9,"0"8,0 4,0 4,5 2,1 4,0 3,0-1,-3-2,-1-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1202.99">1008 827,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1751.99">1621 620,'4'0,"7"0,7 0,27 0,22 5,8 1,5 0,-5-1,-7-2,-10-1,-10-1,-7 3,-13 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2305.01">1621 931,'10'0,"35"0,26 0,18 0,9 0,3 0,-8 0,-9 0,-19 5,-21 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3487">2792 233,'-1'0,"1"0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0-1,0 1,0 0,0 0,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0-1,0 1,0 0,2 0,-2 0,15-11,2 4,-1 1,1 1,1 1,-1 1,1 0,25-1,108 3,-142 1,1 1,-1-1,-1 2,2-1,-1 1,0 0,-1 0,2 1,-2 1,15 7,-18-7,-1-1,0 1,0-1,0 1,0 0,0 0,-1 0,0 0,0 1,-1 0,2 0,-2 0,0 0,0-1,-1 1,0 0,0 1,1 9,1 12,-2 0,-1 2,-1-2,-2 1,-1 0,-11 39,14-62,0-1,0 0,0 0,1 0,0 0,0 1,0-2,0 1,1 0,0 0,-1 0,2 1,-1-1,0 0,1-1,0 1,0-1,0 1,1-1,3 6,7 4,0 0,0-1,26 19,14 12,-39-29,-8-9,1 1,0 1,-2-1,1 0,0 0,-2 2,1-1,-1 0,0 1,0-1,-1 1,0 0,-1 0,3 12,-5-20,2 18,1-1,-3 1,0 0,-3 17,2-30,0 0,0-1,0 1,-1-1,1 1,-1 0,0-1,0 0,-1 1,-1-1,2 0,-1-1,-1 1,1-1,-1 1,0-1,0 0,0 0,0 0,-5 2,-13 5,1-3,-1 1,-1-1,1-2,-2 0,-39 3,-149-1,173-6,-20-2,14 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3893">3741 879,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5452.99">5526 155,'0'6,"0"0,0 1,0-1,-1 0,1-1,-1 0,-1 1,1 0,-5 7,4-10,0 0,-1-1,1 0,-1 0,1 0,-2 0,1 0,0-1,0 1,0 0,0-1,0 0,-1 0,1 0,-1 0,1 0,0-1,-2 1,-2-1,-105 10,-183-6,175-6,10 1,2-1,-119 13,211-10,2 0,-1 2,-1 0,1 1,-14 6,26-9,-1 1,0 0,1 0,0 0,0 0,-1 0,2 0,-1 1,0 0,1-2,0 2,-1 0,1 0,1 0,-2 1,1-1,1 0,-1 1,1-1,0 1,0-1,1 1,-2 5,2 2,-1 0,2 0,-1-1,1 1,1 0,0 0,1-1,0 0,1 1,0-1,0-1,1 1,1-1,0 1,0-2,2 1,-2-1,2 1,0-1,0-2,1 2,0-1,1-1,-1 0,1 0,0-1,1-1,-1 1,1-1,-1-1,2 1,-1-2,0 0,1 0,21 0,17-3,-23 0,53 3,-69 0,-2 0,2 0,0 0,-2 2,1-1,-1 0,0 1,16 9,-7 0,-1-1,-2 2,1 0,-1 0,0 2,-2 0,0 0,-1 2,10 17,-2 2,-1 1,-3 0,17 58,-32-91,5 13,-1-1,-1 2,-2-1,2 32,-4-46,0 0,0 0,-1 0,1 0,-1 0,0 0,0 0,-1-1,1 1,-1 0,0 0,0-1,0 1,0-1,-2 1,2-1,-1-1,0 1,0 0,0 0,-2-1,2 1,0-1,-1 0,0 0,0 0,-5 1,-21 6,0-2,0-1,0-1,-40 2,-130-3,154-4,28 0,-212-5,190 2,0-1,0-2,-64-17,80 14</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8362,24 +8490,24 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">241 478,'-1'-2,"1"0,0-1,-1 1,1-1,-1 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,0 1,-1 0,1-1,0 1,0 0,0 0,-1 1,1-1,0 0,-1 1,1 0,-1-1,1 1,-1 0,1 0,-4 1,0-1,0 0,0 0,0 1,0 0,0 0,1 0,-1 1,0 0,1 0,-1 0,1 1,0 0,0 0,-7 5,9-6,1 1,0-1,0 0,0 1,0-1,0 1,1 0,-1 0,1 0,0-1,0 1,0 0,0 1,0-1,1 0,-1 0,1 0,0 0,0 6,0-7,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 1,-1-1,1 0,0 0,0 1,0-2,1 1,-1 0,0 0,0 0,0-1,1 0,2 1,78 6,-62-6,-1 0,1 1,23 6,-22-2,0 1,0 2,-1 0,0 1,0 1,-1 0,22 19,-33-24,-1 1,0 1,0 0,-1 0,1 0,-2 1,1 0,-2 0,1 1,-1 0,0 0,-1 0,-1 0,1 1,-1-1,-1 1,1 13,-2-21,1 17,-1 1,-1-1,0 0,-6 37,5-52,-1 0,1 1,-1-1,0 0,-1 0,1 0,-1-1,0 1,0 0,0-1,-1 0,1 0,-1 0,0 0,0-1,0 1,-1-1,0 0,1 0,-1-1,0 1,-10 2,-14 4,0-2,-1-1,0-1,-40 1,-127-6,122-2,36 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1666.92">823 134,'41'89,"-3"2,-4 2,32 139,-33-76,16 216,-47-343,7 114,-9-122,-1-1,-1 1,-1-1,-9 36,11-52,-1 0,1 0,-1 1,0-1,0-1,-1 1,1 0,-1-1,-4 6,-9 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2913.92">1088 2,'124'-1,"135"3,-253-2,1 1,-1-1,0 1,1 0,-1 1,0 0,0 0,0 0,0 0,0 1,0 0,-1 1,7 4,-9-5,1 1,-1 0,0 1,0-1,-1 0,1 1,-1 0,0-1,0 1,-1 0,1 0,-1 0,0 0,0 0,-1 0,0 9,1 8,2 7,-2 0,-1 1,-1-1,-2 0,-8 40,8-63,1 0,-2-1,1 1,0-1,-1 0,0 0,0 0,-1-1,1 0,-1 1,-9 5,12-8,-1 0,0 0,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,-1-1,1 1,0-1,-1 1,1-1,0 0,-1 0,1 0,-1-1,1 1,0-1,-7-2,10 3,0 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,0-1,-1 1,1 0,-1 0,1-1,0 1,-1 0,1-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,17-10,26-1,-21 10,-1 1,0 1,0 1,0 1,0 1,29 7,-31-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3578.95">2517 504,'0'5,"0"19,0 15,0 14,0 2,0 6,0-3,0-3,0-6,0-6,0-7,0-5,0-2,0-3,-5-5,-1-2,0-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4183.92">2146 954,'4'0,"7"0,5 0,5 0,3 0,6 0,3 0,1 0,-2 0,3 0,0 0,4 0,3 0,4 0,-2 0,-3 0,-4 0,-9 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5121.92">3390 769,'28'-17,"0"-1,-1-1,-1-2,30-30,-49 46,-4 2,-1 0,1 1,0-1,0 1,1 0,-1 0,0 0,1 0,-1 1,1-1,-1 1,1 0,0 0,6 0,-8 1,0 0,1 1,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 1,-1 0,1-1,-1 1,0 0,0 0,0 0,0-1,0 1,0 0,0 0,-1 1,2 2,6 28,-1 0,-2 1,-1 0,-2 0,-3 65,0-41,-4 296,5-315</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5514.92">3866 1298,'4'0,"2"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6700.92">4713 822,'-109'-1,"-110"3,217-2,-1 0,0 0,0 0,0 1,0-1,0 1,0-1,0 1,1 0,-1 0,0 0,0 1,1-1,-1 1,1-1,0 1,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,1 1,-1-1,1 1,0-1,0 1,-1 0,2 0,-1-1,0 1,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,1 4,-1 1,1 0,0-1,1 0,0 1,0-1,0 0,1 0,0-1,1 1,-1-1,1 0,0 0,1-1,0 1,9 6,62 30,-57-33,-1 2,1 0,-1 1,-1 1,28 25,-34-24,0 0,-1 0,-1 1,0 1,-1 0,-1 0,0 0,-1 1,-1 0,-1 1,0-1,-2 1,0 0,0 0,-2 0,0 0,-4 34,3-49,0 1,-1-1,0 1,0-1,0 1,0-1,-1 0,1 0,-1 1,0-1,0 0,0-1,0 1,0 0,-1-1,1 1,-1-1,0 0,0 1,0-1,0-1,0 1,0 0,0-1,-1 0,1 1,0-1,-7 1,-9 1,0-1,0 0,0-1,-23-2,20 0,11 1,0-1,0 0,0-1,1 0,-1-1,0 0,1-1,0 0,0 0,0-1,0-1,1 1,-1-2,2 1,-16-15,-11-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7376.92">3390 346,'-3'2,"1"0,0 0,1 0,-1 0,0 0,1 1,-1-1,1 0,-1 1,1-1,0 1,0-1,0 1,1 0,-1-1,0 6,-1 0,-38 155,7-74,-49 155,72-205,1 1,2-1,2 1,0 56,6-78,0 0,2 0,0 0,1 0,1 0,0-1,1 0,1 0,1 0,1-1,18 28,7 0,1-2,63 58,-64-67</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8360.45">4898 637,'2'-1,"0"0,0-1,0 1,0 0,0 0,0 0,1 1,-1-1,0 0,1 1,-1 0,0-1,1 1,-1 0,0 0,1 0,-1 1,1-1,-1 0,0 1,1 0,-1-1,0 1,0 0,0 0,1 1,-1-1,2 2,5 2,-1 0,0 1,0 0,0 0,9 11,-2 2,-2 0,0 1,0 0,-2 1,-1 0,0 1,7 26,-2 5,17 105,-20-67,-4 0,-4 0,-16 183,9-251,-2-1,-1 1,-1-1,-1-1,0 0,-2 0,-22 36,9-23,-1-1,-2-1,-44 42,51-56</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10111.99">5983 451,'5'4,"0"0,0-1,1 0,-1 0,1 0,0 0,0-1,0 0,11 2,21 7,38 19,-2 2,-1 4,127 85,-191-114,0 1,-1 0,0 0,0 1,-1 0,0 0,0 1,8 17,-13-24,0 1,0 0,0 0,-1 0,0 0,0 1,0-1,0 0,0 1,-1-1,0 0,0 1,0-1,-1 0,1 1,-1-1,0 0,0 0,-1 0,1 0,-1 0,0 0,0 0,0 0,-1 0,-2 3,-29 21,27-22,0-1,0 1,0 1,0-1,-7 11,12-15,1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,1-1,0 0,-1 0,1 1,0-1,0 0,0 0,1 0,-1 1,0-1,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,2 3,17 21,38 42,-45-56,0 1,-2 0,0 0,0 2,-1-1,-1 1,0 0,-1 1,-1 0,10 34,-15-42,0 0,-1 0,0 0,0 1,-1-1,0 0,-1 0,0 0,0 1,-4 12,3-17,0 1,0-1,-1 1,1-1,-1 0,0 0,0-1,-1 1,1 0,-1-1,0 0,1 0,-2 0,1 0,0-1,0 0,-1 1,-8 1,-15 5,0-2,-1-2,0 0,0-2,0-1,0-1,0-2,0-1,-56-11,79 13,0-2,0 1,0-1,0 1,0-2,1 1,-1-1,1 1,-1-2,1 1,0-1,0 1,0-1,1-1,0 1,-1 0,2-1,-1 0,-5-9,1-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10618.97">6935 1298,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11865.98">7941 742,'-4'-2,"1"-1,-1 1,0-1,0 1,0 0,0 1,0-1,0 1,0 0,-1 0,1 0,-5 0,-59-2,42 3,-29-1,4 0,-64-9,110 9,0 1,0-1,1 1,-1 0,0 0,0 0,0 0,1 1,-1 0,0 0,1 0,-1 1,-4 2,6-3,0 2,0-1,1 0,-1 0,1 1,0-1,0 1,-1 0,2 0,-1 0,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,0 1,0 4,0 2,0 0,0 0,1 0,0 0,1 0,0 0,1-1,0 1,0 0,1 0,0-1,1 1,0-1,6 10,-6-12,0-1,1 0,0 0,0-1,0 1,1-1,-1 0,1 0,1-1,-1 0,0 0,1 0,0-1,0 0,0-1,0 1,0-1,1 0,10 0,81 0,-82-3,-1 0,0 1,1 1,-1 0,0 2,0 0,0 0,31 12,-37-11,-1 1,1 0,-1 0,0 1,-1 0,1 1,-1 0,-1 0,1 1,-1 0,-1 0,1 0,-1 1,-1 0,0 1,0-1,-1 1,0 0,0 0,-1 0,-1 0,1 0,-2 1,1-1,-2 20,1-19,0 0,-2 0,1 1,-1-1,-1 0,0 0,-1 0,0-1,-9 21,8-23,-1 0,0 0,-1-1,0 0,0 0,0-1,-1 0,0 0,0 0,-1-1,1 0,-15 7,3-4,0 0,0-1,0-1,-1-1,0 0,-32 2,-123-2,131-6,-146-2,150 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12728.97">5771 266,'0'760,"1"-730,1 0,2 0,1 0,2-1,1 0,0 0,3-1,0 0,2-1,22 35,-15-25,2-2,1 0,40 44,-38-52</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13727.97">9158 372,'15'423,"-4"93,-13-495,-1 1,0-1,-2 1,-1-1,0-1,-1 1,-1-1,-2 0,0-1,0 0,-2-1,-22 27,9-15,-2-1,-1-2,-1-1,-2-1,0-1,-39 21,32-25,-1-1,0-3,-77 22,95-32</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14215.97">9316 1139,'4'0,"11"0,17 0,11 0,12 0,5 0,-2 0,-7 0,-8 0,12 0,5 0,-3 0,-11 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14689">10401 637,'0'14,"0"26,0 25,0 19,0 9,0 34,0 4,0-16,0-18,0-22,0-18,0-15,0-10,0-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15913.97">11036 690,'-2'7,"0"-1,0 0,0 0,0-1,-1 1,0 0,0-1,-1 1,1-1,-1 0,-5 4,-1 4,-40 55,3 2,-40 81,73-121,0 0,2 1,1 0,1 0,2 1,2 1,0-1,-1 45,7-69,0 0,1 0,-1 0,1 0,1-1,0 1,0 0,0-1,1 0,0 1,0-1,1 0,0 0,8 10,-2-7,0-1,0 0,1 0,0-1,1 0,0-1,17 8,-21-11,5 3,1 0,1 0,-1-1,1-1,17 3,-27-7,0 0,0-1,-1 0,1 0,0 0,0-1,0 0,-1 0,1 0,0 0,-1-1,1 0,-1 1,0-2,1 1,-1-1,0 1,0-1,-1 0,1 0,3-4,15-19,-2-1,0-1,-2 0,28-60,-9 17,-26 51,-1-1,0 0,-2 0,0-1,-2-1,0 1,-1-1,-2 0,0 0,-1-45,-3 46,2-19,-3 0,-1 0,-14-63,16 101,0 1,0-1,0 0,-1 1,1-1,-1 0,1 1,-1 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,0 1,1 0,-1-1,0 1,-4-1,-5-1,-1 1,0 0,-26 0,27 1,-621 5,590-3,15-2,0 1,1 2,-1 1,1 1,0 1,-44 15,69-19,-1 0,1 1,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,1 0,-1 1,0-1,1 1,-1-1,1 1,0-1,0 1,0 0,0 0,0 0,1-1,-1 5,-4 17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">253 467,'-1'-2,"1"0,0-1,-1 1,1-1,-1 2,0-1,0-1,0 1,0 0,0 0,0 0,-2 0,2 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,0 1,-1 0,0-1,1 1,0 0,0 0,-1 1,1-1,0 0,-1 1,1 0,-2-1,2 1,-1 0,1 0,-4 1,-1-1,1 0,0 0,0 1,-1 0,1 0,1 0,-2 1,1 0,1 0,-1 0,0 1,1 0,0 0,-8 5,10-6,1 1,0-1,0 0,0 0,0 0,-1 1,2 0,-1 0,1 0,0-1,0 1,0 0,0 1,0-1,1 0,-1 0,1 0,0 0,0 5,0-6,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,2 0,-2-1,1 1,0-1,0 1,-1-1,1 0,0 0,0 1,0-2,2 1,-2-1,0 1,0 0,0-1,1 0,2 1,82 6,-64-6,-2 0,1 1,24 6,-23-2,0 1,0 1,-1 1,0 1,0 1,-1 0,23 18,-34-23,-2 1,1 0,-1 1,-1 0,2 0,-3 1,1-1,-1 1,0 1,-1 0,0 0,0-1,-2 1,1 1,-1-1,-1 0,1 14,-2-21,2 16,-2 2,-1-2,0 1,-7 36,6-51,-1-1,1 2,-1-1,0 0,-1 0,1 0,-2-1,1 1,0 0,0-2,-1 1,1 0,-2 0,1 0,0-1,0 1,-1-1,-1 0,2 0,-1-1,0 1,-11 1,-15 5,1-2,-1-1,-1-1,-41 1,-134-6,128-2,38 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1666.92">864 131,'43'87,"-3"2,-4 2,33 136,-34-75,16 212,-49-336,8 112,-10-120,-1 0,-1 0,-2 0,-8 35,11-52,-1 1,1 0,-2 1,1-1,0-1,-1 1,1 0,-1-1,-4 6,-10 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2913.92">1142 2,'131'-1,"140"3,-264-2,0 1,-1-1,1 1,0 0,-1 1,1 0,-1 0,0 0,1 0,-1 1,0 0,-1 0,8 5,-10-5,1 1,0 0,-1 1,0-1,-1 0,1 1,-1-1,0 0,0 1,-1 0,2 0,-2 0,0 0,0 0,-1 0,0 8,1 9,2 6,-2 0,-1 2,-1-2,-2 0,-9 40,9-62,1 0,-2-1,1 0,-1 0,0 0,0 0,0 0,-1-1,0 0,0 1,-10 4,13-7,-1 0,0 0,0 0,0-1,0 1,-1-1,1 1,0-1,0 0,0 0,-1-1,0 1,1-1,-1 1,1-1,0 0,-1 0,0 0,0-1,1 1,0-1,-8-2,11 3,0 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,0-1,-1 1,1 0,-1 0,1-1,0 1,-1 0,1-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1-1,1 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,18-9,27-2,-22 10,-1 1,0 1,0 1,0 1,0 1,31 7,-33-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3578.95">2643 493,'0'5,"0"18,0 15,0 14,0 2,0 5,0-2,0-3,0-6,0-6,0-7,0-5,0-2,0-2,-6-6,0-1,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4183.92">2253 932,'4'0,"8"0,5 0,5 0,3 0,6 0,4 0,1 0,-3 0,4 0,0 0,4 0,3 0,4 0,-2 0,-2 0,-6 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5121.92">3559 752,'30'-17,"-1"-1,0 0,-2-3,32-29,-52 46,-4 1,-1 0,1 1,1-1,-1 1,1 0,-1 0,0 0,1 0,0 1,0-1,-1 1,1 0,0 0,7 0,-9 1,0 0,1 1,-1-1,0 1,0 0,1 0,-1 0,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 1,-1 0,1-1,0 1,-1 0,0 0,0 0,0-1,0 1,0 0,0-1,-1 2,2 2,6 28,0-1,-3 1,-1 0,-2 0,-3 64,0-40,-4 289,5-308</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5514.92">4059 1269,'4'0,"3"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6700.92">4948 803,'-114'-1,"-116"3,228-2,-1 0,0 0,0 0,-1 1,1-1,0 1,0-1,0 1,1 0,-1 0,-1 0,1 1,1-1,-1 1,1-1,0 1,-1 0,1 0,-1 0,1 0,0 0,0 1,0-1,1 1,-1-1,1 1,0-1,0 0,-1 1,2 0,-1-1,0 1,1 0,-2 0,2 0,0 0,0 0,0 0,0 0,0 0,2 0,0 3,-1 2,1 0,0-1,1 0,0 1,0-2,0 1,2 0,-1-1,1 1,-1-1,2 0,-1-1,1 0,0 1,10 6,65 29,-60-32,-1 1,1 1,-1 1,-1 1,29 24,-35-24,-1 1,0 0,-2 0,1 2,-2 0,0-1,-1 1,-1 1,0-1,-2 2,0-2,-2 2,1 0,-1-1,-2 1,0-1,-4 34,3-48,0 1,-1-1,0 1,0-1,-1 1,1-1,-1 0,1 0,-1 1,0-2,0 1,0-1,0 1,0 0,-1-1,0 1,0-1,0 0,0 1,0-1,0-1,0 1,-1 0,1-1,-1 0,1 1,0-1,-8 1,-9 1,0-2,0 1,0-1,-24-2,21 0,12 1,-1-1,1 1,-1-2,2 0,-2-1,0 0,2-1,-1 0,1 0,-1-1,1-1,0 1,0-1,2 0,-18-15,-10-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7376.92">3559 338,'-3'2,"1"0,0 0,1 0,-1 0,0 0,1 1,-1-1,1 0,-2 1,2-1,0 1,0-1,0 0,1 1,-1-1,0 6,-1 0,-40 151,7-72,-51 152,76-201,0 1,3-1,2 1,0 55,6-76,0-1,2 1,0-1,1 1,1 0,1-2,0 1,1-1,2 1,0-1,19 27,8 0,1-2,66 56,-67-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8360.44">5143 623,'2'-1,"0"0,0-1,0 1,0 0,0 0,0 0,2 1,-2-1,0 0,1 1,-1 0,0-1,1 1,-1 0,0 0,2 0,-2 1,1-1,-1 0,0 1,1 0,-1-1,0 1,1 0,-1 0,1 1,-1-1,2 2,6 1,-2 1,0 1,1 0,-1 0,10 11,-2 1,-3 1,1 0,0 1,-3 0,0 1,-1 0,8 26,-2 5,17 102,-20-65,-5 0,-3 0,-18 179,10-245,-2-2,-2 2,0-2,-1 0,-1-1,-1 1,-24 34,10-21,-1-2,-3-1,-45 41,53-54</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10111.99">6282 441,'5'4,"0"0,1-1,0-1,-1 1,2 0,-1 0,0-1,0 0,12 2,22 7,40 18,-2 2,-2 5,134 82,-200-111,-1 1,0-1,-1 1,0 1,0 0,-1 0,0 0,9 18,-14-24,0 1,1 0,-1-1,-1 1,0 0,0 1,0-1,0 0,0 1,-1-1,0 0,0 1,0-2,-1 1,1 1,-1-1,0 0,0 0,-1 0,1 0,-2 0,1 0,0 0,0-1,-1 1,-2 3,-31 21,29-23,-1 0,1 1,0 1,-1-1,-6 10,12-14,0 0,1 0,0 0,0 0,0 0,1 0,-1 0,0 1,1-1,0 0,-1 0,1 1,0-1,0 0,0 0,1 0,-1 1,0-1,1 0,0-1,-1 1,1 0,0 0,0 0,0 0,1 0,1 3,18 20,40 42,-48-55,1 0,-3 1,1 0,0 1,-2 0,-1 1,1-1,-2 2,0 0,10 33,-16-42,0 1,-1 0,0 0,0 1,-1-2,0 1,-1 0,0 0,0 1,-5 11,4-16,0 1,0-1,-1 1,1-1,-1 0,0 0,-1-1,0 0,1 1,-1-1,0 0,1 0,-3 0,2 0,0-1,0 0,-2 1,-7 1,-17 5,1-3,-1-1,-1 0,1-2,-1-1,1-1,-1-2,1-1,-59-11,82 13,1-2,0 1,-1 0,1 0,0-2,1 1,-2-1,2 1,-1-2,0 1,1-1,0 1,0-1,1-1,-1 1,0 0,2 0,-1-1,-6-9,2-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10618.97">7282 1269,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11865.98">8338 725,'-4'-2,"0"-1,0 1,0-1,0 1,0 1,-1 0,1-1,0 1,0 0,-1 0,0 0,-4 0,-62-2,43 3,-30-1,5 0,-68-9,116 9,0 1,-1-1,2 1,-1 0,0 0,0 0,-1 0,2 1,-1 0,0 0,0 0,0 1,-4 2,6-3,-1 2,1-1,1 0,-1 0,1 1,0-1,0 0,-1 1,1 0,0 0,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,0 1,0 4,0 1,0 1,0 0,1 0,0-1,1 1,0 0,1-1,0 0,0 1,1 0,0-1,2 1,-1-2,6 11,-6-12,1-1,0 0,0-1,0 0,1 1,0-1,-1 0,2 0,0-1,-1 0,0 0,2-1,-1 0,0 0,1-1,-1 1,1-1,0 0,11 0,85 0,-86-3,-2 0,1 1,1 1,-1 0,0 2,-1 0,1 0,33 11,-40-10,0 1,0 0,0 0,-1 1,-1 0,2 1,-2-1,0 1,0 1,-1 0,0 0,0 0,-1 0,0 1,-1 1,0-1,-1 1,0-1,1 1,-2 0,-1 0,1-1,-2 2,1-1,-2 19,1-18,0 0,-2-1,1 2,-1-1,-1 0,0-1,-1 1,0-1,-10 20,9-22,-1 0,-1 0,0-1,0-1,-1 1,1-1,-1 0,-1 0,1 0,-1-1,0-1,-15 8,3-4,0 0,0-1,0-1,-1-2,0 1,-33 2,-130-2,138-6,-154-2,158 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12728.97">6059 260,'0'743,"1"-714,1 0,3 1,0-1,2-1,2 1,-1-1,4-1,-1 1,3-2,23 35,-16-25,2-2,1 0,42 44,-40-52</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13727.97">9616 364,'15'413,"-3"91,-14-483,-1 0,0 0,-3 0,0 0,0-2,-2 2,0-1,-3-1,1 0,-1-1,-1 0,-24 26,10-15,-2-1,-2-1,0-2,-3 0,1-2,-42 21,34-24,-1-2,0-2,-81 21,100-31</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14215.97">9782 1113,'4'0,"11"0,19 0,11 0,13 0,5 0,-2 0,-8 0,-7 0,11 0,6 0,-3 0,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14689">10921 623,'0'13,"0"26,0 25,0 18,0 9,0 33,0 4,0-16,0-17,0-21,0-19,0-14,0-9,0-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15913.97">11587 674,'-2'7,"0"-1,0 0,0 0,0-1,-1 1,0-1,0 0,-2 1,2-1,-1 0,-5 4,-2 3,-41 55,2 1,-41 80,76-119,0 1,3 0,0 0,2 0,1 2,3 0,0-1,-2 45,8-69,0 1,1 0,-1 0,2 0,0-2,0 2,0 0,0-1,1 0,0 1,0-2,2 1,-1 0,8 10,-1-7,-1-2,1 1,0 0,1-1,1 0,-1-2,19 9,-23-11,6 3,0 0,2-1,-1 0,1-1,17 3,-28-7,1 0,-1-1,-1 0,1 0,1 0,-1-1,0 0,-1 0,2 0,-1 0,-1-1,1 0,-1 1,1-2,0 1,-1-1,0 1,1 0,-2-1,1 0,3-4,16-19,-2 0,0-1,-2-1,30-58,-11 17,-26 49,-2 0,1-1,-3 1,1-2,-3 0,0 0,0 0,-3-1,0 1,-1-45,-3 46,2-19,-3 0,-1 0,-15-62,17 99,0 1,0-1,0 0,-1 1,1-1,-2 0,2 2,-1-1,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,-1 1,0-1,0 1,1 0,-1-1,0 1,-5-1,-4-1,-2 1,0 0,-26 0,27 1,-652 5,620-3,16-2,-1 1,2 2,-1 1,0 1,1 1,-47 14,73-18,-1 0,1 1,-1-1,1 1,0 0,-2 0,2 0,0 0,0 0,1 0,-1 1,0-1,1 1,-1-1,1 1,0-1,0 1,0 0,0 0,-1-1,2 0,-1 5,-4 17</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8491,7 +8619,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 27,'42'-2,"45"-8,20-1,-87 10,206-1,-222 2,0 0,-1 0,1 0,0 1,-1 0,1-1,0 1,-1 0,1 1,-1-1,1 1,-1-1,0 1,0 0,0 0,0 1,0-1,4 5,-4-2,-1-1,0 0,0 1,-1-1,1 1,-1 0,0-1,0 1,-1 0,0-1,1 1,-2 0,1 0,-1 5,1-8,-2 12,2 0,0 0,2 20,-1-29,0 1,0-1,1 0,0 0,0 0,0 0,1 0,0 0,0-1,0 1,0-1,6 5,-2 0,0 1,0-1,-1 1,0 0,-1 0,0 1,-1-1,0 1,0 0,-1 0,-1 1,2 18,-2-10,-1 0,-1 0,-1 0,0 0,-2-1,-7 32,8-46,0 0,-1 0,1 0,-1 0,0 0,0 0,-1-1,1 1,-1-1,0 0,0 0,0 0,-1-1,1 0,-1 1,0-2,0 1,0 0,0-1,0 0,-1 0,1-1,-1 0,1 0,-1 0,0 0,1-1,-1 0,-9-1,-4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="338.99">1032 504,'4'0,"2"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="338.98">1032 504,'4'0,"2"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8573,19 +8701,19 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 502,'-1'-21,"2"-1,1 0,0 0,2 0,6-22,-9 38,2 0,-1 0,0 0,1 1,0-1,0 0,1 1,0 0,0 0,0 0,0 0,1 1,-1 0,1 0,1 0,-1 0,0 1,1 0,-1 0,1 0,11-3,8 1,0 0,1 2,-1 0,30 2,105 10,-143-8,-6 0,-1 1,0 0,0 1,0 0,0 0,0 1,-1 1,0-1,0 2,0-1,0 1,-1 0,0 1,8 8,9 11,-2 2,34 52,-38-52,106 166,79 105,-197-289,4 4,1 0,23 21,-31-32,0 0,0 0,1 0,-1 0,1-1,-1 0,1 0,0 0,0 0,0-1,0 0,0 0,0 0,7-1,19-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="599.99">1403 0,'-4'1,"1"-1,-1 1,1 0,0 0,-1 0,1 0,0 0,0 1,0-1,0 1,0 0,0 0,0 0,1 0,-5 5,-2 0,-536 423,520-412,2 2,1 1,0 1,2 1,0 0,-31 51,17-22,-2-2,-57 63,71-89</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1863.99">1297 978,'2'-2,"0"-1,1 1,-1-1,1 1,0 0,0 0,0 0,0 0,0 0,0 1,1 0,-1-1,0 1,6-1,-7 3,0-1,0 1,-1 0,1-1,0 1,0 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 1,0-1,0 1,1-1,-1 1,0-1,0 1,-1 0,1 0,0-1,-1 1,1 0,-1 0,1 3,7 24,-2 1,-1-1,-1 1,-1 45,-1-34,9 62,-6-74,1 46,-5-52</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2323">1694 1005,'4'0,"2"5,0 14,-1 18,-2 21,-1 18,-1 1,0 1,-1-4,0-10,-1-16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3001">1641 1375,'-5'5,"-5"1,-6 4,-1 6,4 3,7-1,15-3,19-5,13-3,14-4,2-2,4-1,2-1,-7 1,-11-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3662.99">2303 1322,'1'-9,"0"0,1 0,0 0,0 0,1 0,0 1,7-12,4-14,143-364,-146 378,-10 20,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 1,4 46,-8 128,-30 195,11-147,14-130,-10 180,19-293</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4132">2779 952,'0'-4,"4"-2,7-4,5-1,5 2,7 3,18-12,14-3,5-1,6 2,0 0,1-1,6 3,-1 5,-4 0,-6 2,-15 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4598">2832 1270,'9'0,"12"0,11 0,10 0,24-9,14-3,13 1,-2 2,-7 2,-13-1,-14-1,-13 3,-9 1,-5 2,-9-3,-8-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5446.99">4393 1005,'-16'-51,"12"30,1 0,1 1,0-1,2 0,0 0,2 0,0 0,1 0,2 1,0-1,1 1,0 0,2 1,0 0,2 0,0 1,24-33,-29 44,6-9,0 2,1-1,1 2,26-24,-35 34,0 0,1 0,0 1,0-1,0 1,0 0,0 1,0-1,0 1,1 0,-1 0,1 0,-1 1,0 0,1 0,-1 1,1-1,-1 1,0 0,1 0,5 3,4 2,1 1,-1 1,0 0,-1 1,1 0,-2 1,0 1,0 0,-1 1,0 0,-1 1,0 0,-1 1,8 15,12 25,-2 2,31 86,-48-113,16 39,72 171,-99-238,25 41,-24-41,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,0 1,0-1,0 1,1-1,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,0 1,0-1,1 1,-1-1,2-1,16-15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5854.99">5187 555,'-5'0,"-10"5,-12 10,-19 16,-28 17,-12 8,-8 9,7-2,13-8,16-8,17-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7044.99">5425 1402,'0'-14,"-1"-12,2 0,6-37,-6 57,0 0,0 0,1 0,0 0,0 1,0-1,1 0,0 1,0 0,1 0,-1 0,1 0,0 0,0 1,9-8,-12 11,1 1,-1-1,0 0,0 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,1 0,-1 1,0-1,1 1,-1-1,0 1,0 0,1 0,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,-1 1,1-1,-1 0,1 1,-1 1,4 6,0 1,-1-1,0 1,2 19,0 31,-3 0,-3 0,-2 0,-3-1,-25 111,14-68,16-86</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7577">5398 926</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8757">5769 873,'4'0,"7"0,5 0,4 0,4 0,3 0,0 0,5 0,1 0,1 0,2 0,5 0,-1 0,-2 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 480,'-1'-20,"2"-1,1 0,0 0,2 0,7-21,-10 36,2 1,-1-1,0 0,1 1,0-1,0 1,2 0,-1 0,0 0,0 1,0-1,2 1,-2 0,1 0,1 1,-1-1,1 1,0 0,-1 0,1 0,12-3,8 2,0-1,1 2,-1 0,31 2,110 10,-149-8,-7 0,-1 1,1 0,-1 0,1 1,-1 0,1 1,-2 1,0-1,1 1,-1 0,0 1,0 0,-1 0,9 9,9 10,-2 1,35 51,-39-50,110 158,82 101,-204-276,3 3,2 1,23 19,-32-30,0 0,0 0,2 0,-2 0,1-1,-1 0,1-1,1 1,-1 0,0-1,0 0,0 0,1 0,6-1,20-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="599.99">1461 0,'-5'1,"2"-1,-1 1,1 0,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,0 1,0 0,0 0,1 0,-6 5,-1 0,-558 404,541-394,2 2,1 2,0 0,2 1,0 0,-32 48,18-20,-3-2,-59 60,75-85</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1863.99">1350 936,'2'-2,"0"-1,2 1,-2-1,1 1,0 1,0-1,0 0,0 0,0 0,1 1,0 0,-1-1,0 1,6-1,-7 3,0-1,1 1,-2 0,1-1,0 1,0 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 1,0-1,0 0,1 0,-1 1,0-1,1 1,-2 0,1 0,0-1,-1 1,1 0,-1 0,1 3,7 22,-2 2,-1-1,0 0,-2 44,-1-33,9 60,-6-71,2 44,-6-50</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2323">1764 962,'4'0,"2"5,0 13,-1 17,-1 21,-2 16,-1 2,0 1,-1-4,0-10,-1-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3001">1708 1316,'-5'5,"-5"0,-7 5,-1 5,5 3,7 0,15-4,20-4,14-4,14-3,2-2,5-1,2-1,-8 1,-11-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3662.99">2398 1265,'1'-8,"0"-1,1 0,0 1,0-1,1 0,0 2,8-12,3-14,150-348,-153 362,-10 19,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 1,5 44,-10 122,-30 187,11-140,15-125,-11 172,20-280</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4132">2893 911,'0'-4,"4"-2,8-3,4-2,6 3,7 2,19-11,15-3,4-1,7 2,0-1,1 0,6 3,0 5,-5-1,-7 3,-14 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4598">2948 1215,'10'0,"12"0,11 0,11 0,24-8,16-4,12 2,-1 1,-7 2,-14 0,-15-2,-13 3,-10 2,-5 1,-9-3,-8-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5446.99">4573 962,'-16'-49,"12"29,1 0,0 1,1-1,2-1,0 1,2 0,1 0,0 0,2 1,0-1,1 1,1 0,1 0,0 1,3 0,-1 1,25-32,-29 42,5-8,1 2,0-2,2 3,26-24,-36 33,0 1,2-1,-1 1,0-1,0 1,1 0,-1 1,0-1,0 1,1 0,0 0,0 0,-1 1,0 0,1 0,0 1,0-1,-1 1,0 0,2 0,4 3,5 2,0 1,0 0,0 1,-2 0,2 1,-3 1,1 0,-1 1,0 0,-1 1,0 0,-1 1,0 0,7 15,14 23,-3 3,32 82,-49-108,16 37,75 163,-103-227,26 40,-25-41,0 1,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,0 1,0-1,0 1,2-1,-2 0,0 1,1-1,-1 0,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,0 0,1 0,-1-1,0 1,0-1,1 1,-1-1,3-1,15-14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5854.99">5400 531,'-5'0,"-11"5,-12 9,-20 16,-29 16,-12 7,-9 10,7-3,14-7,17-8,17-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7044.99">5648 1342,'0'-14,"-1"-11,2 1,6-37,-6 55,0 1,0-1,1 0,0 1,1 0,-1-1,1 0,0 1,0 1,1-1,-1 0,1 0,1 1,-1 0,9-8,-12 11,1 1,-1-1,0 0,1 1,0-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,1 0,0 1,-1-1,1 1,-1-1,0 1,0 0,1 0,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,-1 1,1-1,-1 0,1 0,-1 2,5 6,-1 1,-1-2,0 2,2 17,0 31,-3-1,-3 1,-2-1,-3 0,-26 105,14-64,17-83</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7577">5620 886</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8757">6006 835,'4'0,"8"0,4 0,5 0,4 0,3 0,0 0,6 0,0 0,1 0,3 0,5 0,-2 0,-1 0,-9 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8669,16 +8797,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1034,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1022">530 267,'-53'47,"38"-34,0 0,1 1,-16 19,25-27,1 1,0-1,1 1,-1 0,1-1,1 2,-1-1,1 0,0 0,1 1,0-1,-1 11,2-13,0 0,0 0,0 0,1 0,0 0,0-1,0 1,0 0,1 0,0-1,-1 1,2-1,-1 0,1 1,-1-1,1 0,0 0,1-1,-1 1,0-1,6 5,5 0,-1 0,1-1,1 0,-1-1,20 5,30 15,-41-15,0 1,0 1,-2 2,35 28,-49-37,-1 0,1 1,-1 0,0 0,-1 1,0-1,0 1,0 0,-1 0,0 1,-1-1,0 1,0 0,-1 0,0 0,1 15,-3-17,0 1,0 0,0-1,-1 1,0-1,-1 1,1-1,-2 1,1-1,-1 0,0 0,-4 8,3-11,0 0,1 0,-1 0,-1 0,1-1,-1 1,1-1,-1 0,0-1,0 1,0-1,0 0,-1 0,1 0,0-1,-1 0,-7 1,-26 2,-67-1,65-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1679">1006 81,'18'14,"-1"0,0 1,-1 1,0 0,-1 1,-1 1,18 29,66 140,-97-185,23 52,-2 2,-3 0,-2 1,12 77,-17-53,-4 0,-5 130,-3-191,-2 37,-9 62,7-99,0-1,-1 0,-1 0,-1-1,0 1,-19 30,-19 12,24-40</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3294">1906 214,'-4'79,"-16"93,16-143,-18 93,10-56,-6 80,18 241,1-377,0 0,0 0,1 0,1-1,0 1,0 0,1-1,0 0,0 0,1 0,0-1,1 0,0 1,0-2,1 1,8 6,7 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5104">2303 425,'0'-1,"0"0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,1 1,-1 0,0 0,0-1,2 1,39-5,-36 5,24-3,0 2,0 1,56 7,-78-5,0 0,1 0,-1 0,0 1,0 1,0-1,-1 1,9 6,-12-7,-1 0,0-1,1 2,-1-1,-1 0,1 1,0-1,-1 1,0 0,0 0,0-1,0 2,0-1,-1 0,0 0,1 9,-1-10,-1 1,0-1,0 1,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,0 1,-1-1,1 0,-1 0,0 0,0 0,0 0,-1 0,1 0,-3 2,-7 5,0 0,-1 0,-20 10,22-13,0 0,0 0,-15 15,25-21,0 1,-1-1,1 1,0 0,0-1,0 1,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,-1 0,2 0,-1 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,1 1,1 0,8 8,0 0,1-1,0 0,15 8,-14-9,-10-6,29 18,-2 1,53 47,-75-61,-1 0,-1 0,0 0,0 1,0 0,-1 1,0-1,0 1,-1 0,-1 0,1 0,-1 0,-1 1,0-1,0 1,0 15,-2-21,-1-1,1 1,-1 0,0-1,0 1,0 0,-1-1,1 0,-1 1,0-1,0 0,0 0,0 0,-1 0,1 0,-1 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,-1-1,1 1,-1-1,1 0,-6 1,-10 3,0 0,0-2,-39 2,-112-5,126-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5491">3229 1034,'0'5,"0"1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6733">3943 399,'-52'-1,"33"-1,0 2,0 0,0 1,0 0,0 2,-28 7,43-8,0 1,0-1,0 1,0-1,0 1,1 1,0-1,-1 0,1 1,0-1,1 1,-1 0,1 0,-1 0,1 1,-3 7,-3 11,2-1,-6 28,7-27,4-17,-3 12,0 0,1 0,-1 28,4-41,0 0,0-1,1 1,-1-1,1 1,0 0,1-1,-1 0,1 1,0-1,0 0,0 0,0 0,1 0,0 0,-1 0,1-1,1 1,4 3,21 12,1-2,0 0,44 15,-42-19,0 1,-1 2,0 1,38 30,-61-41,-1 0,-1 0,1 1,-1 0,-1 0,1 0,-1 1,0 0,-1 0,0 0,0 1,-1-1,0 1,0 0,-1 0,0 0,-1 0,0 0,0 1,-1-1,-1 11,1-17,0 1,-1-1,0 1,1-1,-1 0,0 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,0 0,0-1,0 1,-1-1,1 1,-1-1,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,-1-1,-5 2,-7 0,1 0,-1-1,1-1,-29 0,38-1,-25-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7713.53">4419 240,'5'88,"4"0,3-1,29 101,-20-102,-3 1,-5 1,3 101,-16-186,1 42,-1 1,-3 0,-2 0,-12 53,13-86,0 0,-1-1,0 1,0-1,-2 0,1 0,-2 0,1-1,-2-1,1 1,-1-1,-1-1,0 1,0-2,-1 1,0-2,-1 1,-22 10,14-9,0-1,-1 0,1-2,-39 7,26-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9176.68">4525 2,'46'0,"-11"-2,1 2,-1 2,1 1,61 14,-89-15,0 0,-1 1,1-1,-1 2,0-1,0 1,0 0,-1 1,1-1,-1 1,0 1,-1-1,1 1,-1 0,0 0,0 0,-1 1,0 0,0 0,-1 0,1 0,-2 0,1 1,-1 0,0-1,-1 1,2 9,-3-10,0 1,0 0,0 0,-1 0,-1 0,1 0,-1-1,0 1,-1-1,0 1,0-1,-5 10,5-12,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,0 0,-1-1,1 0,-1 1,0-1,0-1,0 1,-1-1,1 0,-9 2,8-6,14-5,15-8,-16 12,1 1,-1 0,1 0,-1 0,1 1,-1 0,1 1,0 0,-1 0,1 1,0 0,-1 0,1 0,8 4,3 3,-1 0,0 1,32 22,24 13,-56-37,1 1,0-2,1-1,-1 0,37 3,103 0,-140-7,12-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9985.21">5716 849,'4'0,"6"0,7 0,12 0,7 0,6 0,5 0,-1 0,-4 0,-5 0,-3 0,-4 0,-2 0,-6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1013,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1022">546 261,'-54'46,"38"-33,1 0,0 1,-16 18,26-26,1 1,0-1,1 0,-1 1,1-1,1 2,-1-1,0 0,1 0,1 0,0 0,-1 11,2-13,0 0,0 0,0-1,1 1,0 0,0-1,0 1,0 0,1 0,1-1,-2 1,2-1,-1-1,1 2,-1-1,1 0,0 0,1-1,-1 1,0-1,7 5,4 0,-1-1,2 0,0 0,0-1,20 5,31 14,-42-14,-1 1,1 0,-2 3,35 27,-49-36,-2 0,1 1,-1 0,0 0,-1 0,1 0,-1 1,0 0,-1 0,0 1,-1-2,0 2,0 0,0 0,-1 0,1 14,-3-16,0 1,0 0,0-1,-1 0,0 0,-1 1,1-1,-3 1,2-1,-1-1,0 1,-4 8,3-11,0 0,1 0,-2 0,0 0,1-1,-1 0,1 0,-1 0,0-1,-1 1,1-1,0 0,-1 0,1 0,0-1,-2 0,-6 1,-27 2,-69-1,66-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1679">1037 79,'18'14,"0"0,0 0,-2 2,1 0,-2 0,-1 2,19 28,68 137,-100-181,24 51,-2 2,-4 0,-1 0,12 77,-18-53,-4 0,-4 128,-4-187,-2 35,-10 62,8-98,0 0,-1 0,-1-1,-2 0,1 1,-20 28,-19 13,24-39</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3294">1965 210,'-4'77,"-17"91,17-139,-19 90,11-54,-7 78,19 236,1-369,0-1,0 1,1 0,1-1,1 1,-1-1,1 0,0 0,0 0,1 0,0-2,1 1,1 1,-1-2,1 1,9 5,6 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5104">2374 416,'0'-1,"0"0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,1 0,-1 0,1 0,-1-1,2 1,40-5,-37 5,25-3,0 2,0 1,58 7,-81-5,0-1,1 1,0 0,-1 1,0 1,0-1,-1 1,10 6,-13-7,-1 0,0-1,1 2,0-1,-2 0,1 0,0 0,-1 1,0 0,0 0,0-1,0 2,0-1,-1 0,0 0,1 8,-1-9,-1 1,0-1,0 1,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,0 1,-1-1,1-1,-1 1,0 0,0 0,0 0,-1 0,1 0,-4 2,-6 5,0 0,-2-1,-20 11,23-13,0 0,-1 0,-15 14,26-20,0 1,-1-1,1 1,0 0,0-1,0 1,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1-1,0 1,0 0,-1 0,2 0,-1 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,2 1,0 0,8 7,0 1,2-1,-1 0,16 7,-15-8,-10-6,30 18,-2 0,55 47,-78-60,-1 0,-1 0,1-1,-1 2,0 0,-1 1,0-1,0 1,0-1,-2 1,1 0,-1 0,-1 1,0-2,0 2,0 15,-2-21,-1-1,1 0,-1 1,0-1,0 1,0 0,-1-1,1 0,-1 1,0-1,0 0,0 0,0 0,-1 0,0 0,0-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,-1-1,1 1,-2-1,2 0,-6 1,-11 3,1 0,-1-2,-40 2,-115-5,130-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5491">3328 1013,'0'4,"0"2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6733">4064 391,'-53'-1,"33"-1,1 2,-1 0,0 1,1 0,-1 2,-28 6,44-7,0 1,-1-1,1 1,0-1,0 1,1 1,0-1,-1 0,1 1,0-1,0 1,0 0,1 0,-1-1,1 2,-3 7,-3 11,2-2,-7 28,8-26,4-17,-3 11,0 1,1-1,-1 28,4-40,0 0,0-1,1 1,-1-1,1 1,0 0,1-1,-1 0,1 0,0 0,0 0,0 0,0 0,1 0,0 0,-1 0,1-1,2 1,3 3,22 11,1-1,0 0,45 14,-43-18,0 0,-1 3,0 1,39 29,-63-40,-1-1,-1 1,2 1,-2 0,-1 0,1 0,-1 1,0-1,0 1,-1 0,0 1,-1-1,0 0,0 1,-1 0,0 0,-1 0,0 0,0 0,-1 0,-1 11,1-17,0 1,-1-1,0 0,1 0,-1 0,0 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,0 0,0-1,0 1,-1-1,1 1,-2-1,1-1,1 1,-1 0,0 0,0 0,0-1,0 1,-1-1,-6 2,-6 0,0 0,0-1,1-1,-31 0,40-1,-26-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7713.53">4555 235,'5'86,"4"0,4 0,29 98,-20-100,-4 1,-4 1,2 99,-16-182,1 41,-1 1,-3 0,-2 0,-13 52,14-84,0 0,-1-1,0 0,0 0,-3 0,2 0,-2-1,1 0,-2-1,0 1,0-2,-1 0,-1 1,1-2,-1 1,-1-2,0 0,-23 11,14-9,1-1,-2-1,2-1,-41 7,27-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9176.68">4664 2,'48'0,"-12"-2,1 2,-1 2,1 1,63 14,-92-15,1-1,-2 2,1-1,-1 2,0-1,1 1,-1 0,-1 1,1-1,-1 1,1 1,-2-1,1 0,-1 1,0 0,0 0,0 1,-1 0,0 0,-1-1,1 1,-2 0,1 1,-1 0,0-1,-1 1,2 8,-3-9,0 1,0 0,0 0,-1-1,-1 1,1 0,-1-1,0 1,-1-1,0 0,0 0,-5 10,5-12,-1 0,0-1,1 0,-1 0,0 1,0-1,0 0,0 0,-2-1,2 0,-1 1,0-1,0-1,0 1,-1-1,0 0,-8 2,8-6,14-5,16-8,-17 12,1 1,-1 0,2 0,-2 0,1 1,-1 0,2 1,-1 0,-1 0,1 1,1 0,-2 0,1 0,8 4,4 3,-1 0,-1 1,34 21,24 13,-57-36,0 1,1-2,0-2,0 1,38 3,106 0,-145-7,13-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9985.21">5892 831,'4'0,"6"0,8 0,12 0,7 0,6 0,6 0,-2 0,-4 0,-5 0,-2 0,-6 0,-1 0,-6 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8843,11 +8971,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 421,'9'-10,"-1"-2,0 1,0-1,6-14,13-20,15-16,-21 28,1 2,1 0,2 2,2 0,31-27,-54 54,0 0,1-1,-1 2,1-1,-1 1,1-1,0 1,9-2,-13 4,1 0,-1 0,1-1,-1 1,1 1,-1-1,1 0,0 0,-1 0,0 1,1-1,-1 1,1-1,-1 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 1,1-1,0 1,-1-1,1 0,-1 1,1 2,6 28,-1 0,-1 0,-3 1,0 0,-4 46,1-21,-9 316,3-291,-3 0,-31 119,14-94,8-28,-34 89,43-148</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="550">848 1268</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2717">2303 24,'-2'4,"1"0,-1 0,0 0,0-1,0 1,-1-1,1 0,-1 1,1-1,-1 0,0-1,-4 4,-2 3,-28 25,-1-1,-2-2,-55 32,-49 39,99-64,2 3,1 1,3 2,1 2,3 2,-39 67,52-78,2 1,-28 77,42-96,1-1,0 2,2-1,0 0,1 1,1-1,1 1,4 32,-3-48,0 0,1 1,-1-1,1-1,0 1,0 0,1 0,-1-1,1 1,0-1,-1 0,2 0,-1 0,0 0,0 0,1-1,0 1,-1-1,1 0,5 2,12 5,1-1,35 9,-32-11,268 58,-290-63,1-1,-1 1,1-1,0 0,-1 0,1 0,-1 0,1-1,0 0,-1 1,1-1,-1-1,0 1,1 0,-1-1,0 1,0-1,0 0,0 0,3-3,-2 0,0 1,-1-1,1 0,-1 0,0 0,-1 0,1 0,-1-1,0 1,-1-1,2-8,1-9,-2 0,-1-1,0 1,-2 0,-5-30,6 49,-1 1,0-1,0 0,0 1,-1-1,1 1,-1-1,0 1,0 0,0-1,0 1,-1 0,1 0,-1 1,-4-5,1 3,-1-1,1 1,-1 0,0 1,0-1,-1 1,-7-2,-8 0,1 0,-1 1,0 2,-27 0,-87 3,112 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4197">2885 183,'-1'0,"1"0,-1 0,1-1,-1 1,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,1-1,-1 1,0 0,1-1,-1 1,1-1,14-25,-10 22,-1 1,1-1,0 1,0 0,0 1,1-1,-1 1,1 0,-1 0,1 1,0 0,-1 0,1 0,0 0,0 1,0 0,0 0,7 2,2 0,0 0,0 2,0 0,-1 0,27 12,-22-6,-1 2,0 0,0 0,-1 2,-1 0,0 1,-1 0,-1 2,0-1,-1 2,19 33,-18-25,-1 1,-1 0,-2 1,0 0,-2 1,-1 0,-2 0,3 32,-5-19,-1 1,-2 0,-2 0,-11 61,9-90,0-1,-2 1,1-1,-2 0,0-1,0 1,-1-1,-1-1,0 1,0-2,-1 1,-1-1,1-1,-18 12,-18 10,-2-2,-73 32,33-18,81-39,1 1,-1-1,0-1,0 1,0-1,0 0,-1-1,1 0,-1 0,1 0,-1-1,0 0,-12-1,19 0,0 0,-1-1,1 1,0-1,0 0,-1 1,1-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,0 0,0-1,-1 1,1 0,0-1,0 1,0-1,0 1,0 0,1-1,-1-1,15-50,5 5,26-47,-36 76,1 2,1 0,0 0,1 1,26-25,-32 36,-1 0,1 1,1-1,-1 1,0 0,1 1,0 0,0 0,0 1,0 0,0 0,1 1,-1 0,0 1,1-1,-1 2,0-1,1 1,-1 0,0 1,0 0,0 0,10 5,11 5,-1 1,0 1,0 2,41 31,-11-1,-3 3,63 69,-70-69,-40-40,1-1,1 0,-1 0,13 6,1-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6078">4896 103,'-104'-1,"-113"3,210-1,0 0,-1 1,1-1,0 2,0-1,1 1,-1 0,0 0,1 0,0 1,0 0,0 1,0-1,1 1,0 0,-7 9,-4 7,1 0,0 2,-13 28,3-3,8-20,2 1,-13 36,23-52,1 0,1 0,0 0,0 0,2 0,-1 1,2-1,0 14,0-25,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0-1,3 0,7 0,1-1,-1 0,0-1,23-6,4 0,-18 5,1 0,0 2,0 1,0 1,25 4,-35-3,0 2,1-1,-1 2,-1-1,1 2,-1-1,1 2,-2-1,1 2,11 9,0 2,-2 0,-1 1,0 0,-1 2,-1 0,21 39,-28-42,-1 0,-1 0,-1 1,-1 0,-1 0,0 0,-2 1,0 0,-1 30,-1-35,-1 0,-1-1,0 1,-2-1,1 1,-8 21,7-31,0 0,0-1,0 1,0-1,-1 0,0 0,0 0,0-1,-1 1,0-1,1 0,-1 0,-1-1,1 1,-1-1,1 0,-1-1,-10 4,-10 0,1-1,-1-1,0-1,0-1,0-1,0-2,0 0,1-2,-45-10,42 4,1 0,0-2,-50-28,-29-12,104 50,-1 0,0 0,1 0,-1-1,1 1,0-1,-1 1,1-1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,0 1,-2-5,-2-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 411,'9'-10,"0"-2,-1 2,0-2,7-13,13-20,15-16,-21 28,1 2,1 0,2 1,2 1,32-27,-56 53,0 0,2 0,-2 1,1-1,-1 1,1-1,1 1,8-2,-13 4,1 0,-1 0,1-1,-1 1,1 1,-1-1,1 0,1 0,-2 0,0 1,1-1,-1 1,1-1,-1 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 1,1-1,1 0,-2 0,1 0,-1 1,1 2,6 28,-1-1,-1 0,-3 1,0 0,-4 45,1-20,-9 308,3-284,-4 0,-31 116,14-91,8-28,-35 87,45-145</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="550">880 1237</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2717">2391 23,'-2'4,"1"0,-1 0,0 0,-1-1,1 1,-1-1,1 0,-1 1,1-1,-1-1,0 0,-5 4,-1 3,-29 24,-2-1,-1-1,-58 30,-50 39,102-63,2 3,2 1,2 2,2 2,2 1,-39 67,53-77,2 1,-29 75,44-93,1-2,0 3,1-2,1 1,1 0,1 0,1 0,4 32,-3-47,0 0,2 1,-2-1,1-1,0 1,0-1,1 1,-1-1,1 1,0-1,-1 0,2 0,0 0,-1 0,0 0,1-1,0 1,-1-1,1 0,6 1,11 6,2-1,36 9,-33-12,279 58,-302-62,1-1,-1 1,1-1,0 0,-1 0,2 0,-2 0,1-1,0 0,-1 1,1-1,-1-1,0 1,2 0,-2-1,0 1,0-1,0 0,0 0,3-3,-1 1,-1 0,-1-1,1 0,-1 0,0 0,-1 0,1 0,0-1,-1 2,-1-2,2-8,1-8,-2-1,-1 0,0 0,-2 1,-5-30,6 48,-1 1,0-1,0 1,0 0,-1-1,1 1,-2-1,1 1,0 0,0-1,0 1,-1 0,1 0,-1 1,-4-4,0 2,0-1,1 1,-1 0,-1 1,1-1,-1 1,-8-2,-8 0,1 1,0 0,-1 2,-28 0,-90 3,116 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4197">2995 179,'-1'0,"1"0,-1 0,1-1,-1 1,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,1-1,-1 1,0 0,1-1,-1 1,1-1,14-24,-9 21,-2 1,1-1,0 1,0 0,1 1,0-1,-1 1,1 0,-1 0,2 1,-1 0,-1 0,1 0,0 1,1 0,-1 0,0 0,8 1,1 1,1 0,-1 2,1 0,-2 0,29 12,-23-7,-2 3,1 0,0 0,-2 1,0 1,0 1,-2-1,0 3,-1-2,0 3,19 32,-18-25,-2 1,0 1,-3 0,0 0,-1 2,-2-1,-2 0,3 32,-5-19,0 1,-3 0,-3 0,-10 59,9-87,0-1,-3 0,2 0,-2 0,0-2,-1 2,0-1,-1-2,-1 2,1-2,-1 1,-2-2,2 0,-19 12,-19 9,-2-2,-75 32,33-18,85-38,1 1,-1-2,-1 0,1 1,0-1,-1 0,0-1,1 0,-1 0,0 0,0-1,0 0,-13-1,20 0,0 0,-1-1,1 1,0-1,0 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1-1,1 1,0 0,0-1,-1 1,1 1,0-2,0 1,0-1,0 1,0 0,1-1,-1-1,16-49,4 5,28-45,-37 73,0 2,1 1,1-1,0 2,28-25,-34 35,-1 0,2 1,0-1,-1 1,1 0,0 1,0 0,0 0,1 2,-1-1,0 0,2 1,-2 0,0 1,2-1,-2 2,0-1,2 1,-2 0,0 1,1 0,-1-1,11 6,11 5,-1 1,0 0,0 3,42 30,-10-1,-4 3,65 67,-72-67,-42-40,2 0,0 0,-1 0,14 5,1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6078">5083 101,'-108'-1,"-118"2,219 0,0 0,-1 1,0-1,1 2,0-1,1 1,-2 0,1 0,1 0,0 1,-1 0,1 1,0-1,1 0,-1 1,-6 9,-5 6,2 1,-1 1,-13 28,3-3,9-20,1 2,-13 34,24-50,1-1,0 1,1 0,0-1,2 1,-1 1,2-1,0 13,0-24,0 0,1 0,-1 0,0 0,1 0,-1 0,1-1,0 1,-1 0,1 0,0 0,0 0,1-1,0 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0-1,1 1,-1-1,0 1,0-1,3 0,7 0,2-1,-2 0,1-1,23-6,5 0,-20 5,2 0,0 2,0 1,0 1,26 4,-37-3,1 2,0-1,-1 2,0-1,0 2,0-1,0 1,-1 0,0 2,12 9,0 1,-3 1,0 0,0 1,-1 1,-2 1,23 37,-30-40,-1-1,0 1,-2 0,-1 1,-1-1,1 1,-3 0,0 1,-1 29,-1-35,-1 1,-1-1,0 0,-2 0,1 0,-9 21,8-30,0 0,0-1,0 1,0-1,-1 0,-1 0,1-1,0 0,-1 1,0-1,1 0,-2 0,0-1,1 1,-1-1,1 0,-2-1,-9 3,-11 1,1-1,-1-1,0-1,0-1,0-1,0-2,0 0,1-2,-47-10,44 5,1-1,0-2,-52-27,-30-12,108 49,-1 0,0 0,1 0,-1-1,1 1,-1-1,0 1,1 0,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,0 1,-3-5,-1-14</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8903,15 +9031,15 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">116 211,'-5'5,"-1"10,1 16,0 17,2 4,1 7,-13 11,-3-1,-4-9,3-9,3-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="482">10 317,'4'0,"7"0,5 0,5-4,7-2,5-4,4-5,1 0,-1 3,-3 3,-7 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="968.99">116 502,'4'0,"7"0,5 0,5 0,3 0,2 0,1 0,5 0,-3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1500.04">407 0,'9'5,"7"1,11 8,4 7,2 9,0 17,3 14,0 10,-6-2,-9 18,-7-1,-6-6,-5-12,-2-13,-7-12,-1-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2561">1042 211,'-3'31,"-1"-1,-1 1,-1-1,-2-1,-17 45,-15 61,29-61,4 2,3-1,7 101,-1-61,-3-49,-1-44,1-1,0 1,2 0,1 0,1-1,0 1,11 32,-9-45,0 0,1 0,1-1,-1 1,1-2,1 1,15 13,-15-14,10 8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3202.99">1069 529,'3'-2,"0"-1,1 1,0-1,-1 1,1 0,0 0,0 1,0-1,1 1,-1 0,0 0,8-1,57-1,-47 3,-2-1,-5 0,0 1,0 1,24 3,-34-3,0 0,0 1,0 0,-1 0,1 0,0 0,-1 1,0 0,0-1,0 2,0-1,0 0,0 1,5 6,0 3,-1 1,0-1,0 1,-2 1,1-1,-2 1,0 0,-1 1,4 29,-2 7,-4 87,-1-48,2-65,1-15,1-12,-1-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3676.02">1492 317,'0'5,"0"10,0 34,-9 23,-8 7,-14 13,-11 0,-2-6,1-14,8-15,10-16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4193">1571 899,'4'0,"2"5,0 6,-1 9,-2 7,-1 3,-1-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4976">1757 317,'1'0,"0"-1,0 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0 0,1 2,32 35,-34-38,12 17,-1 1,0 0,-2 1,0 1,-1-1,-1 1,-1 0,7 42,-3 13,1 82,-10-146,0 13,2 290,-6-273,-1 0,-3-1,-1 1,-1-2,-25 64,25-81</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">121 205,'-5'5,"-1"9,0 17,1 15,2 5,1 6,-14 11,-3-1,-3-8,2-10,3-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="482">10 308,'5'0,"6"0,6 0,5-4,7-2,5-3,5-6,1 0,-2 4,-2 2,-8 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="968.99">121 488,'4'0,"8"0,4 0,6 0,3 0,2 0,2 0,4 0,-3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1500.04">425 0,'9'5,"8"1,11 7,4 8,3 8,-1 17,4 13,-1 10,-6-2,-9 17,-7 0,-7-6,-5-12,-2-13,-7-11,-1-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2561">1087 205,'-3'30,"-1"-1,-2 1,0 0,-2-2,-18 44,-16 59,31-59,3 2,4-1,7 98,-1-60,-3-47,-1-42,1-2,0 2,2-1,1 0,1 0,0 0,12 32,-10-45,1 1,0 0,1-1,-1 0,2-1,0 1,16 12,-16-13,11 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3202.99">1115 514,'3'-2,"0"-1,2 1,-1-1,-1 1,1 0,0 1,0 0,1-1,0 1,-1 0,0 0,9-1,59-1,-49 3,-3-1,-4 0,0 1,-1 1,26 3,-36-3,0 0,1 1,-1 0,-1 0,1-1,1 1,-2 1,0 0,0-1,0 2,0-1,1 0,-1 1,5 6,0 2,0 2,-1-2,1 2,-3 1,1-2,-2 2,1-1,-2 2,4 28,-2 6,-4 85,-1-46,3-64,0-14,1-12,-1-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3676.02">1556 308,'0'5,"0"9,0 34,-9 22,-9 7,-14 12,-12 1,-2-7,1-13,9-14,10-17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4193">1639 874,'4'0,"2"4,0 7,0 9,-3 6,-1 3,-1-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4976">1833 308,'1'0,"0"-1,0 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,1 0,0 0,0 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 2,33 34,-35-37,13 16,-2 2,1-1,-3 2,0 0,0 0,-2 0,-1 0,8 42,-4 12,2 79,-11-141,0 12,2 282,-6-265,-1 0,-4-1,0 1,-1-2,-27 62,27-79</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8993,11 +9121,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 104,'0'-2,"1"0,-1 0,1 0,0 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,1 0,-1 1,1 0,-1-1,1 1,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,1 1,-1-1,0 1,3-1,2-1,1 1,-1 0,1 0,0 0,-1 1,11 1,-11 1,0 0,-1 1,0-1,1 2,-1-1,0 1,0-1,-1 2,1-1,-1 1,0 0,0 0,-1 0,1 0,-1 1,0 0,-1 0,1 0,4 13,2 4,-1 1,-1 0,-1 1,5 31,-9-27,0 0,-3 33,-1-41,1 1,1-1,1 0,1 1,10 37,8 4,2-2,3-1,3-1,57 88,-83-143,-1 0,1 0,0-1,0 0,0 0,0 0,1 0,-1 0,1 0,0-1,0 0,0 0,0 0,5 2,-6-4,-1 0,1 0,0 0,0 0,0 0,0 0,-1-1,1 0,0 1,0-1,-1 0,1 0,0-1,-1 1,1 0,-1-1,0 1,1-1,-1 0,0 0,0 0,0 0,3-4,22-29,-2 0,-1-2,-2 0,-1-2,16-44,8-51,-28 80,-2-2,-3 0,7-80,7-34,-9 63,-15 80</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1257.5">1165 898,'0'-3,"1"-1,0 0,1 1,-1-1,0 1,1-1,0 1,0 0,0-1,0 1,1 0,-1 1,1-1,0 0,0 1,0-1,0 1,0 0,0 0,0 0,5-1,12-8,1 2,24-8,-42 16,49-17,68-14,-102 28,0 1,1 1,-1 1,0 0,0 1,1 1,31 6,-43-4,0-1,-1 1,1 0,-1 0,1 1,-1 0,0 0,-1 0,1 1,-1 0,0 0,0 0,6 8,6 11,-2 0,15 30,14 22,-29-57,0-2,0 0,20 16,-12-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2103.51">2091 501,'-4'2,"0"1,0-1,0 1,0-1,1 1,-1 0,1 0,0 0,0 1,0-1,1 1,-1 0,-2 5,-2 0,-109 150,-102 125,177-240,15-17,2 1,-26 38,38-46</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2854.07">2515 236,'0'-4,"4"-2,6 1,16 0,11 6,4 3,23 5,4 1,-5-1,-8-2,-13-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3650.03">2594 633,'9'0,"7"0,10 0,10 5,26 1,6 4,1 1,-2-2,1 2,-7-1,-9-2,-9-2,-11 2,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 102,'0'-2,"1"0,-1 0,1 0,0 0,0 0,0 1,0-1,0 0,0 0,2 1,-2-1,1 0,-1 1,1 0,-1-1,1 1,0 1,0-1,0 0,1 0,-2 0,1 0,0 0,1 1,-1-1,0 1,4-1,1-1,1 1,0 0,0 0,1 0,-2 1,12 1,-11 1,-1 0,-1 1,1-1,0 2,0-2,-1 2,0-1,0 2,0-1,-1 1,0 0,1 0,-2 0,1 0,0 0,-1 1,-1 0,1 0,5 13,1 3,0 2,-2-1,0 2,4 30,-8-27,-1 0,-3 33,-1-40,1 0,1 0,1 0,1 0,11 37,8 4,2-3,4 0,3-1,60 86,-88-140,-1 0,1 0,0-1,0 0,1 0,-1 0,1-1,-1 1,1 0,1-1,-1 0,0 0,0 0,6 2,-7-4,-1 0,1 0,1 0,-1 0,0 0,0 0,-1-1,1 0,1 1,-1-1,-1 0,1 0,0-1,-1 1,1 0,0-1,-1 1,1-1,-1 0,0 0,0 0,0 1,4-5,22-29,-1 1,-2-2,-2 0,0-3,16-42,8-50,-29 78,-2-2,-3 0,7-78,8-34,-10 62,-16 79</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1257.5">1233 880,'0'-3,"1"-1,0 0,1 1,0-1,-1 1,1-1,0 1,0 0,0 0,0 0,1 0,-1 1,2-1,-1 0,0 1,0-1,0 1,1 0,-1 0,0 0,5-1,14-8,0 3,25-9,-43 16,51-17,72-13,-108 27,0 1,1 1,-1 1,0 0,0 1,1 1,33 6,-45-4,-1-1,-1 1,2 0,-2 0,1 1,0 0,-1-1,-1 1,2 1,-2 0,0 0,1 0,5 8,7 10,-2 1,16 29,15 21,-32-55,1-3,0 1,21 15,-12-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2103.51">2214 491,'-5'2,"1"1,0-1,0 1,-1-1,2 1,-1 0,1-1,0 1,-1 1,1-1,1 1,-1 0,-2 5,-3 0,-115 147,-107 122,186-235,17-17,1 2,-27 36,41-44</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2854.07">2662 231,'0'-4,"5"-2,5 2,18-1,11 6,4 3,25 4,4 2,-5-1,-9-2,-14-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3650.03">2746 620,'10'0,"7"0,10 0,11 5,28 1,6 4,1 1,-2-3,1 3,-8-1,-9-2,-9-2,-12 2,-13-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9222,15 +9350,15 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">33 344,'4'5,"7"1,0 4,0 10,1 14,0 6,-3 11,-3-1,-3-2,-1-7,-1-4,-1-5,0-3,-1-2,5-6,6-15,1-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="673.04">33 158,'13'0,"23"0,19 0,18 0,5 0,3 0,-7 0,-17 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1218.99">86 450,'4'0,"7"0,14 0,8 0,7 0,1 0,-1 0,-4 0,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2014">907 0,'-10'17,"6"-3,-81 191,-54 156,129-327,-1 1,1 1,2 1,-7 68,14-95,1 0,1 0,-1 0,1 0,1 0,0 0,1-1,-1 1,2-1,-1 1,1-1,1 0,0-1,0 1,1-1,0 0,0 0,1-1,10 10,4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3116">933 608,'0'-14,"-1"-31,8-50,-5 79,1 0,1 0,1 0,0 0,1 1,12-23,-14 31,0 0,1 0,0 1,1 0,-1 0,1 0,0 0,1 1,-1 0,1 1,0-1,0 1,0 1,1-1,0 1,-1 0,1 1,0 0,0 0,0 1,0 0,1 0,-1 1,0 0,0 1,0-1,0 2,0-1,0 1,0 0,0 1,0 0,-1 0,1 0,-1 1,0 0,0 1,0 0,-1 0,0 0,0 1,6 6,11 18,-1 2,-1 0,-2 1,-1 1,-2 1,-1 0,17 64,-7-24,-22-69,0 0,0 0,0-1,1 1,-1-1,1 0,0 0,1 0,8 8,3-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3714">1595 317,'-5'0,"-5"0,-7 0,-4 0,2 5,-1 6,-2 5,-5 14,-4 6,0 6,-8 9,1 1,4-9,7-7,4-10,6-4,6-2,4-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4184.99">1780 688,'0'5,"0"5,0 6,0 14,0 10,-5 4,-1-2,0-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4934">1806 106,'11'1,"0"1,0 0,0 0,0 1,0 1,0 0,-1 0,0 1,0 0,0 1,0 0,-1 0,0 1,0 1,-1-1,0 1,-1 1,10 11,-1 1,-1 1,-1 0,-1 1,-1 0,-1 1,15 47,-13-20,-2 0,-3 0,2 61,-7 158,-4-222,0-33,0-1,0 1,-2-1,0 0,0 0,-2 0,1 0,-2-1,0 1,0-1,-11 14,11-17,-1-2,0 1,-1-1,1 0,-2 0,1-1,-1 0,0-1,0 0,-1 0,0-1,0 0,0-1,0 0,-14 3,0-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5673.99">7 1270,'-5'0,"4"0,37 0,31 0,27 0,32 0,23 0,21 0,14 0,12 0,-6 0,-3 0,-16 0,-23 0,-32 0,-36 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">34 333,'4'5,"8"1,-1 3,1 11,0 12,1 7,-4 11,-3-2,-3-2,-1-6,0-4,-2-5,0-3,-2-2,7-6,5-14,1-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="673.04">34 153,'14'0,"23"0,20 0,19 0,5 0,4 0,-9 0,-16 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1218.99">89 435,'5'0,"6"0,15 0,8 0,8 0,0 0,0 0,-5 0,-7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2014">943 0,'-11'16,"7"-2,-84 184,-57 152,135-317,-1 0,0 2,3 1,-8 66,15-93,1 1,1 0,-1-1,1 1,1 0,0-1,2 0,-2 1,2-1,-1 0,1 0,1 0,0-2,1 2,0-1,0 0,0-1,2 0,9 10,5-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3116">970 588,'0'-13,"-1"-31,8-48,-5 77,1-1,1 1,2-1,-1 1,1 0,13-21,-15 29,0 0,1 0,0 1,2 1,-2-1,1 0,0 0,2 1,-2 1,1 0,0-1,1 1,-1 1,1-1,1 1,-2 0,1 1,1 1,-1-1,0 1,0 0,2 0,-2 1,0 0,1 1,-1-1,0 2,1-1,-1 1,0-1,1 2,-1 0,-1 0,2 0,-2 1,0 0,0 1,1-1,-2 1,0 0,0 1,7 6,11 17,-1 2,-2 0,-1 0,-1 2,-2 1,-2 0,18 62,-7-24,-22-66,-1 0,0 0,0-1,1 1,-1-2,1 1,0 0,2 0,7 7,4-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3714">1658 307,'-5'0,"-6"0,-6 0,-5 0,2 5,-1 5,-2 6,-5 13,-4 6,0 5,-9 10,2 0,4-8,6-8,6-9,5-3,6-3,5-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4184.99">1850 666,'0'5,"0"4,0 7,0 13,0 9,-5 5,-1-2,0-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4934">1877 103,'12'1,"-1"0,1 1,-1 0,0 1,1 1,-1 0,0 0,-1 1,1 0,-1 0,0 1,0 0,-1 1,0 0,0 0,-1 1,-1 1,11 10,-1 1,-2 2,0-1,-2 1,0 0,-2 2,16 44,-13-18,-3-1,-3 0,3 60,-8 152,-4-214,0-33,0 0,0 0,-2 0,0-1,-1 1,-1-1,1 1,-2-2,0 2,-1-1,-10 13,10-17,0-1,0 1,-1-1,0-1,-1 1,1-1,-2 0,1-2,0 1,-2 0,1-1,-1 0,1-1,0-1,-15 4,0-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5673.99">7 1229,'-5'0,"4"0,38 0,33 0,28 0,33 0,24 0,21 0,16 0,11 0,-5 0,-4 0,-16 0,-24 0,-34 0,-36 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9367,7 +9495,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">117 1,'2'0,"1"1,-1-1,0 1,1 0,-1 0,0 0,0 0,1 0,-1 1,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,-1 1,1-1,-1 4,4 12,-1 0,0 34,-2-41,0 278,-2-146,1-115</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="856.84">0 501,'5'0,"7"0,6 0,4 0,5 0,7 0,8 0,2 0,-7 5,-5 2,-2-1,-2-1,0-1,-5-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="856.83">0 501,'5'0,"7"0,6 0,4 0,5 0,7 0,8 0,2 0,-7 5,-5 2,-2-1,-2-1,0-1,-5-2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9700,11 +9828,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1959046-2DC6-4331-8086-8723FFDB0E43}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="H17" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9719,7 +9847,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9730,17 +9858,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAF04F6-4A68-4264-A965-ED4BAF59DEE2}">
   <dimension ref="I1:Q35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="16" max="18" width="5.5703125" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" customWidth="1"/>
+    <col min="16" max="18" width="5.5546875" customWidth="1"/>
+    <col min="19" max="19" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I1" t="s">
         <v>11</v>
       </c>
@@ -9757,7 +9885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I2" t="s">
         <v>0</v>
       </c>
@@ -9765,19 +9893,19 @@
         <v>1.5</v>
       </c>
       <c r="K2">
-        <f>J11</f>
+        <f t="shared" ref="K2:M3" si="0">J11</f>
         <v>2.0360288230584467</v>
       </c>
       <c r="L2">
-        <f>K11</f>
+        <f t="shared" si="0"/>
         <v>1.9987006090558244</v>
       </c>
       <c r="M2">
-        <f>L11</f>
+        <f t="shared" si="0"/>
         <v>1.9999999838762601</v>
       </c>
     </row>
-    <row r="3" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
         <v>1</v>
       </c>
@@ -9785,19 +9913,19 @@
         <v>3.5</v>
       </c>
       <c r="K3">
-        <f>J12</f>
+        <f t="shared" si="0"/>
         <v>2.8438751000800639</v>
       </c>
       <c r="L3">
-        <f>K12</f>
+        <f t="shared" si="0"/>
         <v>3.002288562924508</v>
       </c>
       <c r="M3">
-        <f>L12</f>
+        <f t="shared" si="0"/>
         <v>2.9999994133889132</v>
       </c>
     </row>
-    <row r="4" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>2</v>
       </c>
@@ -9818,7 +9946,7 @@
         <v>-1.2860883433774006E-6</v>
       </c>
     </row>
-    <row r="5" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
         <v>3</v>
       </c>
@@ -9839,7 +9967,7 @@
         <v>-2.2139948953281419E-5</v>
       </c>
     </row>
-    <row r="6" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I6" t="s">
         <v>4</v>
       </c>
@@ -9860,7 +9988,7 @@
         <v>6.9999993811414338</v>
       </c>
     </row>
-    <row r="7" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I7" t="s">
         <v>5</v>
       </c>
@@ -9881,7 +10009,7 @@
         <v>1.9999999838762601</v>
       </c>
     </row>
-    <row r="8" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
         <v>6</v>
       </c>
@@ -9902,7 +10030,7 @@
         <v>26.999989441001471</v>
       </c>
     </row>
-    <row r="9" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
         <v>7</v>
       </c>
@@ -9923,7 +10051,7 @@
         <v>36.999992670439696</v>
       </c>
     </row>
-    <row r="10" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
         <v>10</v>
       </c>
@@ -9944,7 +10072,7 @@
         <v>204.99994734865331</v>
       </c>
     </row>
-    <row r="11" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I11" t="s">
         <v>8</v>
       </c>
@@ -9965,7 +10093,7 @@
         <v>1.99999999999998</v>
       </c>
     </row>
-    <row r="12" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I12" t="s">
         <v>9</v>
       </c>
@@ -9986,7 +10114,7 @@
         <v>3.0000000000000751</v>
       </c>
     </row>
-    <row r="13" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
         <v>12</v>
       </c>
@@ -9995,15 +10123,15 @@
         <v>26.327172630751079</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:M13" si="0">(L2-K2)/L2*100</f>
+        <f t="shared" ref="L13:M13" si="1">(L2-K2)/L2*100</f>
         <v>-1.8676240870440306</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4968741545556499E-2</v>
       </c>
     </row>
-    <row r="34" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P34" t="s">
         <v>15</v>
       </c>
@@ -10011,7 +10139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N35" t="s">
         <v>13</v>
       </c>
@@ -10033,20 +10161,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE744686-E7BF-4051-8C38-1ED889B4DB33}">
-  <dimension ref="A3:J21"/>
+  <dimension ref="A3:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="A19:D21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="1.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>19</v>
       </c>
@@ -10054,7 +10185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>24</v>
       </c>
@@ -10062,7 +10193,64 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="K6" s="5">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>7.0033300000000001</v>
+      </c>
+      <c r="K8" s="5">
+        <v>-0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <f>10.02+0.19/7.0033*-0.29333</f>
+        <v>10.012041937372381</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>21</v>
       </c>
@@ -10073,18 +10261,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E12">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E12" s="5">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>7.0033300000000001</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>-0.29899999999999999</v>
       </c>
+      <c r="J12">
+        <f>-0.19-0.19/7.00333*7.00333</f>
+        <v>-0.38</v>
+      </c>
     </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>26</v>
       </c>
@@ -10095,78 +10287,242 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E14">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="5">
         <v>0</v>
       </c>
-      <c r="F14" s="1">
-        <f>-0.2-0.3/3*-0.1</f>
+      <c r="F14" s="6">
         <v>-0.19</v>
       </c>
-      <c r="G14">
-        <f>10-0.3/3*-0.2</f>
+      <c r="G14" s="5">
         <v>10.02</v>
       </c>
-      <c r="I14" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" t="s">
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E15">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E16" s="5">
         <v>0</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="5">
         <v>0</v>
       </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="G16">
+      <c r="G16" s="5">
         <f>10.02+0.19/7.0033*-0.29333</f>
         <v>10.012041937372381</v>
       </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="2">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="2">
         <f>0.1/3</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <f>0.3/3</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="2">
         <f>-0.19/7.00333</f>
         <v>-2.712995103757784E-2</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5874FDE-3A89-4775-B935-89301D48D7A2}">
+  <dimension ref="B2:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H2" s="5">
+        <v>2.04</v>
+      </c>
+      <c r="I2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1.55</v>
+      </c>
+      <c r="J3" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1.395</v>
+      </c>
+      <c r="K4" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I5" s="6">
+        <f>-0.645-(-0.645/1.55)*1.55</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1.323</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J6" s="5">
+        <f>-0.717-(-0.717/1.395)*1.395</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>2.04</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10">
+        <v>1.55</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>1.395</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>1.323</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19">
+        <f>-0.49/2.04</f>
+        <v>-0.24019607843137253</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20">
+        <f>-0.645/1.55</f>
+        <v>-0.41612903225806452</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <f>-0.717/1.395</f>
+        <v>-0.51397849462365586</v>
+      </c>
+      <c r="K21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se les coloco nombre a las pestañas
</commit_message>
<xml_diff>
--- a/Excel/Clase 24-abr-2021.xlsx
+++ b/Excel/Clase 24-abr-2021.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clases-octave\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943B8472-6C16-4E1A-91D3-AC8BD050916E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EE07C3-201F-4249-A7CF-CA7D83E3847C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C23CBDC8-AF82-4E14-AFB7-38945A7880BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C23CBDC8-AF82-4E14-AFB7-38945A7880BB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Newtom_Raphson_Formulas" sheetId="1" r:id="rId1"/>
+    <sheet name="Newtom_Raphson_Formulas2" sheetId="2" r:id="rId2"/>
     <sheet name="Newtom-Raphson" sheetId="3" r:id="rId3"/>
     <sheet name="Descomposicion LU" sheetId="4" r:id="rId4"/>
-    <sheet name="Gauss-Seidel" sheetId="5" r:id="rId5"/>
+    <sheet name="Thomas-LU" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja3" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Xi</t>
   </si>
@@ -162,6 +164,9 @@
   <si>
     <t>-0.717-(-0.717/1.395)*1.395</t>
   </si>
+  <si>
+    <t xml:space="preserve">Paginas 242 para la descomposicion LU y para lo de cholesky </t>
+  </si>
 </sst>
 </file>
 
@@ -6646,6 +6651,861 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>570360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>505320</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="15" name="Entrada de lápiz 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D7CDA4-6C01-4BC0-9A10-C25CC62FAE29}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2155320" y="510120"/>
+            <a:ext cx="1519920" cy="1832040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="15" name="Entrada de lápiz 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D7CDA4-6C01-4BC0-9A10-C25CC62FAE29}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2137320" y="492483"/>
+              <a:ext cx="1555560" cy="1867673"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>713760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>75960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>84240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33480</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="22" name="Entrada de lápiz 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDA851F-3F99-4F1F-9BC4-1310CDCFD571}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1506240" y="624600"/>
+            <a:ext cx="3332880" cy="2152080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Entrada de lápiz 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDA851F-3F99-4F1F-9BC4-1310CDCFD571}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1488242" y="606600"/>
+              <a:ext cx="3368516" cy="2187720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>677880</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106440</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>90360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="31" name="Entrada de lápiz 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1A71F5-7D07-4743-9A0C-3C53D1756AB8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6225240" y="1386360"/>
+            <a:ext cx="221040" cy="167040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="31" name="Entrada de lápiz 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1A71F5-7D07-4743-9A0C-3C53D1756AB8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6207240" y="1368360"/>
+              <a:ext cx="256680" cy="202680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>562560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>45360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>249480</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="52" name="Entrada de lápiz 51">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166F04E1-4705-41BF-B2BF-4409C958E3B4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6902400" y="776880"/>
+            <a:ext cx="1271880" cy="1120680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="52" name="Entrada de lápiz 51">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166F04E1-4705-41BF-B2BF-4409C958E3B4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6884400" y="759240"/>
+              <a:ext cx="1307520" cy="1156320"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533280</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>98640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>544440</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="54" name="Entrada de lápiz 53">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE48DAB-C4B6-48D8-8FF1-4D784C3A2D86}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7665600" y="1195920"/>
+            <a:ext cx="11160" cy="72720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="54" name="Entrada de lápiz 53">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE48DAB-C4B6-48D8-8FF1-4D784C3A2D86}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7647600" y="1177920"/>
+              <a:ext cx="46800" cy="108360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>387360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>396000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="63" name="Entrada de lápiz 62">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C07E3AE-BB2D-42A0-983E-17097D434991}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6727200" y="563400"/>
+            <a:ext cx="2386080" cy="1571760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="63" name="Entrada de lápiz 62">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C07E3AE-BB2D-42A0-983E-17097D434991}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6709203" y="545760"/>
+              <a:ext cx="2421715" cy="1607400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>456960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>679800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139320</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="66" name="Entrada de lápiz 65">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA0C3243-25C9-43AF-BCD1-9B832159C8AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9966720" y="1226520"/>
+            <a:ext cx="222840" cy="375840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="66" name="Entrada de lápiz 65">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA0C3243-25C9-43AF-BCD1-9B832159C8AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9948720" y="1208520"/>
+              <a:ext cx="258480" cy="411480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>752400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>151920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>764400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>169920</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="82" name="Entrada de lápiz 81">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF912C4A-0A63-46AA-AA6E-4AECDF7C7B81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11054640" y="517680"/>
+            <a:ext cx="1596960" cy="1298160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="82" name="Entrada de lápiz 81">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF912C4A-0A63-46AA-AA6E-4AECDF7C7B81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11036996" y="500040"/>
+              <a:ext cx="1632608" cy="1333800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>508680</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>83520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>608040</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>122760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="91" name="Entrada de lápiz 90">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CD7FE0-716B-4DDB-9611-27D50BD60475}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10810920" y="449280"/>
+            <a:ext cx="2476800" cy="1502280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="91" name="Entrada de lápiz 90">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CD7FE0-716B-4DDB-9611-27D50BD60475}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10793277" y="431640"/>
+              <a:ext cx="2512445" cy="1537920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>792360</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>174960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>623760</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>16200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="98" name="Entrada de lápiz 97">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FE508A3-2C92-4BE9-99D7-A9353D23BACE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13472040" y="906480"/>
+            <a:ext cx="623880" cy="572760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="98" name="Entrada de lápiz 97">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FE508A3-2C92-4BE9-99D7-A9353D23BACE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13454040" y="888480"/>
+              <a:ext cx="659520" cy="608400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7320</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>129240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60480</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="106" name="Entrada de lápiz 105">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5145C6EC-08DA-4DD6-8FAD-0134DC859186}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7139640" y="677880"/>
+            <a:ext cx="360" cy="114120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="106" name="Entrada de lápiz 105">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5145C6EC-08DA-4DD6-8FAD-0134DC859186}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7121640" y="659880"/>
+              <a:ext cx="36000" cy="149760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>174960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>151800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="113" name="Entrada de lápiz 112">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B2F2A3-596C-4B5B-B0EB-A8ADAD87ABD8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="640080" y="174960"/>
+            <a:ext cx="304200" cy="704160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="113" name="Entrada de lápiz 112">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B2F2A3-596C-4B5B-B0EB-A8ADAD87ABD8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="622440" y="157320"/>
+              <a:ext cx="339840" cy="739800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>327480</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>327840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7560</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98100FA-C6CF-4132-9E7B-3016FA2176C6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1119960" y="555840"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98100FA-C6CF-4132-9E7B-3016FA2176C6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1101960" y="538200"/>
+              <a:ext cx="36000" cy="36000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -6700,6 +7560,274 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink100.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:55:28.951"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1,'0'3,"0"6,0 4,0 3,0 4,0 0,4-1,1-2,-1 0,0 2,-2 0,4-3,-1-4</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink101.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:55:37.800"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4321 488,'1'10,"0"0,1 0,0 0,0 0,7 15,-3-5,129 330,29-9,76 180,-161-306,52 227,-97-295,-7 2,12 237,-38 366,-6-296,5-432</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="949.91">87 1,'-8'171,"0"-42,5-45,-28 584,-6 192,38 2,1-332,-2-482,2-1,1 0,3 0,2 0,2 0,31 88,137 228,-134-280,-30-56,1 2,1-1,31 43,-46-69,1 0,0-1,0 1,-1-1,1 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0-1,5 2,16 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1599.88">5612 2478,'0'7,"4"6,8 15,13 21,16 17,6 7,12 6,7 4,3-1,1-8,-9-9,-6-11,-10-13,-9-12,-10-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2112.62">6120 2541,'0'0,"-1"0,1 0,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,1-1,0 0,-1 1,1-1,0 1,-1-1,1 1,0-1,-1 1,1 0,0-1,0 2,-5 19,4-15,-16 64,-4-1,-53 120,22-61,-9 32,61-160,-1 1,1-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,1 1,-1 0,0-1,0 0,1 1,-1-1,0 1,1-1,0 1,17 1,3-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2648.24">6628 2880,'0'3,"0"9,0 13,0 9,-3 10,-2 12,-3 7,0 0,-3 0,0-3,3-9,2-8,3-13</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink102.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:55:48.887"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">212 1,'0'14,"0"23,0 23,0 20,0 10,0 8,0 5,4 0,8-4,5-7,1-13,0-12,1-18,-3-13,0-13,-4-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="530.16">0 763,'12'-5,"0"2,0 0,1 0,-1 1,1 0,-1 1,19 1,-6 0,294-3,-187 4,-107-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink103.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:55:52.708"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">301 319,'-4'4,"1"1,-1 1,1-1,0 1,0-1,-3 10,-8 17,12-29,-61 106,-50 116,97-187,2 1,1 0,2 2,2-1,2 1,1 0,1 47,4-42,2 0,3 0,1-1,2 1,23 74,144 281,-110-267,7 36,84 305,-140-417,-3 0,-3 1,-2 0,-3 1,-2-1,-3 1,-3-1,-13 74,13-114,0 1,-2-1,0 0,-1 0,-1-1,-1 0,0 0,-18 24,21-34,0 0,-1-1,0 0,0-1,0 1,-1-1,0-1,0 1,0-1,-1-1,1 1,-1-2,0 1,-1-1,1 0,0-1,-1 0,0-1,-11 1,12-2,-54-1,58 0,0 1,0-1,0 0,1 0,-1 0,0-1,0 0,1 0,-8-4,12 6,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1-1,1 1,0 0,-1-1,1 1,-1 0,1-1,0 1,-1 0,1-1,0 1,0-1,-1 1,1-1,0 1,0 0,0-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,1 0,-1-1,0 1,1-1,-1 1,1-1,24-10,0 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1104.89">1148 3176,'-10'1,"0"0,0 1,0 1,0 0,0 0,1 1,0 0,-1 1,1-1,-11 10,16-10,0 0,-1 1,2 0,-1 0,1 0,-1 0,1 1,1-1,-1 1,1 0,0-1,0 1,1 0,-2 8,-1 13,-1 48,5-71,0 1,0 0,0 0,0-1,1 1,-1 0,1-1,0 1,1 0,-1-1,1 0,0 1,0-1,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,1-1,-1 0,5 3,11 7,0-2,1 0,1-1,-1-1,1-1,1-1,0 0,0-2,0-1,0 0,1-2,-1 0,1-2,41-4,-62 4,0-1,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,-1 1,1-1,-1 1,1-1,-1 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,-1-1,1 1,-1 0,0-3,2-9,-2 1,1-1,-4-23,1 13,1-14,2 20,-2 0,0 0,-6-26,6 39,-1-1,0 0,0 1,0 0,-1-1,0 1,0 0,0 0,-1 1,1-1,-1 1,0 0,-1 0,-7-7,-6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2408.52">597 1,'4'0,"1"3,0 6,-1 7,-2 9,4 4,-1 4,0 0,-1-3,-2-1,0-4,2-4,1-4,3-4,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3248.36">1740 1483,'1'0,"-1"0,1 0,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 0,1 1,-1-1,0 0,0 1,1-1,-1 0,0 1,0-1,0 1,3 5,54 76,131 148,-91-119,220 252,-251-291,-57-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3850.26">2227 1547,'0'10,"0"12,0 12,-3 14,-6 15,-3 10,-1 0,-2 2,-1-5,1-3,1-9,1-12,4-9,3-8,3-5,2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5142.27">2375 954,'47'-1,"54"2,-99-1,0 1,0-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 1,0-1,2 4,-2-1,1 1,0 0,-1-1,0 1,0 0,0 0,1 7,0 9,0 0,0 40,-3-48,1-1,-1 1,-1-1,0 1,-1-1,0 1,0-1,-2 0,0 0,0 0,-1 0,0-1,-1 0,0 0,-13 17,19-28,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,16 1,-13-1,9 1,35 2,-1 1,0 3,79 21,-101-17,-8-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6196.68">3561 1801,'-39'-1,"21"0,-1 0,1 2,-21 3,34-3,-1 1,0-1,0 1,0 0,1 1,-1-1,1 1,0 0,0 0,0 1,0 0,0 0,-5 6,0 2,2 0,-1 0,1 1,1 0,0 0,1 1,1-1,0 1,1 1,0-1,-2 22,1 14,2 0,4 53,0-57,0-34,0 0,0 1,1-1,1 0,0 0,1 0,0 0,1-1,0 1,1-1,0 0,0-1,2 0,-1 0,12 12,-11-15,0 1,0-2,0 1,1-1,0 0,0-1,0 0,1-1,0 0,0 0,0-1,0 0,0-1,1 0,-1-1,1 0,0 0,15-2,-21 0,-1 0,1 1,0-2,-1 1,1-1,-1 1,1-1,-1 0,0-1,0 1,0-1,0 0,5-4,-3 0,0 1,0-1,-1 0,0-1,0 1,6-14,-1-5,0 1,-2-1,7-44,-6 17,-3 1,-2-1,-3 0,-8-85,4 112,-2 1,0 0,-2 0,-1 1,-1 0,-1 0,-1 1,-26-42,15 33</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6871.43">3455 785,'0'18,"-1"105,6 1,21 126,-22-228,211 1092,-212-1097,12 37,-14-52,0 1,0-1,0 1,1-1,-1 0,1 0,-1 1,1-1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,1-1,2 1,9 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7437.15">3878 1822,'1'7,"0"0,0 0,0 0,1 0,0 0,0 0,1 0,0-1,5 8,38 57,-29-48,20 30,3-2,57 57,-75-86,1-2,1 0,0-2,2 0,0-2,53 24,-76-38,1-1,-1 1,0-1,1 0,-1-1,1 1,-1-1,1 1,0-1,6-1,-9 1,1 0,-1-1,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1-1,1 1,0 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,0 0,0-3,2-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7867.26">4238 1970,'-3'10,"-9"15,-6 18,-3 8,-2 6,-4 2,-1 0,4-6,6-4,3-7,0-8,3-5,6-8,5-4,3-5</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink104.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:56:24.235"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4894 1,'2'7,"-1"0,1 0,0-1,0 1,1 0,0 0,0-1,1 0,0 0,6 8,1 3,52 82,-22-38,-2 3,31 71,63 225,-57-145,17 56,98 474,-181-697,152 793,-149-752,3 121,-16 88,-2-133,2-150,1-2,-1 0,-1 1,0-1,-1 0,-4 19,5-29,0 0,-1 0,1-1,0 1,-1 0,0-1,1 1,-1-1,0 1,0-1,0 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 1,0-1,0 0,1-1,-1 1,0 0,-1-1,1 0,0 0,-4 0,-23-1,-3-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1097.68">153 424,'0'5,"-1"0,0 1,0-1,-1 0,0 0,-3 8,-5 14,-30 140,8 2,-18 274,42 652,11-664,-1-249,47 342,39-121,-83-383,2-1,0 0,1 0,1-1,0 0,1-1,2 0,-1 0,25 25,-28-36,0 0,0-1,1 0,-1 0,1-1,0 0,0-1,0 0,1 0,-1-1,14 1,15 1,58-1,-64-2,23-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1972.38">6058 2160,'4'0,"1"3,3 13,4 10,4 15,5 16,8 11,5 13,4 0,4-3,4-5,-1-6,-2-9,-8-9,-6-14,-8-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2502.26">6397 2139,'-3'7,"-6"13,-4 14,-7 16,-8 17,-2 12,-4 14,-2-2,0-2,3-9,4-10,7-14,6-13,7-11,4-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3997.03">6630 2710,'0'-11,"1"0,0 0,0 0,1 1,1-1,6-17,-8 25,0-1,0 1,1 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,1 0,0-1,0 1,0 0,0 1,0-1,0 0,0 1,0 0,1 0,-1 0,1 0,3 0,-5 0,-1 1,1 0,0 1,0-1,-1 0,1 0,0 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 1,2 8,0-1,-1 0,2 21,-2-11,4 17,-2 0,-1 0,-2 0,-2 1,-6 45,-5-51,10-28,0 0,0 1,0-1,1 0,0 1,-1 7,2-11,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,0 0,1 0,-1 0,1-1,0 1,-1 0,1-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0-1,0 0,0 1,0-1,-1 0,1 0,0 1,0-1,0 0,0 0,0 0,1 0,35 1,-31-1,38-5,-25-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink105.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:56:33.124"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 657,'4'0,"8"0,5 0,12 0,10 0,11 0,10 0,10 0,7 0,-2 0,-3 0,-11 0,-15 3,-15 5,-13 5,-10 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="499.98">232 1123,'4'0,"5"0,7 0,13 0,8 0,12 0,9 0,-2 0,-3 0,-8 0,-7 0,-7 0,-4 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1131.37">1354 128,'5'342,"28"-3,95 385,-127-712,-1-9,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,0 0,0 0,0 0,1-1,-1 1,1 0,2 3,0-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1971.08">1227 1,'0'3,"0"5,0 9,-3 4,-2 7,0 8,2 7,0 1,-2 2,-4-4,-4-5,0-5,2-6,3-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2640.52">1354 1546,'4'0,"4"0,13 0,12 0,9 0,7 0,7 0,-3 0,-7 0,-8 0,-10 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink106.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:58:07.972"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1,'0'3,"0"5,0 5,0 4,0 2,0 2,0 4,0 2,0 0,0-1,0-2,0-1,0-1,0 0,0-1,0-3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink107.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:58:14.507"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">444 594,'-3'3,"-2"5,0 5,-2 11,-4 12,-4 18,-2 18,-3 21,3 10,0 2,0-3,-1-11,2-11,1-8,2-12,4-10,4-9,2-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="705.72">317 551,'-3'0,"-6"0,-4 0,-4 0,-2 0,-2 0,0-4,-1-1,-4 1,-1 0,1 1,1 2,1 0,1 1,1 0,4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1322.76">105 1080,'0'-4,"4"-1,4-3,5 0,8-3,6 1,3 2,4 2,-1 3,-2 1,-3 1,-2 1,-3 1,-1-1,0 1,-5-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2159.97">613 1,'2'36,"2"0,15 66,-3-21,68 354,-5-36,-67-324,-3 0,-2 133,-10-161,-1 1,-2-1,-3 0,-2-1,-24 69,18-72,-33 61,44-93</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink108.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T19:13:26.783"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -6724,7 +7852,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">7053 0,'0'2448,"-43"-1590,2-66,38 153,-9 443,-1 1124,16-1536,-2-721,-20 600,14-795</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1171.36">1 5512,'71'3,"78"11,-70-5,330 36,803 67,474-60,18-51,-1144-3,4952-4,1200 6,-6651 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1171.35">1 5512,'71'3,"78"11,-70-5,330 36,803 67,474-60,18-51,-1144-3,4952-4,1200 6,-6651 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4000.47">2480 9905,'0'0,"1"0,0-1,0 0,0 1,0-1,0 1,-1 0,1-1,0 0,1 1,-2-1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,0-2,8-11,100-170,-8-5,-8-3,81-257,-32-102,-45-9,-37 252,136-401,-114 476,11 3,11 4,179-287,-123 272,211-246,237-184,-447 511,223-175,-266 246,6 3,267-136,-210 139,3 7,3 9,5 7,1 7,2 8,3 8,237-16,-275 45,268 17,-387-4,-2 1,1 2,0 1,-2 2,48 20,174 88,-226-103,87 45,220 151,-274-162,-2 2,-3 3,-2 3,70 89,-25-6,-8 5,90 186,118 327,-108-219,45 107,39 83,-218-504,148 220,-168-290,3 0,2-2,3-2,2-2,105 76,-70-67,1-4,3-5,2-2,178 64,-238-103,1 0,0-1,0-3,66 4,140-13,-173 1,2-1,2-5,-1-2,-1-3,-1-2,103-39,315-155,-412 174,324-159,-10-15,485-347,-82-56,-618 459,-6-6,185-233,-198 192,-10-5,-8-7,188-408,-306 577,289-723,-176 366,48-143,-118 393,-34 90,-2-2,28-118,-28 72,53-134,-42 141,-15 49,-13 35</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="67069.59">9946 13335,'0'0,"0"0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,-2 0,2 0,0 0,0 0,-1 0,1 0,-12 7,-9 19,2 6,1 0,1 2,2 1,-13 45,-27 151,45-182,-120 713,34 12,62-485,-111 1554,113 18,32-1801,-3 701,-55-6,36-600,-32 258,4-85,-7 88,55-369</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="68312.59">249 17398,'1214'-42,"-779"-4,94-11,206-18,4431-175,-4481 248,-74 4,-80 2,1247-12,-449 0,-855 10,460-4,-746-12,17 2,-79 15,184 24,-247-17</inkml:trace>
@@ -6817,7 +7945,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">2229 0,'1'215,"-3"238,-9-347,6-62</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="507.98">2010 1529,'0'5,"0"5,0 6,0 4,0 3,0 2,0 1,0 1,0-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="507.97">2010 1529,'0'5,"0"5,0 6,0 4,0 3,0 2,0 1,0 1,0-5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="858">1954 2166,'0'9,"0"7,0 9,0 2</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1559.99">1 2727,'4'0,"12"5,8 1,8-2,8 1,7-2,5-1,-6-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1907">964 2702,'4'0,"2"0</inkml:trace>
@@ -6964,7 +8092,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">292 222,'0'5,"0"32,0 24,0 11,0-3,0-9,0-5,0-8,-5-16,-6-13,0-15,-4-7,1-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="453.98">1 433,'0'-4,"8"-2,9 1,14 0,6 2,6 1,14 1,1 0,1 1,-7 0,-2 1,-5-1,-1 0,-9 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="453.97">1 433,'0'-4,"8"-2,9 1,14 0,6 2,6 1,14 1,1 0,1 1,-7 0,-2 1,-5-1,-1 0,-9 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1183.99">662 301,'11'-20,"2"0,22-28,4-6,-14 15,-12 17,2 0,0 0,26-26,-40 47,-1 1,0-1,0 1,1 0,-1-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,0 0,2 1,7 19,-2 35,-7-52,2 51,-3 0,-3-1,-2 1,-23 97,-85 200,94-300</inkml:trace>
 </inkml:ink>
 </file>
@@ -7074,7 +8202,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">54 0,'9'0,"12"0,16 0,10 0,12 0,26 0,8 0,2 0,-2 0,-8 0,-9 0,-13 0,-13 0,-15 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="502.98">1 212,'0'5,"4"6,11 0,12 0,15-4,13-1,2-3,5-2,10 0,11 3,9 2,16 4,-6 0,-16 3,-22-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="502.97">1 212,'0'5,"4"6,11 0,12 0,15-4,13-1,2-3,5-2,10 0,11 3,9 2,16 4,-6 0,-16 3,-22-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7190,7 +8318,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61708.63">10260 1266,'15'17,"-1"0,0 0,12 22,7 9,16 18,51 89,-87-129,1 2,-3 0,0-1,-3 1,0 1,6 53,-9 5,-4 0,-4 0,-17 90,15-145,-1-1,-2 0,-3 0,1-2,-3 1,-1-1,-1-1,-1 0,-2 0,-2-2,0-1,-31 31,31-41,4-5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="62329.06">10892 2025,'5'0,"6"0,6 0,14 0,16 0,14 0,5 0,7 0,18 9,3 2,-10 1,-14-4,-15-1,-11 1,-14-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63736.06">11168 760,'297'-2,"319"5,-279 20,30 1,658-19,-548-8,1764 3,-2193 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73095.43">12598 1418,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 0,-1 0,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,3-1,0 1,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1 1,0-1,0 1,0-1,-1 1,2 0,-1 0,-1 1,1-1,-1 0,4 4,47 55,-43-47,-2 0,0 1,-1-1,0 0,-1 2,-1-1,-1 0,-1 0,4 22,-4 14,-4 81,-1-48,-13 54,2 2,13-135,-1 4,1 1,0 1,1-2,0 1,1-1,4 14,-5-20,0 0,1-1,-1 1,1 0,0-2,0 1,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,1 0,-2 0,1-1,0 1,0 0,0-1,1 1,6-1,15 2,1-1,-1-1,1-1,-1-1,43-8,-62 8,1-1,-1 0,-1 0,1 0,-1 0,1-1,-1 0,0 0,0-1,-1 1,1 0,-1-1,0-1,-1 1,1 1,-1-2,-1 0,4-6,2-9,-1-1,-1 0,6-34,43-165,-3 17,5-57,-72 454,11-166,-1-1,-1 1,-20 49,17-53,0 0,2 0,1 1,2 0,-4 32,11 321,-4-369,2 0,-1-1,1 1,0-1,2 0,-1 1,0-1,5 10,-5-13,0-1,0 0,0 0,1 0,1 1,-2-1,1-1,0 1,0 0,0-2,1 2,-1-1,2 0,-2 0,1 0,0-1,7 3,12 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73095.42">12598 1418,'-1'0,"0"1,1-1,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 0,-1 0,0 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,3-1,0 1,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1 1,0-1,0 1,0-1,-1 1,2 0,-1 0,-1 1,1-1,-1 0,4 4,47 55,-43-47,-2 0,0 1,-1-1,0 0,-1 2,-1-1,-1 0,-1 0,4 22,-4 14,-4 81,-1-48,-13 54,2 2,13-135,-1 4,1 1,0 1,1-2,0 1,1-1,4 14,-5-20,0 0,1-1,-1 1,1 0,0-2,0 1,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,1 0,-2 0,1-1,0 1,0 0,0-1,1 1,6-1,15 2,1-1,-1-1,1-1,-1-1,43-8,-62 8,1-1,-1 0,-1 0,1 0,-1 0,1-1,-1 0,0 0,0-1,-1 1,1 0,-1-1,0-1,-1 1,1 1,-1-2,-1 0,4-6,2-9,-1-1,-1 0,6-34,43-165,-3 17,5-57,-72 454,11-166,-1-1,-1 1,-20 49,17-53,0 0,2 0,1 1,2 0,-4 32,11 321,-4-369,2 0,-1-1,1 1,0-1,2 0,-1 1,0-1,5 10,-5-13,0-1,0 0,0 0,1 0,1 1,-2-1,1-1,0 1,0 0,0-2,1 2,-1-1,2 0,-2 0,1 0,0-1,7 3,12 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74868.95">13561 2253,'-2'48,"0"-20,3 46,-1-68,1-1,0 1,0 0,0 0,1-1,0 0,0 1,0 0,1-2,0 1,0 0,1 0,6 8,-7-10,-1-1,0 0,2 1,-1-1,-1 0,1 0,0-2,0 2,0-1,0 1,0-1,1 0,0 0,-1 0,0-1,0 1,1-1,-1 0,2 0,-2 0,5-1,-3 0,-1-1,2 0,-2 0,1 0,-1 0,0 0,0-1,1 0,-1 0,-1-1,1 1,-1 0,3-4,6-8,-1-1,0 1,-2-1,-1-1,0 0,6-20,-14 37,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,2 19,-4 30,-7 29,-4 0,-5-1,-40 113,53-177,-1 0,-1-1,0 0,0 0,-1 0,-1-1,0 1,0-2,-2 1,0-2,-17 15,19-18,-1 0,0-1,0 0,-1 0,1-1,-2 0,2-1,-1-1,-1 1,1-1,-1 0,1-1,0 0,-1 0,0-1,-13-2,19 1,1 0,-1 0,0 0,1-1,0 0,0 1,0-1,-1 0,1 0,1-1,-1 0,1 0,-1 0,1 0,-1 1,1-2,1 1,-1-1,1 0,0 0,0 1,0-1,0 0,1 0,-1-1,0-6,-2 1,2 0,1 0,0 0,0-1,1 2,0-2,1 1,0 0,1-1,5-12,-5 18,1-1,0 1,0 0,0 1,1-1,1 0,-1 1,0-1,1 2,6-6,-2 1,13-9</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="76160">14276 1493,'0'73,"2"13,-4-1,-26 153,15-164,2 0,5-1,3 2,9 91,-6-159,1-1,0 0,0 0,1 0,-1 0,1 0,2-1,-2 1,1 0,7 9,-9-13,1 0,0 0,0 0,0 0,1-1,0 0,-1 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,0-1,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,0-1,0 1,0-1,4-1,11-3</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="77063">14634 2101,'-1'-19,"2"-1,0 1,1 1,1-1,1 0,13-35,-14 49,-1 0,1-1,0 0,1 2,0-1,0 0,0 0,0 0,1 2,-1-2,2 1,-1 0,0 1,0-1,1 2,1-1,-2 0,1 1,0 0,1 0,-1 0,0 1,0-1,2 2,10-1,-10 1,-1 0,0 1,0 0,1 1,-1 0,0 0,0 0,0 1,0 0,-1 0,1-1,0 2,-1 0,-1 1,1-1,0 0,-1 1,9 11,7 8,-1 1,31 55,-30-47,13 25,-2 0,32 85,-60-131,1-1,0 2,0-2,2 0,11 17,-17-28,0 1,0 1,-1-1,1 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,2 0,-2 0,0 0,1-1,-1 1,0 0,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,0 0,2-2,24-21</inkml:trace>
@@ -8160,7 +9288,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">233 1166,'0'5,"-5"4,-6 11,-11 5,-1 4,-7 1,-3-6,-5-2,0-3,5-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1212.64">761 2,'116'-1,"122"3,-233-1,-2-1,0 1,0 0,0 0,1 0,0 0,-1 0,0 1,0-2,-1 2,1 0,0 0,-1 0,2 0,-2 1,0-1,1 1,-1-1,-1 0,1 1,0 0,0 0,-1 0,0 0,1 0,-1 0,0-1,0 1,0 1,-1-1,0 0,1 4,0 7,-1 0,0 0,-1 0,0-1,-2 2,-5 17,-1-6,-2 1,0-2,-3-1,-25 38,-80 93,63-85,-28 31,35-42,-58 88,106-146,0 1,0-1,0 1,0-1,-1 1,2-2,-1 2,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,1-1,-1 0,0 1,1 0,-1-1,1 1,-1 0,2-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,-1-1,1 1,2-1,13 4,-1 0,0-2,0-1,22 1,-24-1,330 0,-270-2,-33 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1212.63">761 2,'116'-1,"122"3,-233-1,-2-1,0 1,0 0,0 0,1 0,0 0,-1 0,0 1,0-2,-1 2,1 0,0 0,-1 0,2 0,-2 1,0-1,1 1,-1-1,-1 0,1 1,0 0,0 0,-1 0,0 0,1 0,-1 0,0-1,0 1,0 1,-1-1,0 0,1 4,0 7,-1 0,0 0,-1 0,0-1,-2 2,-5 17,-1-6,-2 1,0-2,-3-1,-25 38,-80 93,63-85,-28 31,35-42,-58 88,106-146,0 1,0-1,0 1,0-1,-1 1,2-2,-1 2,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,1-1,-1 0,0 1,1 0,-1-1,1 1,-1 0,2-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,-1-1,1 1,2-1,13 4,-1 0,0-2,0-1,22 1,-24-1,330 0,-270-2,-33 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1715.65">1648 584,'0'17,"0"15,0 6,0 9,0 5,-5 11,-1 1,-9 0,-3-6,-2-4,3-7,3-7,4-15,4-10</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2073.65">1788 281,'-5'0,"-7"5,1 13,-5 26,1 6</inkml:trace>
 </inkml:ink>
@@ -8619,7 +9747,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 27,'42'-2,"45"-8,20-1,-87 10,206-1,-222 2,0 0,-1 0,1 0,0 1,-1 0,1-1,0 1,-1 0,1 1,-1-1,1 1,-1-1,0 1,0 0,0 0,0 1,0-1,4 5,-4-2,-1-1,0 0,0 1,-1-1,1 1,-1 0,0-1,0 1,-1 0,0-1,1 1,-2 0,1 0,-1 5,1-8,-2 12,2 0,0 0,2 20,-1-29,0 1,0-1,1 0,0 0,0 0,0 0,1 0,0 0,0-1,0 1,0-1,6 5,-2 0,0 1,0-1,-1 1,0 0,-1 0,0 1,-1-1,0 1,0 0,-1 0,-1 1,2 18,-2-10,-1 0,-1 0,-1 0,0 0,-2-1,-7 32,8-46,0 0,-1 0,1 0,-1 0,0 0,0 0,-1-1,1 1,-1-1,0 0,0 0,0 0,-1-1,1 0,-1 1,0-2,0 1,0 0,0-1,0 0,-1 0,1-1,-1 0,1 0,-1 0,0 0,1-1,-1 0,-9-1,-4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="338.98">1032 504,'4'0,"2"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="338.97">1032 504,'4'0,"2"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9526,6 +10654,136 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2025.98">972 382,'-3'-2,"1"0,0-1,0 0,0 1,0-1,0 0,0 0,1 0,0 0,-1 0,1-1,0 1,1 0,-1-1,0 1,1 0,0-1,0 1,0 0,0-1,0 1,1-1,0 1,-1 0,1 0,1-1,-1 1,2-4,1 1,-1 0,1 0,1 0,-1 0,1 0,0 1,0 0,1 0,-1 0,1 1,12-7,-7 5,-1 1,1 0,-1 1,1 0,0 1,1 0,-1 1,1 0,-1 1,1 0,16 1,-23 1,1 0,-1 0,1 0,-1 1,0 0,1 0,-1 0,0 1,0 0,-1 0,1 0,-1 0,1 1,-1 0,0 0,0 0,-1 0,1 1,-1-1,0 1,0 0,0 0,-1 0,0 0,2 6,4 14,8 46,6 20,-19-85,0 0,0-1,1 1,0-1,0 1,0-1,1 0,0-1,0 1,0-1,0 0,1 0,8 5,6 1,1 0,34 12,-28-14</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2618.99">1590 59,'-10'5,"-14"17,-22 19,-13 18,-8 4,-1 1,-5-5,-4-2,5-7,11-6,10-6,13-9</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4673">1972 89,'-3'156,"7"163,-4-316,0-1,0 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,1-1,0 1,-1 0,1-1,0 1,3 1,-2-1,0-1,0 0,1 0,-1 0,0-1,1 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,5-2,9-3,1 0,-1-1,0-1,21-12,-36 18,36-18,118-66,-138 73,1 0,-2-2,1 0,-2-1,26-29,-37 36,0 0,-1-1,0 1,0-1,-1 1,0-1,0 0,-1 0,-1 0,1-1,-1 1,-1-14,0 0,-2 0,0 0,-10-38,9 123,-31 367,24-349,8-58,-34 213,29-208,-1-1,-1 1,-1-2,-2 1,0-2,-25 37,1-5,14-21,-1-2,-2 0,-41 42,59-68,0 0,-1-1,0 0,0 0,0 0,-1-1,0-1,0 0,0 0,0 0,-1-1,1-1,-1 1,0-2,1 1,-1-1,0-1,0 0,-14-1,21 0,-1 1,1-1,-1 0,1 0,0-1,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,1-1,-1 1,0-1,-3-5,2 3,1-1,0 1,0-1,1 0,-1 0,1-1,1 1,-3-11,2-6,1 1,1-1,1 0,4-29,-4 48,0-1,0 1,0 0,0-1,1 1,0 0,0 0,0 0,0 0,0 0,1 1,0-1,0 1,0-1,0 1,0 0,1 0,-1 1,1-1,0 1,0-1,0 1,0 0,0 1,0-1,1 1,-1 0,8-1,12-2,1 2,-1 1,0 1,32 4,-9-1,253 0,-272-3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink96.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:52:53.680"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">383 552,'-7'0,"0"0,0 1,1 0,-1 1,0-1,0 1,1 1,-1-1,1 1,-1 0,-6 5,3-1,0 1,0 0,1 0,1 1,-15 18,3 2,1 2,1 0,-19 48,10-12,4 1,2 1,3 1,3 0,4 1,2 1,1 85,22 345,1-361,50 215,75 151,-15-60,-31 6,-82-331,-7 221,-6-260,1-76,0 0,-1 0,0 0,0 0,0-1,-1 1,0 0,0-1,-7 13,7-16,0 0,0 0,0 0,-1-1,1 1,-1 0,0-1,0 0,0 0,0 0,0 0,-1 0,1-1,0 1,-1-1,1 0,-1 0,0 0,1 0,-6-1,-52 1,43-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1420.1">934 1,'0'3,"0"6,0 4,0 3,-3 7,-2 3,0 0,2 7,0 1,2 6,0 3,0 2,1 0,1 0,-1-5,0-1,0-4,0-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3608.63">934 4531,'-5'-1,"-1"1,1 0,-1 1,0-1,1 1,-1 0,1 0,-11 5,14-5,0 1,0-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,0 1,0-1,0 1,1-1,-1 1,1-1,0 1,-1 4,-1 30,0 0,3 0,9 68,-4-82,1 0,1-1,2 0,0 0,1-1,1 0,1-1,0-1,29 30,-39-45,1 0,1-1,-1 1,0-1,1-1,-1 1,1 0,0-1,0 0,0 0,0-1,1 1,-1-1,0 0,6 0,2 0,1-1,-1 0,0-1,26-5,-33 4,-1 1,1-1,0 0,-1 0,0-1,1 0,-1 0,0 0,-1 0,1-1,0 0,-1 0,0 0,0 0,0-1,-1 0,1 1,-1-1,0-1,-1 1,1 0,-1-1,0 1,0-1,1-10,2-11,-2 0,-1-1,-1 1,-3-36,1 25,1 33,0-21,-1 1,-7-37,6 53,-1 0,0 0,0 0,-1 0,0 1,0 0,-1-1,0 1,0 1,-8-8,-4-5,-1 2,0 0,-35-25,45 38,0-1,-1 1,0 0,0 1,0 0,0 1,0 0,-1 0,0 1,1 0,-1 1,-15-1,17 2,-9 0,1 1,0 0,1 1,-29 8,31-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6009.65">1548 2076,'1'3,"-1"1,1 0,0-1,0 1,0 0,0-1,1 1,-1-1,1 0,0 1,0-1,0 0,5 4,40 39,-28-29,50 41,2-4,135 78,-136-90,-27-14,1-3,1-1,80 29,-120-52,0 0,-1 1,1 0,-1 0,1 0,6 5,-3 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6635.96">2161 2076,'-3'1,"0"1,0 0,0 0,0 1,0-1,0 1,0-1,1 1,-1 0,1 0,0 0,0 0,-3 7,-3 3,-166 257,96-140,15-9,20-37,47-90,5-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7958.52">2246 1631,'-4'0,"0"0,0 0,0 1,0-1,0 1,0 0,0 1,0-1,0 1,0-1,1 1,-1 0,1 1,-1-1,-3 4,2-1,0 0,1 0,0 1,0-1,0 1,1 0,0 0,-4 11,1 2,1 0,1 0,0 0,2 1,-1 32,3-49,0-1,0 1,0-1,0 1,0 0,1-1,-1 1,1-1,-1 0,1 1,0-1,0 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,0 0,2 1,0-1,0 0,1 0,-1 0,1-1,0 0,-1 0,1 0,0-1,0 1,-1-1,6-1,-7 2,0-1,0 0,-1 0,1-1,0 1,0-1,0 1,-1-1,1 0,0 0,-1 0,1 0,-1-1,0 1,1 0,-1-1,0 0,0 0,0 0,4-3,-3-2,1 1,-1 0,-1-1,1 1,-1-1,0 0,1-9,1-7,-1 0,-1-40,-2 45</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9714">3072 1949,'-1'2,"0"1,0 0,-1 0,1 0,-1-1,0 1,0-1,0 1,0-1,0 0,-1 0,1 0,-5 3,-1 2,-28 26,1 2,1 2,2 1,-49 77,68-95,-3 7,-22 46,35-64,-1-1,1 1,1 1,0-1,0 0,0 0,2 1,-1-1,2 18,-1-25,0-1,1 1,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,0 0,0-1,0 1,0-1,1 1,-1-1,0 0,1 1,-1-1,1 0,3 2,-1-1,0 0,1-1,-1 1,1-1,0 0,-1 0,1-1,7 1,-1-1,-1 0,0-1,0 0,1-1,-1 0,0-1,16-6,-18 4,0 0,0-1,0 0,-1 0,0-1,0 0,0 0,-1 0,0-1,-1 0,1 0,4-12,7-15,20-64,-32 84,10-27,-2-1,-2-1,-2 0,-2 0,2-87,-12-376,20 592,103 549,-95-512,-16-81,0-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10463.86">3537 2139,'4'0,"4"0,9 0,12 7,8 9,8 10,12 8,10 1,4 2,5-2,-7-7,-8-7,-11-9,-10-5,-9-4,-8-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10973.84">4088 2118,'-3'10,"-10"12,-8 8,-5 11,-1 5,-4 5,0-2,2-5,6-4,3-8,5-7,1-6,3-4,4-4</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink97.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:53:08.767"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6208 43,'1'3,"1"1,-1 0,1 0,0 0,-1-1,2 1,-1-1,0 1,1-1,4 5,2 2,292 327,-62-78,-111-97,-6 5,-7 6,-9 5,-7 4,126 324,-176-364,-5 2,-7 2,21 173,-39-143,-7 1,-15 247,-12-265,-7-1,-85 303,-83 60,70-217,119-301,-2 5,1-1,-1 0,-1 0,-5 9,8-14,0-1,0 0,1 0,-1 0,0 0,0 0,-1 0,1 0,0-1,0 1,0 0,0 0,-1-1,1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 0,1 0,0 0,-1 0,1 0,-1 0,1-1,0 1,-3-1,-15-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="969.22">1086 1,'-79'123,"6"4,-66 157,-87 285,215-541,-132 376,-112 511,199-642,12 2,-16 549,62-681,41 276,-25-326,4 0,4-2,71 167,-53-165,4-2,4-3,4-2,4-2,3-3,4-3,3-3,94 78,-126-122,2-1,1-2,1-2,58 26,-73-40,0-2,1-1,0-1,0-1,1-1,0-2,0-1,47-1,-41-3,-2-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2342.66">8134 2096,'1'4,"-1"1,1-1,0 1,0 0,0-1,0 0,1 1,0-1,0 0,0 0,1 0,-1 0,6 7,5 2,0 0,18 15,-17-16,221 184,67 60,-268-219,-28-29,0-1,1 0,0 0,14 11,-14-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2975.97">8790 2033,'-1'2,"-1"0,0 1,1-1,0 1,0 0,0-1,0 1,0 0,-1 5,-2 8,-39 94,-4-2,-70 116,103-196,1 1,-13 42,4-10,12-45,9-15,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,0 2,6 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4347.74">9150 2604,'-43'16,"39"-14,1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-1 0,1-1,-1 1,1 0,0 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1 3,-1 8,0 1,1 0,0 24,0-14,-2 2,3-22,0 0,0 1,1-1,0 1,0-1,1 9,0-13,-1 0,1 1,0-1,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1-1,0 1,0-1,-1 1,1-1,0 1,0-1,1 0,-1 0,4 1,0 0,0 0,0 0,0-1,0 0,1-1,-1 1,0-1,1 0,-1-1,10-1,-12 2,-1-1,0 0,0 0,0 1,0-2,0 1,0 0,0-1,0 1,-1-1,1 0,0 0,-1 0,0 0,1 0,-1-1,0 1,0-1,0 0,-1 1,1-1,1-4,16-40,-14 38,-1-1,0 0,0 0,-1 0,-1 0,0-1,2-16,-4 20,-2-35,1 40,1 0,-1 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 1,0-1,0 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,-3-1,-9-3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink98.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:53:28.610"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">318 1,'0'7,"0"6,0 12,0 12,0 7,0 7,0 2,0-4,0-4,4-2,1-5,-1-5,0-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="755.98">0 213,'7'-4,"7"-1,7 1,8-4,5 1,6 1,1 1,3 3,3 0,5 1,5 1,3 0,-5 1,-8-1,-9 0,-10 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink99.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-04-25T18:53:34.855"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">405 397,'-4'1,"1"0,-1 1,0 0,1 0,-1 0,1 0,0 1,-1-1,1 1,0 0,1 0,-5 5,1-2,-5 6,1-1,1 1,0 1,1-1,-12 25,5-2,-13 42,-9 27,17-53,-22 94,33-76,3 1,3-1,7 98,-2-137,3 41,21 104,30 68,-12-57,40 299,-79-451,3 22,17 127,-23-146,-1-1,-1 1,-6 38,4-64,0 1,-1-1,-1 0,0 1,0-2,-1 1,0 0,-1-1,0 0,-1-1,0 1,-13 13,6-10,0-1,-1 0,0-1,0 0,-2-1,1-1,-20 8,15-8,-47 18,64-25,-1-1,1 0,-1 0,1 0,-1-1,1 0,-1 0,1 0,-1 0,1 0,-1-1,-7-2,3-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1073.93">765 3106,'-4'1,"-1"2,1-1,-1 1,1-1,0 1,0 1,-6 5,1-2,-4 3,2 0,0 0,0 1,1 0,0 1,-12 19,17-21,0 0,0 0,1 0,0 0,1 1,0-1,1 1,0 0,0 22,1-24,1 0,0 0,0 1,1-1,1 0,2 11,-3-17,1 0,-1 0,1-1,0 1,-1 0,1 0,0-1,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,0 0,-1-1,1 1,0-1,1 0,4 2,17 4,0-1,1-1,-1-2,1 0,37-1,-60-2,0 0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0-1,0 1,0-1,-1 1,1-1,-1 0,1 0,-1 0,0 0,1 0,-1 0,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 0,0 0,0 0,0 0,0 0,0-3,1-11,0 0,-1 0,-1 0,-3-28,1 9,2 26,0-1,-1 1,-1-1,1 1,-6-17,5 22,-1 0,1 1,-1-1,1 1,-1-1,0 1,-1 0,1 0,-1 0,0 1,0-1,0 1,-5-3,-8-5,3 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5186.01">1400 1731,'1'4,"0"0,1-1,-1 1,1 0,-1 0,1-1,1 1,-1 0,0-1,1 0,-1 0,1 0,0 0,0 0,0 0,6 2,5 8,88 80,64 65,-116-104,2-2,2-3,79 55,-109-89,-5-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5806.86">1971 1900,'-1'1,"1"1,-2 0,1 0,0 0,0 0,0-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,0 0,-1 1,-8 7,-19 24,1 1,-36 59,-40 85,35-54,67-120,3-3,0 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1-1,0 1,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 0,0 1,-2-1,-2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7960.87">2903 1942,'-24'-1,"-1"1,0 0,0 2,-39 6,56-6,0 1,1-1,-1 1,1 0,-1 1,1 0,0 0,1 1,-1-1,1 1,0 1,0-1,0 1,1 0,-6 9,4-6,1 1,1 0,-1 0,2 0,-1 1,2 0,-4 13,6-20,0-1,1 1,-1-1,1 1,0-1,0 1,0-1,0 1,1-1,-1 1,1-1,0 0,0 1,0-1,0 0,1 1,-1-1,1 0,0 0,0 0,0-1,1 1,-1 0,0-1,1 1,0-1,3 3,15 5,0-1,0 0,0-2,1 0,0-2,1 0,45 3,-65-8,-1 0,1 0,0 0,0 0,-1 0,1-1,0 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,1 0,-1-1,0 1,0-1,1 1,1-3,-1 0,0 0,0 0,0 0,0-1,-1 1,0-1,0 0,0 0,2-7,0-9,0 0,-2 0,0-39,-2 59,0-24,-1-1,-5-29,4 44,0 1,-1-1,-1 1,1 0,-1 0,-1 1,-10-17,-1 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8568.49">2628 566,'4'68,"3"0,31 130,-13-80,15 92,145 677,-109-618,-74-263,-1-1,1 0,0 0,0 0,1 0,0 0,-1-1,1 1,1-1,4 6,0-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9116.88">3072 1879,'0'3,"0"5,0 5,7 7,7 8,7 6,0 1,5 1,0-5,-4-4,-1-7,-5-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9553.27">3241 1836,'0'7,"0"6,0 12,-3 8,-2 10,0 1,-2 1,0-5,1-5,-2-4,0-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="49527.44">3009 1773,'0'3,"4"13,8 6,9 8,5 4,9 2,5 1,3-6,2-1,0-1,4 0,0 0,-5-1,-5-7,-7-5,-8-3,-8-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="50417.47">3326 1688,'0'0,"-1"0,0 0,0 0,1 1,-1-1,0 0,1 1,-1-1,0 0,1 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,0-1,-1 1,1 0,0-1,0 1,-1 0,1 1,-4 26,3-20,-101 563,96-539,-2 7,-14 45,17-71</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9828,7 +11086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1959046-2DC6-4331-8086-8723FFDB0E43}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P7" workbookViewId="0">
       <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
@@ -9844,7 +11102,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10163,7 +11421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE744686-E7BF-4051-8C38-1ED889B4DB33}">
   <dimension ref="A3:K22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -10376,8 +11634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5874FDE-3A89-4775-B935-89301D48D7A2}">
   <dimension ref="B2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10530,4 +11788,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83B3F64-7529-4070-A6B8-3F87722D4C0B}">
+  <dimension ref="C21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB0AADC-DCBA-471B-8C69-640108A9C1BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>